<commit_message>
Add results of banks business group and some correction in R code
</commit_message>
<xml_diff>
--- a/f_Vector_for_family.xlsx
+++ b/f_Vector_for_family.xlsx
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.6394</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2223,7 +2223,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -3071,7 +3071,7 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>0</v>
+        <v>0.3516</v>
       </c>
     </row>
     <row r="166">
@@ -5791,7 +5791,7 @@
         </is>
       </c>
       <c r="D335" t="n">
-        <v>0.0106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="336">
@@ -6175,7 +6175,7 @@
         </is>
       </c>
       <c r="D359" t="n">
-        <v>0</v>
+        <v>0.1104</v>
       </c>
     </row>
     <row r="360">
@@ -7503,7 +7503,7 @@
         </is>
       </c>
       <c r="D442" t="n">
-        <v>0.0408</v>
+        <v>0</v>
       </c>
     </row>
     <row r="443">
@@ -8095,7 +8095,7 @@
         </is>
       </c>
       <c r="D479" t="n">
-        <v>0.0114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="480">
@@ -9071,7 +9071,7 @@
         </is>
       </c>
       <c r="D540" t="n">
-        <v>0</v>
+        <v>0.701</v>
       </c>
     </row>
     <row r="541">
@@ -9615,7 +9615,7 @@
         </is>
       </c>
       <c r="D574" t="n">
-        <v>0</v>
+        <v>0.3224</v>
       </c>
     </row>
     <row r="575">
@@ -10495,7 +10495,7 @@
         </is>
       </c>
       <c r="D629" t="n">
-        <v>0.0223</v>
+        <v>0</v>
       </c>
     </row>
     <row r="630">
@@ -10559,7 +10559,7 @@
         </is>
       </c>
       <c r="D633" t="n">
-        <v>0</v>
+        <v>0.7128</v>
       </c>
     </row>
     <row r="634">
@@ -10655,7 +10655,7 @@
         </is>
       </c>
       <c r="D639" t="n">
-        <v>0.0201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="640">
@@ -11231,7 +11231,7 @@
         </is>
       </c>
       <c r="D675" t="n">
-        <v>0</v>
+        <v>0.8582</v>
       </c>
     </row>
     <row r="676">
@@ -11383,11 +11383,11 @@
         <v>683</v>
       </c>
       <c r="B685" t="n">
-        <v>10101044869</v>
+        <v>14005751499</v>
       </c>
       <c r="C685" t="inlineStr">
         <is>
-          <t>سرمايه گذاري تامين اجتماعي</t>
+          <t>پيشگامان فن آوري و دانش آراميس</t>
         </is>
       </c>
       <c r="D685" t="n">
@@ -11399,11 +11399,11 @@
         <v>684</v>
       </c>
       <c r="B686" t="n">
-        <v>14005751499</v>
+        <v>10320839651</v>
       </c>
       <c r="C686" t="inlineStr">
         <is>
-          <t>پيشگامان فن آوري و دانش آراميس</t>
+          <t>بيمه تعاون</t>
         </is>
       </c>
       <c r="D686" t="n">
@@ -11415,11 +11415,11 @@
         <v>685</v>
       </c>
       <c r="B687" t="n">
-        <v>10320839651</v>
+        <v>10100478433</v>
       </c>
       <c r="C687" t="inlineStr">
         <is>
-          <t>بيمه تعاون</t>
+          <t>تايدواترخاورميانه‌</t>
         </is>
       </c>
       <c r="D687" t="n">
@@ -11431,11 +11431,11 @@
         <v>686</v>
       </c>
       <c r="B688" t="n">
-        <v>10100478433</v>
+        <v>10200142417</v>
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>تايدواترخاورميانه‌</t>
+          <t>سرمايه‌گذاري‌توسعه‌آذربايجان‌</t>
         </is>
       </c>
       <c r="D688" t="n">
@@ -11447,11 +11447,11 @@
         <v>687</v>
       </c>
       <c r="B689" t="n">
-        <v>10200142417</v>
+        <v>10260357602</v>
       </c>
       <c r="C689" t="inlineStr">
         <is>
-          <t>سرمايه‌گذاري‌توسعه‌آذربايجان‌</t>
+          <t>ذغال‌سنگ‌ نگين‌ ط‌بس‌</t>
         </is>
       </c>
       <c r="D689" t="n">
@@ -11463,11 +11463,11 @@
         <v>688</v>
       </c>
       <c r="B690" t="n">
-        <v>10260357602</v>
+        <v>10260377008</v>
       </c>
       <c r="C690" t="inlineStr">
         <is>
-          <t>ذغال‌سنگ‌ نگين‌ ط‌بس‌</t>
+          <t>فرآوري زغال سنگ پروده طبس</t>
         </is>
       </c>
       <c r="D690" t="n">
@@ -11479,11 +11479,11 @@
         <v>689</v>
       </c>
       <c r="B691" t="n">
-        <v>10260377008</v>
+        <v>10101907666</v>
       </c>
       <c r="C691" t="inlineStr">
         <is>
-          <t>فرآوري زغال سنگ پروده طبس</t>
+          <t>گروه سرمايه گذاري تدبير</t>
         </is>
       </c>
       <c r="D691" t="n">
@@ -11495,11 +11495,11 @@
         <v>690</v>
       </c>
       <c r="B692" t="n">
-        <v>10101907666</v>
+        <v>10260439863</v>
       </c>
       <c r="C692" t="inlineStr">
         <is>
-          <t>گروه سرمايه گذاري تدبير</t>
+          <t>سرمايه گذاري توسعه توكا</t>
         </is>
       </c>
       <c r="D692" t="n">
@@ -11511,11 +11511,11 @@
         <v>691</v>
       </c>
       <c r="B693" t="n">
-        <v>10260439863</v>
+        <v>10380266337</v>
       </c>
       <c r="C693" t="inlineStr">
         <is>
-          <t>سرمايه گذاري توسعه توكا</t>
+          <t>توسعه‌شهري‌توس‌گستر</t>
         </is>
       </c>
       <c r="D693" t="n">
@@ -11527,11 +11527,11 @@
         <v>692</v>
       </c>
       <c r="B694" t="n">
-        <v>10380266337</v>
+        <v>10100254685</v>
       </c>
       <c r="C694" t="inlineStr">
         <is>
-          <t>توسعه‌شهري‌توس‌گستر</t>
+          <t>داروسازي‌ تهران‌ دارو</t>
         </is>
       </c>
       <c r="D694" t="n">
@@ -11543,11 +11543,11 @@
         <v>693</v>
       </c>
       <c r="B695" t="n">
-        <v>10100254685</v>
+        <v>10380466986</v>
       </c>
       <c r="C695" t="inlineStr">
         <is>
-          <t>داروسازي‌ تهران‌ دارو</t>
+          <t>گروه كارخانجات صنعتي تبرك</t>
         </is>
       </c>
       <c r="D695" t="n">
@@ -11559,11 +11559,11 @@
         <v>694</v>
       </c>
       <c r="B696" t="n">
-        <v>10380466986</v>
+        <v>10103251617</v>
       </c>
       <c r="C696" t="inlineStr">
         <is>
-          <t>گروه كارخانجات صنعتي تبرك</t>
+          <t>صنايع پتروشيمي تخت جمشيد</t>
         </is>
       </c>
       <c r="D696" t="n">
@@ -11575,11 +11575,11 @@
         <v>695</v>
       </c>
       <c r="B697" t="n">
-        <v>10103251617</v>
+        <v>10260289240</v>
       </c>
       <c r="C697" t="inlineStr">
         <is>
-          <t>صنايع پتروشيمي تخت جمشيد</t>
+          <t>تكادو</t>
         </is>
       </c>
       <c r="D697" t="n">
@@ -11591,11 +11591,11 @@
         <v>696</v>
       </c>
       <c r="B698" t="n">
-        <v>10260289240</v>
+        <v>10101477062</v>
       </c>
       <c r="C698" t="inlineStr">
         <is>
-          <t>تكادو</t>
+          <t>كنترل ‌خوردگي ‌تكين ‌كوي</t>
         </is>
       </c>
       <c r="D698" t="n">
@@ -11607,11 +11607,11 @@
         <v>697</v>
       </c>
       <c r="B699" t="n">
-        <v>10101477062</v>
+        <v>10000000004</v>
       </c>
       <c r="C699" t="inlineStr">
         <is>
-          <t>كنترل ‌خوردگي ‌تكين ‌كوي</t>
+          <t>توليدكنندگان بورس كالاي ايران</t>
         </is>
       </c>
       <c r="D699" t="n">
@@ -11623,11 +11623,11 @@
         <v>698</v>
       </c>
       <c r="B700" t="n">
-        <v>10000000004</v>
+        <v>10861658680</v>
       </c>
       <c r="C700" t="inlineStr">
         <is>
-          <t>توليدكنندگان بورس كالاي ايران</t>
+          <t>تكنوتار</t>
         </is>
       </c>
       <c r="D700" t="n">
@@ -11639,11 +11639,11 @@
         <v>699</v>
       </c>
       <c r="B701" t="n">
-        <v>10861658680</v>
+        <v>10260294158</v>
       </c>
       <c r="C701" t="inlineStr">
         <is>
-          <t>تكنوتار</t>
+          <t>توليدي‌ كاشي‌ تكسرام‌</t>
         </is>
       </c>
       <c r="D701" t="n">
@@ -11655,11 +11655,11 @@
         <v>700</v>
       </c>
       <c r="B702" t="n">
-        <v>10260294158</v>
+        <v>10101021508</v>
       </c>
       <c r="C702" t="inlineStr">
         <is>
-          <t>توليدي‌ كاشي‌ تكسرام‌</t>
+          <t>دامداري تليسه نمونه</t>
         </is>
       </c>
       <c r="D702" t="n">
@@ -11671,11 +11671,11 @@
         <v>701</v>
       </c>
       <c r="B703" t="n">
-        <v>10101021508</v>
+        <v>10320741707</v>
       </c>
       <c r="C703" t="inlineStr">
         <is>
-          <t>دامداري تليسه نمونه</t>
+          <t>تامين سرمايه تمدن</t>
         </is>
       </c>
       <c r="D703" t="n">
@@ -11687,11 +11687,11 @@
         <v>702</v>
       </c>
       <c r="B704" t="n">
-        <v>10320741707</v>
+        <v>10102501905</v>
       </c>
       <c r="C704" t="inlineStr">
         <is>
-          <t>تامين سرمايه تمدن</t>
+          <t>سرمايه‌گذاري‌توسعه‌ملي‌</t>
         </is>
       </c>
       <c r="D704" t="n">
@@ -11703,15 +11703,15 @@
         <v>703</v>
       </c>
       <c r="B705" t="n">
-        <v>10102501905</v>
+        <v>10320585987</v>
       </c>
       <c r="C705" t="inlineStr">
         <is>
-          <t>سرمايه‌گذاري‌توسعه‌ملي‌</t>
+          <t>بين المللي توسعه ص. معادن غدير</t>
         </is>
       </c>
       <c r="D705" t="n">
-        <v>0.2674</v>
+        <v>0</v>
       </c>
     </row>
     <row r="706">
@@ -11719,11 +11719,11 @@
         <v>704</v>
       </c>
       <c r="B706" t="n">
-        <v>10320585987</v>
+        <v>10101136712</v>
       </c>
       <c r="C706" t="inlineStr">
         <is>
-          <t>بين المللي توسعه ص. معادن غدير</t>
+          <t>توليدمحورخودرو</t>
         </is>
       </c>
       <c r="D706" t="n">
@@ -11735,11 +11735,11 @@
         <v>705</v>
       </c>
       <c r="B707" t="n">
-        <v>10101136712</v>
+        <v>10320453421</v>
       </c>
       <c r="C707" t="inlineStr">
         <is>
-          <t>توليدمحورخودرو</t>
+          <t>تامين سرمايه بانك ملت</t>
         </is>
       </c>
       <c r="D707" t="n">
@@ -11751,11 +11751,11 @@
         <v>706</v>
       </c>
       <c r="B708" t="n">
-        <v>10320453421</v>
+        <v>10320826260</v>
       </c>
       <c r="C708" t="inlineStr">
         <is>
-          <t>تامين سرمايه بانك ملت</t>
+          <t>تجلي توسعه معادن و فلزات</t>
         </is>
       </c>
       <c r="D708" t="n">
@@ -11767,11 +11767,11 @@
         <v>707</v>
       </c>
       <c r="B709" t="n">
-        <v>10320826260</v>
+        <v>10101725603</v>
       </c>
       <c r="C709" t="inlineStr">
         <is>
-          <t>تجلي توسعه معادن و فلزات</t>
+          <t>توليدمواداوليه‌داروپخش‌</t>
         </is>
       </c>
       <c r="D709" t="n">
@@ -11783,11 +11783,11 @@
         <v>708</v>
       </c>
       <c r="B710" t="n">
-        <v>10101725603</v>
+        <v>14005725237</v>
       </c>
       <c r="C710" t="inlineStr">
         <is>
-          <t>توليدمواداوليه‌داروپخش‌</t>
+          <t>بيمه تجارت نو</t>
         </is>
       </c>
       <c r="D710" t="n">
@@ -11799,11 +11799,11 @@
         <v>709</v>
       </c>
       <c r="B711" t="n">
-        <v>14005725237</v>
+        <v>10103584900</v>
       </c>
       <c r="C711" t="inlineStr">
         <is>
-          <t>بيمه تجارت نو</t>
+          <t>تامين سرمايه نوين</t>
         </is>
       </c>
       <c r="D711" t="n">
@@ -11815,11 +11815,11 @@
         <v>710</v>
       </c>
       <c r="B712" t="n">
-        <v>10103584900</v>
+        <v>14005652664</v>
       </c>
       <c r="C712" t="inlineStr">
         <is>
-          <t>تامين سرمايه نوين</t>
+          <t>سرمايه گذاري اقتصاد شهر طوبي</t>
         </is>
       </c>
       <c r="D712" t="n">
@@ -11831,11 +11831,11 @@
         <v>711</v>
       </c>
       <c r="B713" t="n">
-        <v>14005652664</v>
+        <v>10260272518</v>
       </c>
       <c r="C713" t="inlineStr">
         <is>
-          <t>سرمايه گذاري اقتصاد شهر طوبي</t>
+          <t>سرمايه‌گذاري‌توكافولاد(هلدينگ‌</t>
         </is>
       </c>
       <c r="D713" t="n">
@@ -11847,11 +11847,11 @@
         <v>712</v>
       </c>
       <c r="B714" t="n">
-        <v>10260272518</v>
+        <v>10260041071</v>
       </c>
       <c r="C714" t="inlineStr">
         <is>
-          <t>سرمايه‌گذاري‌توكافولاد(هلدينگ‌</t>
+          <t>توسعه و عمران شهرستان نائين</t>
         </is>
       </c>
       <c r="D714" t="n">
@@ -11863,11 +11863,11 @@
         <v>713</v>
       </c>
       <c r="B715" t="n">
-        <v>10260041071</v>
+        <v>10101912330</v>
       </c>
       <c r="C715" t="inlineStr">
         <is>
-          <t>توسعه و عمران شهرستان نائين</t>
+          <t>توسعه و عمران اميد</t>
         </is>
       </c>
       <c r="D715" t="n">
@@ -11879,11 +11879,11 @@
         <v>714</v>
       </c>
       <c r="B716" t="n">
-        <v>10101912330</v>
+        <v>10100595801</v>
       </c>
       <c r="C716" t="inlineStr">
         <is>
-          <t>توسعه و عمران اميد</t>
+          <t>تولي‌پرس‌</t>
         </is>
       </c>
       <c r="D716" t="n">
@@ -11895,11 +11895,11 @@
         <v>715</v>
       </c>
       <c r="B717" t="n">
-        <v>10100595801</v>
+        <v>10260450980</v>
       </c>
       <c r="C717" t="inlineStr">
         <is>
-          <t>تولي‌پرس‌</t>
+          <t>توكاريل</t>
         </is>
       </c>
       <c r="D717" t="n">
@@ -11911,11 +11911,11 @@
         <v>716</v>
       </c>
       <c r="B718" t="n">
-        <v>10260450980</v>
+        <v>10101702561</v>
       </c>
       <c r="C718" t="inlineStr">
         <is>
-          <t>توكاريل</t>
+          <t>گروه س توسعه صنعتي ايران</t>
         </is>
       </c>
       <c r="D718" t="n">
@@ -11927,11 +11927,11 @@
         <v>717</v>
       </c>
       <c r="B719" t="n">
-        <v>10101702561</v>
+        <v>10103637809</v>
       </c>
       <c r="C719" t="inlineStr">
         <is>
-          <t>گروه س توسعه صنعتي ايران</t>
+          <t>توسعه سامانه ي نرم افزاري نگين</t>
         </is>
       </c>
       <c r="D719" t="n">
@@ -11943,11 +11943,11 @@
         <v>718</v>
       </c>
       <c r="B720" t="n">
-        <v>10103637809</v>
+        <v>10840053064</v>
       </c>
       <c r="C720" t="inlineStr">
         <is>
-          <t>توسعه سامانه ي نرم افزاري نگين</t>
+          <t>زغال سنگ پروده طبس</t>
         </is>
       </c>
       <c r="D720" t="n">
@@ -11959,11 +11959,11 @@
         <v>719</v>
       </c>
       <c r="B721" t="n">
-        <v>10840053064</v>
+        <v>10860726096</v>
       </c>
       <c r="C721" t="inlineStr">
         <is>
-          <t>زغال سنگ پروده طبس</t>
+          <t>پتروشيمي تندگويان</t>
         </is>
       </c>
       <c r="D721" t="n">
@@ -11975,11 +11975,11 @@
         <v>720</v>
       </c>
       <c r="B722" t="n">
-        <v>10860726096</v>
+        <v>10260322490</v>
       </c>
       <c r="C722" t="inlineStr">
         <is>
-          <t>پتروشيمي تندگويان</t>
+          <t>مهندسي مرآت پولاد</t>
         </is>
       </c>
       <c r="D722" t="n">
@@ -11991,11 +11991,11 @@
         <v>721</v>
       </c>
       <c r="B723" t="n">
-        <v>10260322490</v>
+        <v>10260492543</v>
       </c>
       <c r="C723" t="inlineStr">
         <is>
-          <t>مهندسي مرآت پولاد</t>
+          <t>توكا رنگ فولاد سپاهان</t>
         </is>
       </c>
       <c r="D723" t="n">
@@ -12007,11 +12007,11 @@
         <v>722</v>
       </c>
       <c r="B724" t="n">
-        <v>10260492543</v>
+        <v>10200044047</v>
       </c>
       <c r="C724" t="inlineStr">
         <is>
-          <t>توكا رنگ فولاد سپاهان</t>
+          <t>تراكتورسازي‌ايران‌</t>
         </is>
       </c>
       <c r="D724" t="n">
@@ -12023,11 +12023,11 @@
         <v>723</v>
       </c>
       <c r="B725" t="n">
-        <v>10200044047</v>
+        <v>10861521552</v>
       </c>
       <c r="C725" t="inlineStr">
         <is>
-          <t>تراكتورسازي‌ايران‌</t>
+          <t>توريستي ورفاهي آبادگران كيش</t>
         </is>
       </c>
       <c r="D725" t="n">
@@ -12039,11 +12039,11 @@
         <v>724</v>
       </c>
       <c r="B726" t="n">
-        <v>10861521552</v>
+        <v>10100433825</v>
       </c>
       <c r="C726" t="inlineStr">
         <is>
-          <t>توريستي ورفاهي آبادگران كيش</t>
+          <t>ايران‌ ترانسفو</t>
         </is>
       </c>
       <c r="D726" t="n">
@@ -12055,11 +12055,11 @@
         <v>725</v>
       </c>
       <c r="B727" t="n">
-        <v>10100433825</v>
+        <v>10103525426</v>
       </c>
       <c r="C727" t="inlineStr">
         <is>
-          <t>ايران‌ ترانسفو</t>
+          <t>تامين سرمايه امين</t>
         </is>
       </c>
       <c r="D727" t="n">
@@ -12071,11 +12071,11 @@
         <v>726</v>
       </c>
       <c r="B728" t="n">
-        <v>10103525426</v>
+        <v>10101117032</v>
       </c>
       <c r="C728" t="inlineStr">
         <is>
-          <t>تامين سرمايه امين</t>
+          <t>توليد سموم‌ علف‌ كش‌</t>
         </is>
       </c>
       <c r="D728" t="n">
@@ -12087,11 +12087,11 @@
         <v>727</v>
       </c>
       <c r="B729" t="n">
-        <v>10101117032</v>
+        <v>10100539090</v>
       </c>
       <c r="C729" t="inlineStr">
         <is>
-          <t>توليد سموم‌ علف‌ كش‌</t>
+          <t>توسعه‌ صنايع‌ بهشهر(هلدينگ‌</t>
         </is>
       </c>
       <c r="D729" t="n">
@@ -12103,11 +12103,11 @@
         <v>728</v>
       </c>
       <c r="B730" t="n">
-        <v>10100539090</v>
+        <v>10101767219</v>
       </c>
       <c r="C730" t="inlineStr">
         <is>
-          <t>توسعه‌ صنايع‌ بهشهر(هلدينگ‌</t>
+          <t>اعتباري توسعه</t>
         </is>
       </c>
       <c r="D730" t="n">
@@ -12119,11 +12119,11 @@
         <v>729</v>
       </c>
       <c r="B731" t="n">
-        <v>10101767219</v>
+        <v>10100782085</v>
       </c>
       <c r="C731" t="inlineStr">
         <is>
-          <t>اعتباري توسعه</t>
+          <t>سرمايه گذاري پارس‌ توشه‌</t>
         </is>
       </c>
       <c r="D731" t="n">
@@ -12135,11 +12135,11 @@
         <v>730</v>
       </c>
       <c r="B732" t="n">
-        <v>10100782085</v>
+        <v>10100993098</v>
       </c>
       <c r="C732" t="inlineStr">
         <is>
-          <t>سرمايه گذاري پارس‌ توشه‌</t>
+          <t>كارخانجات‌توليدي‌شيشه‌رازي‌</t>
         </is>
       </c>
       <c r="D732" t="n">
@@ -12151,11 +12151,11 @@
         <v>731</v>
       </c>
       <c r="B733" t="n">
-        <v>10100993098</v>
+        <v>10380019602</v>
       </c>
       <c r="C733" t="inlineStr">
         <is>
-          <t>كارخانجات‌توليدي‌شيشه‌رازي‌</t>
+          <t>قند تربت حيدريه</t>
         </is>
       </c>
       <c r="D733" t="n">
@@ -12167,11 +12167,11 @@
         <v>732</v>
       </c>
       <c r="B734" t="n">
-        <v>10380019602</v>
+        <v>10460096368</v>
       </c>
       <c r="C734" t="inlineStr">
         <is>
-          <t>قند تربت حيدريه</t>
+          <t>ترانسفورماتور توزيع زنگان</t>
         </is>
       </c>
       <c r="D734" t="n">
@@ -12183,11 +12183,11 @@
         <v>733</v>
       </c>
       <c r="B735" t="n">
-        <v>10460096368</v>
+        <v>10260057369</v>
       </c>
       <c r="C735" t="inlineStr">
         <is>
-          <t>ترانسفورماتور توزيع زنگان</t>
+          <t>توليدي و خدمات صنايع نسوز توكا</t>
         </is>
       </c>
       <c r="D735" t="n">
@@ -12199,11 +12199,11 @@
         <v>734</v>
       </c>
       <c r="B736" t="n">
-        <v>10260057369</v>
+        <v>10220079472</v>
       </c>
       <c r="C736" t="inlineStr">
         <is>
-          <t>توليدي و خدمات صنايع نسوز توكا</t>
+          <t>پتروشيمي اروميه</t>
         </is>
       </c>
       <c r="D736" t="n">
@@ -12215,11 +12215,11 @@
         <v>735</v>
       </c>
       <c r="B737" t="n">
-        <v>10220079472</v>
+        <v>10220022017</v>
       </c>
       <c r="C737" t="inlineStr">
         <is>
-          <t>پتروشيمي اروميه</t>
+          <t>سيمان سفيد اروميه</t>
         </is>
       </c>
       <c r="D737" t="n">
@@ -12231,11 +12231,11 @@
         <v>736</v>
       </c>
       <c r="B738" t="n">
-        <v>10220022017</v>
+        <v>10103024860</v>
       </c>
       <c r="C738" t="inlineStr">
         <is>
-          <t>سيمان سفيد اروميه</t>
+          <t>ليزينگ اقتصاد نوين</t>
         </is>
       </c>
       <c r="D738" t="n">
@@ -12247,11 +12247,11 @@
         <v>737</v>
       </c>
       <c r="B739" t="n">
-        <v>10103024860</v>
+        <v>10380270277</v>
       </c>
       <c r="C739" t="inlineStr">
         <is>
-          <t>ليزينگ اقتصاد نوين</t>
+          <t>احياء صنايع خراسان</t>
         </is>
       </c>
       <c r="D739" t="n">
@@ -12263,11 +12263,11 @@
         <v>738</v>
       </c>
       <c r="B740" t="n">
-        <v>10380270277</v>
+        <v>10260326724</v>
       </c>
       <c r="C740" t="inlineStr">
         <is>
-          <t>احياء صنايع خراسان</t>
+          <t>م .صنايع و معادن احياء سپاهان</t>
         </is>
       </c>
       <c r="D740" t="n">
@@ -12279,11 +12279,11 @@
         <v>739</v>
       </c>
       <c r="B741" t="n">
-        <v>10260326724</v>
+        <v>10101324421</v>
       </c>
       <c r="C741" t="inlineStr">
         <is>
-          <t>م .صنايع و معادن احياء سپاهان</t>
+          <t>سرمايه گذاري صنايع ايران</t>
         </is>
       </c>
       <c r="D741" t="n">
@@ -12295,11 +12295,11 @@
         <v>740</v>
       </c>
       <c r="B742" t="n">
-        <v>10101324421</v>
+        <v>10100304130</v>
       </c>
       <c r="C742" t="inlineStr">
         <is>
-          <t>سرمايه گذاري صنايع ايران</t>
+          <t>ويتانا</t>
         </is>
       </c>
       <c r="D742" t="n">
@@ -12311,11 +12311,11 @@
         <v>741</v>
       </c>
       <c r="B743" t="n">
-        <v>10100304130</v>
+        <v>10103972003</v>
       </c>
       <c r="C743" t="inlineStr">
         <is>
-          <t>ويتانا</t>
+          <t>واسپاري ملت</t>
         </is>
       </c>
       <c r="D743" t="n">
@@ -12327,11 +12327,11 @@
         <v>742</v>
       </c>
       <c r="B744" t="n">
-        <v>10103972003</v>
+        <v>10102617399</v>
       </c>
       <c r="C744" t="inlineStr">
         <is>
-          <t>واسپاري ملت</t>
+          <t>شركت ليزينگ آريا دانا</t>
         </is>
       </c>
       <c r="D744" t="n">
@@ -12343,11 +12343,11 @@
         <v>743</v>
       </c>
       <c r="B745" t="n">
-        <v>10102617399</v>
+        <v>14004810068</v>
       </c>
       <c r="C745" t="inlineStr">
         <is>
-          <t>شركت ليزينگ آريا دانا</t>
+          <t>گ.مديريت ارزش سرمايه ص ب كشوري</t>
         </is>
       </c>
       <c r="D745" t="n">
@@ -12359,11 +12359,11 @@
         <v>744</v>
       </c>
       <c r="B746" t="n">
-        <v>14004810068</v>
+        <v>10320821816</v>
       </c>
       <c r="C746" t="inlineStr">
         <is>
-          <t>گ.مديريت ارزش سرمايه ص ب كشوري</t>
+          <t>بانك مهر اقتصاد</t>
         </is>
       </c>
       <c r="D746" t="n">
@@ -12375,11 +12375,11 @@
         <v>745</v>
       </c>
       <c r="B747" t="n">
-        <v>10320821816</v>
+        <v>10102681950</v>
       </c>
       <c r="C747" t="inlineStr">
         <is>
-          <t>بانك مهر اقتصاد</t>
+          <t>سرمايه گذاري وثوق امين</t>
         </is>
       </c>
       <c r="D747" t="n">
@@ -12391,11 +12391,11 @@
         <v>746</v>
       </c>
       <c r="B748" t="n">
-        <v>10102681950</v>
+        <v>10860246171</v>
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>سرمايه گذاري وثوق امين</t>
+          <t>بانك سينا</t>
         </is>
       </c>
       <c r="D748" t="n">
@@ -12407,11 +12407,11 @@
         <v>747</v>
       </c>
       <c r="B749" t="n">
-        <v>10860246171</v>
+        <v>10102529006</v>
       </c>
       <c r="C749" t="inlineStr">
         <is>
-          <t>بانك سينا</t>
+          <t>بيمه سينا</t>
         </is>
       </c>
       <c r="D749" t="n">
@@ -12423,11 +12423,11 @@
         <v>748</v>
       </c>
       <c r="B750" t="n">
-        <v>10102529006</v>
+        <v>10861638925</v>
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>بيمه سينا</t>
+          <t>فرانسوز يزد</t>
         </is>
       </c>
       <c r="D750" t="n">
@@ -12439,11 +12439,11 @@
         <v>749</v>
       </c>
       <c r="B751" t="n">
-        <v>10861638925</v>
+        <v>10100440525</v>
       </c>
       <c r="C751" t="inlineStr">
         <is>
-          <t>فرانسوز يزد</t>
+          <t>ايران‌ياساتايرورابر</t>
         </is>
       </c>
       <c r="D751" t="n">
@@ -12455,11 +12455,11 @@
         <v>750</v>
       </c>
       <c r="B752" t="n">
-        <v>10100440525</v>
+        <v>10101016508</v>
       </c>
       <c r="C752" t="inlineStr">
         <is>
-          <t>ايران‌ياساتايرورابر</t>
+          <t>مجتمع صنايع لاستيك يزد</t>
         </is>
       </c>
       <c r="D752" t="n">
@@ -12471,11 +12471,11 @@
         <v>751</v>
       </c>
       <c r="B753" t="n">
-        <v>10101016508</v>
+        <v>10102967236</v>
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>مجتمع صنايع لاستيك يزد</t>
+          <t>پتروشيمي مرجان</t>
         </is>
       </c>
       <c r="D753" t="n">
@@ -12487,11 +12487,11 @@
         <v>752</v>
       </c>
       <c r="B754" t="n">
-        <v>10102967236</v>
+        <v>10000000005</v>
       </c>
       <c r="C754" t="inlineStr">
         <is>
-          <t>پتروشيمي مرجان</t>
+          <t>عمران و مسكن سازان شمالغرب</t>
         </is>
       </c>
       <c r="D754" t="n">
@@ -12503,11 +12503,11 @@
         <v>753</v>
       </c>
       <c r="B755" t="n">
-        <v>10000000005</v>
+        <v>10000000006</v>
       </c>
       <c r="C755" t="inlineStr">
         <is>
-          <t>عمران و مسكن سازان شمالغرب</t>
+          <t>سرمايه گذاري حافظ اعتماد</t>
         </is>
       </c>
       <c r="D755" t="n">
@@ -12519,11 +12519,11 @@
         <v>754</v>
       </c>
       <c r="B756" t="n">
-        <v>10000000006</v>
+        <v>10102801066</v>
       </c>
       <c r="C756" t="inlineStr">
         <is>
-          <t>سرمايه گذاري حافظ اعتماد</t>
+          <t>سرمايه گذاري ارشك</t>
         </is>
       </c>
       <c r="D756" t="n">
@@ -12535,11 +12535,11 @@
         <v>755</v>
       </c>
       <c r="B757" t="n">
-        <v>10102801066</v>
+        <v>10000000007</v>
       </c>
       <c r="C757" t="inlineStr">
         <is>
-          <t>سرمايه گذاري ارشك</t>
+          <t>سرمايه گذاري سيراف</t>
         </is>
       </c>
       <c r="D757" t="n">
@@ -12551,11 +12551,11 @@
         <v>756</v>
       </c>
       <c r="B758" t="n">
-        <v>10000000007</v>
+        <v>10102801961</v>
       </c>
       <c r="C758" t="inlineStr">
         <is>
-          <t>سرمايه گذاري سيراف</t>
+          <t>سرمايه گذاري سليم</t>
         </is>
       </c>
       <c r="D758" t="n">
@@ -12567,11 +12567,11 @@
         <v>757</v>
       </c>
       <c r="B759" t="n">
-        <v>10102801961</v>
+        <v>10102773137</v>
       </c>
       <c r="C759" t="inlineStr">
         <is>
-          <t>سرمايه گذاري سليم</t>
+          <t>سرمايه گذاري زعيم</t>
         </is>
       </c>
       <c r="D759" t="n">
@@ -12583,11 +12583,11 @@
         <v>758</v>
       </c>
       <c r="B760" t="n">
-        <v>10102773137</v>
+        <v>10000000008</v>
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>سرمايه گذاري زعيم</t>
+          <t>سرمايه گذاري اعتصام</t>
         </is>
       </c>
       <c r="D760" t="n">
@@ -12599,11 +12599,11 @@
         <v>759</v>
       </c>
       <c r="B761" t="n">
-        <v>10000000008</v>
+        <v>10000000009</v>
       </c>
       <c r="C761" t="inlineStr">
         <is>
-          <t>سرمايه گذاري اعتصام</t>
+          <t>سرمايه گذاري مفتاح</t>
         </is>
       </c>
       <c r="D761" t="n">
@@ -12615,11 +12615,11 @@
         <v>760</v>
       </c>
       <c r="B762" t="n">
-        <v>10000000009</v>
+        <v>10320856814</v>
       </c>
       <c r="C762" t="inlineStr">
         <is>
-          <t>سرمايه گذاري مفتاح</t>
+          <t>مولدنيروگاهي تجارت فارس</t>
         </is>
       </c>
       <c r="D762" t="n">
@@ -12631,11 +12631,11 @@
         <v>761</v>
       </c>
       <c r="B763" t="n">
-        <v>10320856814</v>
+        <v>10102399345</v>
       </c>
       <c r="C763" t="inlineStr">
         <is>
-          <t>مولدنيروگاهي تجارت فارس</t>
+          <t>گسترش صنعت علوم زيستي</t>
         </is>
       </c>
       <c r="D763" t="n">
@@ -12647,11 +12647,11 @@
         <v>762</v>
       </c>
       <c r="B764" t="n">
-        <v>10102399345</v>
+        <v>10320814852</v>
       </c>
       <c r="C764" t="inlineStr">
         <is>
-          <t>گسترش صنعت علوم زيستي</t>
+          <t>توليد برق پرند مپنا</t>
         </is>
       </c>
       <c r="D764" t="n">
@@ -12663,11 +12663,11 @@
         <v>763</v>
       </c>
       <c r="B765" t="n">
-        <v>10320814852</v>
+        <v>10102169938</v>
       </c>
       <c r="C765" t="inlineStr">
         <is>
-          <t>توليد برق پرند مپنا</t>
+          <t>سرمايه گذاري اعتضاد غدير</t>
         </is>
       </c>
       <c r="D765" t="n">
@@ -12679,11 +12679,11 @@
         <v>764</v>
       </c>
       <c r="B766" t="n">
-        <v>10102169938</v>
+        <v>10000000010</v>
       </c>
       <c r="C766" t="inlineStr">
         <is>
-          <t>سرمايه گذاري اعتضاد غدير</t>
+          <t>شركت اعتباري ثامن</t>
         </is>
       </c>
       <c r="D766" t="n">
@@ -12695,11 +12695,11 @@
         <v>765</v>
       </c>
       <c r="B767" t="n">
-        <v>10000000010</v>
+        <v>10000000011</v>
       </c>
       <c r="C767" t="inlineStr">
         <is>
-          <t>شركت اعتباري ثامن</t>
+          <t>خدمات مديريت صندوق بازنشستگي</t>
         </is>
       </c>
       <c r="D767" t="n">
@@ -12711,11 +12711,11 @@
         <v>766</v>
       </c>
       <c r="B768" t="n">
-        <v>10000000011</v>
+        <v>10102855345</v>
       </c>
       <c r="C768" t="inlineStr">
         <is>
-          <t>خدمات مديريت صندوق بازنشستگي</t>
+          <t>خدمات هوايي سامان</t>
         </is>
       </c>
       <c r="D768" t="n">
@@ -12727,11 +12727,11 @@
         <v>767</v>
       </c>
       <c r="B769" t="n">
-        <v>10102855345</v>
+        <v>10103754436</v>
       </c>
       <c r="C769" t="inlineStr">
         <is>
-          <t>خدمات هوايي سامان</t>
+          <t>فولاد زرند ايرانيان</t>
         </is>
       </c>
       <c r="D769" t="n">
@@ -12743,11 +12743,11 @@
         <v>768</v>
       </c>
       <c r="B770" t="n">
-        <v>10103754436</v>
+        <v>10104088225</v>
       </c>
       <c r="C770" t="inlineStr">
         <is>
-          <t>فولاد زرند ايرانيان</t>
+          <t>فولاد سيرجان ايرانيان</t>
         </is>
       </c>
       <c r="D770" t="n">
@@ -12759,11 +12759,11 @@
         <v>769</v>
       </c>
       <c r="B771" t="n">
-        <v>10104088225</v>
+        <v>10000000012</v>
       </c>
       <c r="C771" t="inlineStr">
         <is>
-          <t>فولاد سيرجان ايرانيان</t>
+          <t>تامين سرمايه كيميا</t>
         </is>
       </c>
       <c r="D771" t="n">
@@ -12775,11 +12775,11 @@
         <v>770</v>
       </c>
       <c r="B772" t="n">
-        <v>10000000012</v>
+        <v>10460086306</v>
       </c>
       <c r="C772" t="inlineStr">
         <is>
-          <t>تامين سرمايه كيميا</t>
+          <t>صنعت روي زنگان</t>
         </is>
       </c>
       <c r="D772" t="n">
@@ -12791,11 +12791,11 @@
         <v>771</v>
       </c>
       <c r="B773" t="n">
-        <v>10460086306</v>
+        <v>10100047773</v>
       </c>
       <c r="C773" t="inlineStr">
         <is>
-          <t>صنعت روي زنگان</t>
+          <t>صنعتي زر ماكارون</t>
         </is>
       </c>
       <c r="D773" t="n">
@@ -12807,11 +12807,11 @@
         <v>772</v>
       </c>
       <c r="B774" t="n">
-        <v>10100047773</v>
+        <v>10101335387</v>
       </c>
       <c r="C774" t="inlineStr">
         <is>
-          <t>صنعتي زر ماكارون</t>
+          <t>مرغ اجداد زربال</t>
         </is>
       </c>
       <c r="D774" t="n">
@@ -12823,11 +12823,11 @@
         <v>773</v>
       </c>
       <c r="B775" t="n">
-        <v>10101335387</v>
+        <v>10000000014</v>
       </c>
       <c r="C775" t="inlineStr">
         <is>
-          <t>مرغ اجداد زربال</t>
+          <t>توسعه گردشگري ايران</t>
         </is>
       </c>
       <c r="D775" t="n">
@@ -12839,11 +12839,11 @@
         <v>774</v>
       </c>
       <c r="B776" t="n">
-        <v>10000000014</v>
+        <v>10000000013</v>
       </c>
       <c r="C776" t="inlineStr">
         <is>
-          <t>توسعه گردشگري ايران</t>
+          <t>حمل و نقل ايران و روسيه</t>
         </is>
       </c>
       <c r="D776" t="n">
@@ -12855,11 +12855,11 @@
         <v>775</v>
       </c>
       <c r="B777" t="n">
-        <v>10000000013</v>
+        <v>10000000015</v>
       </c>
       <c r="C777" t="inlineStr">
         <is>
-          <t>حمل و نقل ايران و روسيه</t>
+          <t>مهندسي جوش ايران</t>
         </is>
       </c>
       <c r="D777" t="n">
@@ -12871,11 +12871,11 @@
         <v>776</v>
       </c>
       <c r="B778" t="n">
-        <v>10000000015</v>
+        <v>10000000016</v>
       </c>
       <c r="C778" t="inlineStr">
         <is>
-          <t>مهندسي جوش ايران</t>
+          <t>خدمات غير صنعتي گاز ايران</t>
         </is>
       </c>
       <c r="D778" t="n">
@@ -12887,11 +12887,11 @@
         <v>777</v>
       </c>
       <c r="B779" t="n">
-        <v>10000000016</v>
+        <v>10000000017</v>
       </c>
       <c r="C779" t="inlineStr">
         <is>
-          <t>خدمات غير صنعتي گاز ايران</t>
+          <t>پايانه ها و مخازن پتروشيمي</t>
         </is>
       </c>
       <c r="D779" t="n">
@@ -12903,11 +12903,11 @@
         <v>778</v>
       </c>
       <c r="B780" t="n">
-        <v>10000000017</v>
+        <v>10000000018</v>
       </c>
       <c r="C780" t="inlineStr">
         <is>
-          <t>پايانه ها و مخازن پتروشيمي</t>
+          <t>كالاي پتروشيمي</t>
         </is>
       </c>
       <c r="D780" t="n">
@@ -12919,11 +12919,11 @@
         <v>779</v>
       </c>
       <c r="B781" t="n">
-        <v>10000000018</v>
+        <v>10861351572</v>
       </c>
       <c r="C781" t="inlineStr">
         <is>
-          <t>كالاي پتروشيمي</t>
+          <t>توليد نيروي برق سهند</t>
         </is>
       </c>
       <c r="D781" t="n">
@@ -12935,11 +12935,11 @@
         <v>780</v>
       </c>
       <c r="B782" t="n">
-        <v>10861351572</v>
+        <v>10101336772</v>
       </c>
       <c r="C782" t="inlineStr">
         <is>
-          <t>توليد نيروي برق سهند</t>
+          <t>بهره برداري نيروگاه دز</t>
         </is>
       </c>
       <c r="D782" t="n">
@@ -12951,11 +12951,11 @@
         <v>781</v>
       </c>
       <c r="B783" t="n">
-        <v>10101336772</v>
+        <v>14008126329</v>
       </c>
       <c r="C783" t="inlineStr">
         <is>
-          <t>بهره برداري نيروگاه دز</t>
+          <t>فن آوا كارت</t>
         </is>
       </c>
       <c r="D783" t="n">
@@ -12967,11 +12967,11 @@
         <v>782</v>
       </c>
       <c r="B784" t="n">
-        <v>14008126329</v>
+        <v>10103978066</v>
       </c>
       <c r="C784" t="inlineStr">
         <is>
-          <t>فن آوا كارت</t>
+          <t>پتروشيمي سلمان فارسي</t>
         </is>
       </c>
       <c r="D784" t="n">
@@ -12983,11 +12983,11 @@
         <v>783</v>
       </c>
       <c r="B785" t="n">
-        <v>10103978066</v>
+        <v>10100627111</v>
       </c>
       <c r="C785" t="inlineStr">
         <is>
-          <t>پتروشيمي سلمان فارسي</t>
+          <t>نوسازي صنايع ايران</t>
         </is>
       </c>
       <c r="D785" t="n">
@@ -12999,11 +12999,11 @@
         <v>784</v>
       </c>
       <c r="B786" t="n">
-        <v>10100627111</v>
+        <v>10100655069</v>
       </c>
       <c r="C786" t="inlineStr">
         <is>
-          <t>نوسازي صنايع ايران</t>
+          <t>ساختماني عمران تكلار</t>
         </is>
       </c>
       <c r="D786" t="n">
@@ -13015,11 +13015,11 @@
         <v>785</v>
       </c>
       <c r="B787" t="n">
-        <v>10100655069</v>
+        <v>10480037917</v>
       </c>
       <c r="C787" t="inlineStr">
         <is>
-          <t>ساختماني عمران تكلار</t>
+          <t>زغالسنگ البرز شرقي</t>
         </is>
       </c>
       <c r="D787" t="n">
@@ -13031,11 +13031,11 @@
         <v>786</v>
       </c>
       <c r="B788" t="n">
-        <v>10480037917</v>
+        <v>10840007960</v>
       </c>
       <c r="C788" t="inlineStr">
         <is>
-          <t>زغالسنگ البرز شرقي</t>
+          <t>سنگ آهن مركزي</t>
         </is>
       </c>
       <c r="D788" t="n">
@@ -13047,11 +13047,11 @@
         <v>787</v>
       </c>
       <c r="B789" t="n">
-        <v>10840007960</v>
+        <v>14005155456</v>
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>سنگ آهن مركزي</t>
+          <t>نيروگاه زاگرس كوثر</t>
         </is>
       </c>
       <c r="D789" t="n">
@@ -13063,11 +13063,11 @@
         <v>788</v>
       </c>
       <c r="B790" t="n">
-        <v>14005155456</v>
+        <v>10680047080</v>
       </c>
       <c r="C790" t="inlineStr">
         <is>
-          <t>نيروگاه زاگرس كوثر</t>
+          <t>شير و گوشت زاگرس شهركرد</t>
         </is>
       </c>
       <c r="D790" t="n">
@@ -13079,11 +13079,11 @@
         <v>789</v>
       </c>
       <c r="B791" t="n">
-        <v>10680047080</v>
+        <v>10320503079</v>
       </c>
       <c r="C791" t="inlineStr">
         <is>
-          <t>شير و گوشت زاگرس شهركرد</t>
+          <t>بانك ايران زمين</t>
         </is>
       </c>
       <c r="D791" t="n">
@@ -13095,11 +13095,11 @@
         <v>790</v>
       </c>
       <c r="B792" t="n">
-        <v>10320503079</v>
+        <v>10100370594</v>
       </c>
       <c r="C792" t="inlineStr">
         <is>
-          <t>بانك ايران زمين</t>
+          <t>زامياد</t>
         </is>
       </c>
       <c r="D792" t="n">
@@ -13111,11 +13111,11 @@
         <v>791</v>
       </c>
       <c r="B793" t="n">
-        <v>10100370594</v>
+        <v>10260482101</v>
       </c>
       <c r="C793" t="inlineStr">
         <is>
-          <t>زامياد</t>
+          <t>سرمايه‌گذاري مسكن زاينده رود</t>
         </is>
       </c>
       <c r="D793" t="n">
@@ -13127,11 +13127,11 @@
         <v>792</v>
       </c>
       <c r="B794" t="n">
-        <v>10260482101</v>
+        <v>10460101525</v>
       </c>
       <c r="C794" t="inlineStr">
         <is>
-          <t>سرمايه‌گذاري مسكن زاينده رود</t>
+          <t>صنايع كشاورزي وكود زنجان</t>
         </is>
       </c>
       <c r="D794" t="n">
@@ -13143,11 +13143,11 @@
         <v>793</v>
       </c>
       <c r="B795" t="n">
-        <v>10460101525</v>
+        <v>10260085303</v>
       </c>
       <c r="C795" t="inlineStr">
         <is>
-          <t>صنايع كشاورزي وكود زنجان</t>
+          <t>ذوب آهن اصفهان</t>
         </is>
       </c>
       <c r="D795" t="n">
@@ -13159,11 +13159,11 @@
         <v>794</v>
       </c>
       <c r="B796" t="n">
-        <v>10260085303</v>
+        <v>10240011565</v>
       </c>
       <c r="C796" t="inlineStr">
         <is>
-          <t>ذوب آهن اصفهان</t>
+          <t>ملي كشت و صنعت و دامپروري پارس</t>
         </is>
       </c>
       <c r="D796" t="n">
@@ -13175,11 +13175,11 @@
         <v>795</v>
       </c>
       <c r="B797" t="n">
-        <v>10240011565</v>
+        <v>10184001687</v>
       </c>
       <c r="C797" t="inlineStr">
         <is>
-          <t>ملي كشت و صنعت و دامپروري پارس</t>
+          <t>گروه ص. پژوهشي فرهيختگان زرنام</t>
         </is>
       </c>
       <c r="D797" t="n">
@@ -13191,11 +13191,11 @@
         <v>796</v>
       </c>
       <c r="B798" t="n">
-        <v>10184001687</v>
+        <v>10861406488</v>
       </c>
       <c r="C798" t="inlineStr">
         <is>
-          <t>گروه ص. پژوهشي فرهيختگان زرنام</t>
+          <t>تولیدی گرانول قزوین</t>
         </is>
       </c>
       <c r="D798" t="n">
@@ -13207,11 +13207,11 @@
         <v>797</v>
       </c>
       <c r="B799" t="n">
-        <v>10861406488</v>
+        <v>10102363667</v>
       </c>
       <c r="C799" t="inlineStr">
         <is>
-          <t>تولیدی گرانول قزوین</t>
+          <t>کوبل دارو</t>
         </is>
       </c>
       <c r="D799" t="n">
@@ -13223,11 +13223,11 @@
         <v>798</v>
       </c>
       <c r="B800" t="n">
-        <v>10102363667</v>
+        <v>14006408218</v>
       </c>
       <c r="C800" t="inlineStr">
         <is>
-          <t>کوبل دارو</t>
+          <t>گروه مدیریت سرمایه لیان</t>
         </is>
       </c>
       <c r="D800" t="n">
@@ -13239,11 +13239,11 @@
         <v>799</v>
       </c>
       <c r="B801" t="n">
-        <v>14006408218</v>
+        <v>14007070869</v>
       </c>
       <c r="C801" t="inlineStr">
         <is>
-          <t>گروه مدیریت سرمایه لیان</t>
+          <t>آرین الوند پارس</t>
         </is>
       </c>
       <c r="D801" t="n">
@@ -13255,11 +13255,11 @@
         <v>800</v>
       </c>
       <c r="B802" t="n">
-        <v>14007070869</v>
+        <v>10000000054</v>
       </c>
       <c r="C802" t="inlineStr">
         <is>
-          <t>آرین الوند پارس</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی صبا گستر نفت و گاز تامین</t>
         </is>
       </c>
       <c r="D802" t="n">
@@ -13271,11 +13271,11 @@
         <v>801</v>
       </c>
       <c r="B803" t="n">
-        <v>10000000054</v>
+        <v>10260181270</v>
       </c>
       <c r="C803" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی صبا گستر نفت و گاز تامین</t>
+          <t>ایثار فجر کاشان</t>
         </is>
       </c>
       <c r="D803" t="n">
@@ -13287,11 +13287,11 @@
         <v>802</v>
       </c>
       <c r="B804" t="n">
-        <v>10260181270</v>
+        <v>10000000019</v>
       </c>
       <c r="C804" t="inlineStr">
         <is>
-          <t>ایثار فجر کاشان</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی آواری زاگرس</t>
         </is>
       </c>
       <c r="D804" t="n">
@@ -13303,11 +13303,11 @@
         <v>803</v>
       </c>
       <c r="B805" t="n">
-        <v>10000000019</v>
+        <v>10102773194</v>
       </c>
       <c r="C805" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی آواری زاگرس</t>
+          <t>سرمایه گذاری امین اعتماد</t>
         </is>
       </c>
       <c r="D805" t="n">
@@ -13319,11 +13319,11 @@
         <v>804</v>
       </c>
       <c r="B806" t="n">
-        <v>10102773194</v>
+        <v>10103492170</v>
       </c>
       <c r="C806" t="inlineStr">
         <is>
-          <t>سرمایه گذاری امین اعتماد</t>
+          <t>گسترش الکترونیک تدبیر ایران</t>
         </is>
       </c>
       <c r="D806" t="n">
@@ -13335,11 +13335,11 @@
         <v>805</v>
       </c>
       <c r="B807" t="n">
-        <v>10103492170</v>
+        <v>10000000063</v>
       </c>
       <c r="C807" t="inlineStr">
         <is>
-          <t>گسترش الکترونیک تدبیر ایران</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی تراز ویستا</t>
         </is>
       </c>
       <c r="D807" t="n">
@@ -13351,11 +13351,11 @@
         <v>806</v>
       </c>
       <c r="B808" t="n">
-        <v>10000000063</v>
+        <v>10103891706</v>
       </c>
       <c r="C808" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی تراز ویستا</t>
+          <t>توسعه سرمایه گذاری دریا ساحل ایرانیان</t>
         </is>
       </c>
       <c r="D808" t="n">
@@ -13367,11 +13367,11 @@
         <v>807</v>
       </c>
       <c r="B809" t="n">
-        <v>10103891706</v>
+        <v>10102987556</v>
       </c>
       <c r="C809" t="inlineStr">
         <is>
-          <t>توسعه سرمایه گذاری دریا ساحل ایرانیان</t>
+          <t>پیشتازان تجارت ویستا</t>
         </is>
       </c>
       <c r="D809" t="n">
@@ -13383,11 +13383,11 @@
         <v>808</v>
       </c>
       <c r="B810" t="n">
-        <v>10102987556</v>
+        <v>10103891690</v>
       </c>
       <c r="C810" t="inlineStr">
         <is>
-          <t>پیشتازان تجارت ویستا</t>
+          <t>توسعه تجارت مجازی سارینا</t>
         </is>
       </c>
       <c r="D810" t="n">
@@ -13399,11 +13399,11 @@
         <v>809</v>
       </c>
       <c r="B811" t="n">
-        <v>10103891690</v>
+        <v>10102911447</v>
       </c>
       <c r="C811" t="inlineStr">
         <is>
-          <t>توسعه تجارت مجازی سارینا</t>
+          <t>نو آوری ستاره پارسیان</t>
         </is>
       </c>
       <c r="D811" t="n">
@@ -13415,11 +13415,11 @@
         <v>810</v>
       </c>
       <c r="B812" t="n">
-        <v>10102911447</v>
+        <v>14008302538</v>
       </c>
       <c r="C812" t="inlineStr">
         <is>
-          <t>نو آوری ستاره پارسیان</t>
+          <t>پیشگامان رشد و نوآوری</t>
         </is>
       </c>
       <c r="D812" t="n">
@@ -13431,11 +13431,11 @@
         <v>811</v>
       </c>
       <c r="B813" t="n">
-        <v>14008302538</v>
+        <v>10103137408</v>
       </c>
       <c r="C813" t="inlineStr">
         <is>
-          <t>پیشگامان رشد و نوآوری</t>
+          <t>سرمایه گذاری آتیه صبا</t>
         </is>
       </c>
       <c r="D813" t="n">
@@ -13447,11 +13447,11 @@
         <v>812</v>
       </c>
       <c r="B814" t="n">
-        <v>10103137408</v>
+        <v>14010024250</v>
       </c>
       <c r="C814" t="inlineStr">
         <is>
-          <t>سرمایه گذاری آتیه صبا</t>
+          <t>توسعه کارآفرینی ماکان</t>
         </is>
       </c>
       <c r="D814" t="n">
@@ -13463,11 +13463,11 @@
         <v>813</v>
       </c>
       <c r="B815" t="n">
-        <v>14010024250</v>
+        <v>14006953961</v>
       </c>
       <c r="C815" t="inlineStr">
         <is>
-          <t>توسعه کارآفرینی ماکان</t>
+          <t>دنیای رشد و نوآوری</t>
         </is>
       </c>
       <c r="D815" t="n">
@@ -13479,11 +13479,11 @@
         <v>814</v>
       </c>
       <c r="B816" t="n">
-        <v>14006953961</v>
+        <v>14009224728</v>
       </c>
       <c r="C816" t="inlineStr">
         <is>
-          <t>دنیای رشد و نوآوری</t>
+          <t>رادیس</t>
         </is>
       </c>
       <c r="D816" t="n">
@@ -13495,11 +13495,11 @@
         <v>815</v>
       </c>
       <c r="B817" t="n">
-        <v>14009224728</v>
+        <v>10101885990</v>
       </c>
       <c r="C817" t="inlineStr">
         <is>
-          <t>رادیس</t>
+          <t>صنعتی آراسته معدن</t>
         </is>
       </c>
       <c r="D817" t="n">
@@ -13511,11 +13511,11 @@
         <v>816</v>
       </c>
       <c r="B818" t="n">
-        <v>10101885990</v>
+        <v>10861503629</v>
       </c>
       <c r="C818" t="inlineStr">
         <is>
-          <t>صنعتی آراسته معدن</t>
+          <t>کوشش آذین قشم</t>
         </is>
       </c>
       <c r="D818" t="n">
@@ -13527,11 +13527,11 @@
         <v>817</v>
       </c>
       <c r="B819" t="n">
-        <v>10861503629</v>
+        <v>10861394039</v>
       </c>
       <c r="C819" t="inlineStr">
         <is>
-          <t>کوشش آذین قشم</t>
+          <t>سرمایه گذاری گلومینکو قشم</t>
         </is>
       </c>
       <c r="D819" t="n">
@@ -13543,11 +13543,11 @@
         <v>818</v>
       </c>
       <c r="B820" t="n">
-        <v>10861394039</v>
+        <v>14001907528</v>
       </c>
       <c r="C820" t="inlineStr">
         <is>
-          <t>سرمایه گذاری گلومینکو قشم</t>
+          <t>بیمه مرکزی جمهوری اسلامی ایران</t>
         </is>
       </c>
       <c r="D820" t="n">
@@ -13559,11 +13559,11 @@
         <v>819</v>
       </c>
       <c r="B821" t="n">
-        <v>14001907528</v>
+        <v>14004046372</v>
       </c>
       <c r="C821" t="inlineStr">
         <is>
-          <t>بیمه مرکزی جمهوری اسلامی ایران</t>
+          <t>گروه مالی پارسیان</t>
         </is>
       </c>
       <c r="D821" t="n">
@@ -13575,11 +13575,11 @@
         <v>820</v>
       </c>
       <c r="B822" t="n">
-        <v>14004046372</v>
+        <v>10103652364</v>
       </c>
       <c r="C822" t="inlineStr">
         <is>
-          <t>گروه مالی پارسیان</t>
+          <t>صنایع آلوم رول نوین</t>
         </is>
       </c>
       <c r="D822" t="n">
@@ -13591,11 +13591,11 @@
         <v>821</v>
       </c>
       <c r="B823" t="n">
-        <v>10103652364</v>
+        <v>10780110885</v>
       </c>
       <c r="C823" t="inlineStr">
         <is>
-          <t>صنایع آلوم رول نوین</t>
+          <t>روان گداز پردیس</t>
         </is>
       </c>
       <c r="D823" t="n">
@@ -13607,11 +13607,11 @@
         <v>822</v>
       </c>
       <c r="B824" t="n">
-        <v>10780110885</v>
+        <v>10103529793</v>
       </c>
       <c r="C824" t="inlineStr">
         <is>
-          <t>روان گداز پردیس</t>
+          <t>مدبر تجارت آریا</t>
         </is>
       </c>
       <c r="D824" t="n">
@@ -13623,11 +13623,11 @@
         <v>823</v>
       </c>
       <c r="B825" t="n">
-        <v>10103529793</v>
+        <v>10103529800</v>
       </c>
       <c r="C825" t="inlineStr">
         <is>
-          <t>مدبر تجارت آریا</t>
+          <t>پرتو کالا پردیس</t>
         </is>
       </c>
       <c r="D825" t="n">
@@ -13639,11 +13639,11 @@
         <v>824</v>
       </c>
       <c r="B826" t="n">
-        <v>10103529800</v>
+        <v>10101195187</v>
       </c>
       <c r="C826" t="inlineStr">
         <is>
-          <t>پرتو کالا پردیس</t>
+          <t>امین آر</t>
         </is>
       </c>
       <c r="D826" t="n">
@@ -13655,11 +13655,11 @@
         <v>825</v>
       </c>
       <c r="B827" t="n">
-        <v>10101195187</v>
+        <v>10380430077</v>
       </c>
       <c r="C827" t="inlineStr">
         <is>
-          <t>امین آر</t>
+          <t>سرمایه گذاری سهام عدالت استان خراسان رضوی</t>
         </is>
       </c>
       <c r="D827" t="n">
@@ -13671,11 +13671,11 @@
         <v>826</v>
       </c>
       <c r="B828" t="n">
-        <v>10380430077</v>
+        <v>10530320996</v>
       </c>
       <c r="C828" t="inlineStr">
         <is>
-          <t>سرمایه گذاری سهام عدالت استان خراسان رضوی</t>
+          <t>سرمایه گذاری استان فارس</t>
         </is>
       </c>
       <c r="D828" t="n">
@@ -13687,11 +13687,11 @@
         <v>827</v>
       </c>
       <c r="B829" t="n">
-        <v>10530320996</v>
+        <v>10860903365</v>
       </c>
       <c r="C829" t="inlineStr">
         <is>
-          <t>سرمایه گذاری استان فارس</t>
+          <t>سرمایه گذاری استان خوزستان</t>
         </is>
       </c>
       <c r="D829" t="n">
@@ -13703,11 +13703,11 @@
         <v>828</v>
       </c>
       <c r="B830" t="n">
-        <v>10860903365</v>
+        <v>10260490269</v>
       </c>
       <c r="C830" t="inlineStr">
         <is>
-          <t>سرمایه گذاری استان خوزستان</t>
+          <t>سرمایه گذاری استان اصفهان</t>
         </is>
       </c>
       <c r="D830" t="n">
@@ -13719,11 +13719,11 @@
         <v>829</v>
       </c>
       <c r="B831" t="n">
-        <v>10260490269</v>
+        <v>10102158022</v>
       </c>
       <c r="C831" t="inlineStr">
         <is>
-          <t>سرمایه گذاری استان اصفهان</t>
+          <t>سازمان توسعه و نوسازی معادن و صنایع معدنی ایران</t>
         </is>
       </c>
       <c r="D831" t="n">
@@ -13735,11 +13735,11 @@
         <v>830</v>
       </c>
       <c r="B832" t="n">
-        <v>10102158022</v>
+        <v>14008307703</v>
       </c>
       <c r="C832" t="inlineStr">
         <is>
-          <t>سازمان توسعه و نوسازی معادن و صنایع معدنی ایران</t>
+          <t>سرو سودمند مدبران</t>
         </is>
       </c>
       <c r="D832" t="n">
@@ -13751,11 +13751,11 @@
         <v>831</v>
       </c>
       <c r="B833" t="n">
-        <v>14008307703</v>
+        <v>14006249920</v>
       </c>
       <c r="C833" t="inlineStr">
         <is>
-          <t>سرو سودمند مدبران</t>
+          <t>تلاش انگیزه دارای آریا</t>
         </is>
       </c>
       <c r="D833" t="n">
@@ -13767,11 +13767,11 @@
         <v>832</v>
       </c>
       <c r="B834" t="n">
-        <v>14006249920</v>
+        <v>14011339503</v>
       </c>
       <c r="C834" t="inlineStr">
         <is>
-          <t>تلاش انگیزه دارای آریا</t>
+          <t>امین سلامت بهاران</t>
         </is>
       </c>
       <c r="D834" t="n">
@@ -13783,11 +13783,11 @@
         <v>833</v>
       </c>
       <c r="B835" t="n">
-        <v>14011339503</v>
+        <v>10320866327</v>
       </c>
       <c r="C835" t="inlineStr">
         <is>
-          <t>امین سلامت بهاران</t>
+          <t>صندوق سرمایه گذاری اندوخته پایدار سپهر</t>
         </is>
       </c>
       <c r="D835" t="n">
@@ -13799,11 +13799,11 @@
         <v>834</v>
       </c>
       <c r="B836" t="n">
-        <v>10320866327</v>
+        <v>14006852814</v>
       </c>
       <c r="C836" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اندوخته پایدار سپهر</t>
+          <t>سازمان اقتصادی کوثر</t>
         </is>
       </c>
       <c r="D836" t="n">
@@ -13815,11 +13815,11 @@
         <v>835</v>
       </c>
       <c r="B837" t="n">
-        <v>14006852814</v>
+        <v>14006012357</v>
       </c>
       <c r="C837" t="inlineStr">
         <is>
-          <t>سازمان اقتصادی کوثر</t>
+          <t>اختصاصی بازارگردانی گروه دی</t>
         </is>
       </c>
       <c r="D837" t="n">
@@ -13831,11 +13831,11 @@
         <v>836</v>
       </c>
       <c r="B838" t="n">
-        <v>14006012357</v>
+        <v>14008473366</v>
       </c>
       <c r="C838" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی گروه دی</t>
+          <t>اختصاصی بازارگردانی پاداش پشتیبان پارس</t>
         </is>
       </c>
       <c r="D838" t="n">
@@ -13847,11 +13847,11 @@
         <v>837</v>
       </c>
       <c r="B839" t="n">
-        <v>14008473366</v>
+        <v>10000000059</v>
       </c>
       <c r="C839" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی پاداش پشتیبان پارس</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی توسعه بازار تمدن</t>
         </is>
       </c>
       <c r="D839" t="n">
@@ -13863,11 +13863,11 @@
         <v>838</v>
       </c>
       <c r="B840" t="n">
-        <v>10000000059</v>
+        <v>14003959426</v>
       </c>
       <c r="C840" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی توسعه بازار تمدن</t>
+          <t>رسا سامان آریا</t>
         </is>
       </c>
       <c r="D840" t="n">
@@ -13879,11 +13879,11 @@
         <v>839</v>
       </c>
       <c r="B841" t="n">
-        <v>14003959426</v>
+        <v>10320600788</v>
       </c>
       <c r="C841" t="inlineStr">
         <is>
-          <t>رسا سامان آریا</t>
+          <t>صندوق سرمایه گذاری بانک گردشگری</t>
         </is>
       </c>
       <c r="D841" t="n">
@@ -13895,11 +13895,11 @@
         <v>840</v>
       </c>
       <c r="B842" t="n">
-        <v>10320600788</v>
+        <v>14005496342</v>
       </c>
       <c r="C842" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری بانک گردشگری</t>
+          <t>صندوق سرمايه گذاري اندوخته توسعه صادرات آرماني</t>
         </is>
       </c>
       <c r="D842" t="n">
@@ -13911,11 +13911,11 @@
         <v>841</v>
       </c>
       <c r="B843" t="n">
-        <v>14005496342</v>
+        <v>10000000099</v>
       </c>
       <c r="C843" t="inlineStr">
         <is>
-          <t>صندوق سرمايه گذاري اندوخته توسعه صادرات آرماني</t>
+          <t>صندوق سرمايه گذاري امين يكم فردا</t>
         </is>
       </c>
       <c r="D843" t="n">
@@ -13927,11 +13927,11 @@
         <v>842</v>
       </c>
       <c r="B844" t="n">
-        <v>10000000099</v>
+        <v>14004128084</v>
       </c>
       <c r="C844" t="inlineStr">
         <is>
-          <t>صندوق سرمايه گذاري امين يكم فردا</t>
+          <t>پارس تامین مجد</t>
         </is>
       </c>
       <c r="D844" t="n">
@@ -13943,11 +13943,11 @@
         <v>843</v>
       </c>
       <c r="B845" t="n">
-        <v>14004128084</v>
+        <v>10103679112</v>
       </c>
       <c r="C845" t="inlineStr">
         <is>
-          <t>پارس تامین مجد</t>
+          <t>گسترش فناوری های نوین</t>
         </is>
       </c>
       <c r="D845" t="n">
@@ -13959,11 +13959,11 @@
         <v>844</v>
       </c>
       <c r="B846" t="n">
-        <v>10103679112</v>
+        <v>10100589211</v>
       </c>
       <c r="C846" t="inlineStr">
         <is>
-          <t>گسترش فناوری های نوین</t>
+          <t>رفاه وتامین اتیه امید</t>
         </is>
       </c>
       <c r="D846" t="n">
@@ -13975,11 +13975,11 @@
         <v>845</v>
       </c>
       <c r="B847" t="n">
-        <v>10100589211</v>
+        <v>10320752394</v>
       </c>
       <c r="C847" t="inlineStr">
         <is>
-          <t>رفاه وتامین اتیه امید</t>
+          <t>صندوق سرمایه گذاری امین آشنا ایرانیان</t>
         </is>
       </c>
       <c r="D847" t="n">
@@ -13991,11 +13991,11 @@
         <v>846</v>
       </c>
       <c r="B848" t="n">
-        <v>10320752394</v>
+        <v>14004183170</v>
       </c>
       <c r="C848" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری امین آشنا ایرانیان</t>
+          <t>حکمت آشنا ایرانیان</t>
         </is>
       </c>
       <c r="D848" t="n">
@@ -14007,11 +14007,11 @@
         <v>847</v>
       </c>
       <c r="B849" t="n">
-        <v>14004183170</v>
+        <v>10100258391</v>
       </c>
       <c r="C849" t="inlineStr">
         <is>
-          <t>حکمت آشنا ایرانیان</t>
+          <t>ملی نفتکش ایران</t>
         </is>
       </c>
       <c r="D849" t="n">
@@ -14023,11 +14023,11 @@
         <v>848</v>
       </c>
       <c r="B850" t="n">
-        <v>10100258391</v>
+        <v>10100906047</v>
       </c>
       <c r="C850" t="inlineStr">
         <is>
-          <t>ملی نفتکش ایران</t>
+          <t>حمل واردات ایران</t>
         </is>
       </c>
       <c r="D850" t="n">
@@ -14039,11 +14039,11 @@
         <v>849</v>
       </c>
       <c r="B851" t="n">
-        <v>10100906047</v>
+        <v>10100976112</v>
       </c>
       <c r="C851" t="inlineStr">
         <is>
-          <t>حمل واردات ایران</t>
+          <t>حمل دریایی ایران</t>
         </is>
       </c>
       <c r="D851" t="n">
@@ -14055,11 +14055,11 @@
         <v>850</v>
       </c>
       <c r="B852" t="n">
-        <v>10100976112</v>
+        <v>10103372005</v>
       </c>
       <c r="C852" t="inlineStr">
         <is>
-          <t>حمل دریایی ایران</t>
+          <t>مفید شیشه</t>
         </is>
       </c>
       <c r="D852" t="n">
@@ -14071,11 +14071,11 @@
         <v>851</v>
       </c>
       <c r="B853" t="n">
-        <v>10103372005</v>
+        <v>14007120347</v>
       </c>
       <c r="C853" t="inlineStr">
         <is>
-          <t>مفید شیشه</t>
+          <t>اختصاصی بازارگردانی سهم آشنا یکم</t>
         </is>
       </c>
       <c r="D853" t="n">
@@ -14087,11 +14087,11 @@
         <v>852</v>
       </c>
       <c r="B854" t="n">
-        <v>14007120347</v>
+        <v>14009518268</v>
       </c>
       <c r="C854" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی سهم آشنا یکم</t>
+          <t>نام آوران تجارت اردستان</t>
         </is>
       </c>
       <c r="D854" t="n">
@@ -14103,11 +14103,11 @@
         <v>853</v>
       </c>
       <c r="B855" t="n">
-        <v>14009518268</v>
+        <v>10630025764</v>
       </c>
       <c r="C855" t="inlineStr">
         <is>
-          <t>نام آوران تجارت اردستان</t>
+          <t>صندوق بازنشستگی شرکت ملی صنایع مس ایران</t>
         </is>
       </c>
       <c r="D855" t="n">
@@ -14119,11 +14119,11 @@
         <v>854</v>
       </c>
       <c r="B856" t="n">
-        <v>10630025764</v>
+        <v>10101915348</v>
       </c>
       <c r="C856" t="inlineStr">
         <is>
-          <t>صندوق بازنشستگی شرکت ملی صنایع مس ایران</t>
+          <t>کارخانجات نورد لوله یاران</t>
         </is>
       </c>
       <c r="D856" t="n">
@@ -14135,11 +14135,11 @@
         <v>855</v>
       </c>
       <c r="B857" t="n">
-        <v>10101915348</v>
+        <v>10320469990</v>
       </c>
       <c r="C857" t="inlineStr">
         <is>
-          <t>کارخانجات نورد لوله یاران</t>
+          <t>پاتین بین الملل پردیس</t>
         </is>
       </c>
       <c r="D857" t="n">
@@ -14151,11 +14151,11 @@
         <v>856</v>
       </c>
       <c r="B858" t="n">
-        <v>10320469990</v>
+        <v>14007123145</v>
       </c>
       <c r="C858" t="inlineStr">
         <is>
-          <t>پاتین بین الملل پردیس</t>
+          <t>تامین آتیه سرزمین ایرانیان</t>
         </is>
       </c>
       <c r="D858" t="n">
@@ -14167,11 +14167,11 @@
         <v>857</v>
       </c>
       <c r="B859" t="n">
-        <v>14007123145</v>
+        <v>10103258569</v>
       </c>
       <c r="C859" t="inlineStr">
         <is>
-          <t>تامین آتیه سرزمین ایرانیان</t>
+          <t>بين المللي سرمايه گذاري ايرانيان</t>
         </is>
       </c>
       <c r="D859" t="n">
@@ -14183,11 +14183,11 @@
         <v>858</v>
       </c>
       <c r="B860" t="n">
-        <v>10103258569</v>
+        <v>10380450359</v>
       </c>
       <c r="C860" t="inlineStr">
         <is>
-          <t>بين المللي سرمايه گذاري ايرانيان</t>
+          <t>سرمایه گذاری آینده نگر شرق</t>
         </is>
       </c>
       <c r="D860" t="n">
@@ -14199,11 +14199,11 @@
         <v>859</v>
       </c>
       <c r="B861" t="n">
-        <v>10380450359</v>
+        <v>14006336023</v>
       </c>
       <c r="C861" t="inlineStr">
         <is>
-          <t>سرمایه گذاری آینده نگر شرق</t>
+          <t>عمران پی ژیوار</t>
         </is>
       </c>
       <c r="D861" t="n">
@@ -14215,11 +14215,11 @@
         <v>860</v>
       </c>
       <c r="B862" t="n">
-        <v>14006336023</v>
+        <v>10320400445</v>
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>عمران پی ژیوار</t>
+          <t>طلایه داران تجارت کاسپین</t>
         </is>
       </c>
       <c r="D862" t="n">
@@ -14231,11 +14231,11 @@
         <v>861</v>
       </c>
       <c r="B863" t="n">
-        <v>10320400445</v>
+        <v>14008157950</v>
       </c>
       <c r="C863" t="inlineStr">
         <is>
-          <t>طلایه داران تجارت کاسپین</t>
+          <t>نیکان سرشت سرزمین ایرانیان</t>
         </is>
       </c>
       <c r="D863" t="n">
@@ -14247,11 +14247,11 @@
         <v>862</v>
       </c>
       <c r="B864" t="n">
-        <v>14008157950</v>
+        <v>10861529184</v>
       </c>
       <c r="C864" t="inlineStr">
         <is>
-          <t>نیکان سرشت سرزمین ایرانیان</t>
+          <t>آی اف اس کیش</t>
         </is>
       </c>
       <c r="D864" t="n">
@@ -14263,11 +14263,11 @@
         <v>863</v>
       </c>
       <c r="B865" t="n">
-        <v>10861529184</v>
+        <v>10000000029</v>
       </c>
       <c r="C865" t="inlineStr">
         <is>
-          <t>آی اف اس کیش</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی افتخار حافظ</t>
         </is>
       </c>
       <c r="D865" t="n">
@@ -14279,11 +14279,11 @@
         <v>864</v>
       </c>
       <c r="B866" t="n">
-        <v>10000000029</v>
+        <v>10102803281</v>
       </c>
       <c r="C866" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی افتخار حافظ</t>
+          <t>سرمایه گذاری دلیران پارس</t>
         </is>
       </c>
       <c r="D866" t="n">
@@ -14295,11 +14295,11 @@
         <v>865</v>
       </c>
       <c r="B867" t="n">
-        <v>10102803281</v>
+        <v>10320650723</v>
       </c>
       <c r="C867" t="inlineStr">
         <is>
-          <t>سرمایه گذاری دلیران پارس</t>
+          <t>پیشگامان توسعه شهری ایرانیان</t>
         </is>
       </c>
       <c r="D867" t="n">
@@ -14311,11 +14311,11 @@
         <v>866</v>
       </c>
       <c r="B868" t="n">
-        <v>10320650723</v>
+        <v>10380305808</v>
       </c>
       <c r="C868" t="inlineStr">
         <is>
-          <t>پیشگامان توسعه شهری ایرانیان</t>
+          <t>آساگستران خراسان</t>
         </is>
       </c>
       <c r="D868" t="n">
@@ -14327,11 +14327,11 @@
         <v>867</v>
       </c>
       <c r="B869" t="n">
-        <v>10380305808</v>
+        <v>14009263200</v>
       </c>
       <c r="C869" t="inlineStr">
         <is>
-          <t>آساگستران خراسان</t>
+          <t>سرمایه گذاری کشاورزی آرتین هیواد</t>
         </is>
       </c>
       <c r="D869" t="n">
@@ -14343,11 +14343,11 @@
         <v>868</v>
       </c>
       <c r="B870" t="n">
-        <v>14009263200</v>
+        <v>10000000060</v>
       </c>
       <c r="C870" t="inlineStr">
         <is>
-          <t>سرمایه گذاری کشاورزی آرتین هیواد</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی توسعه تاک دانا</t>
         </is>
       </c>
       <c r="D870" t="n">
@@ -14359,11 +14359,11 @@
         <v>869</v>
       </c>
       <c r="B871" t="n">
-        <v>10000000060</v>
+        <v>10320813657</v>
       </c>
       <c r="C871" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی توسعه تاک دانا</t>
+          <t>صندوق سرمایه گذاری مشترک آسمان یکم</t>
         </is>
       </c>
       <c r="D871" t="n">
@@ -14375,11 +14375,11 @@
         <v>870</v>
       </c>
       <c r="B872" t="n">
-        <v>10320813657</v>
+        <v>10102694700</v>
       </c>
       <c r="C872" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری مشترک آسمان یکم</t>
+          <t>سرمایه گذاری گروه صنعتی رازی</t>
         </is>
       </c>
       <c r="D872" t="n">
@@ -14391,11 +14391,11 @@
         <v>871</v>
       </c>
       <c r="B873" t="n">
-        <v>10102694700</v>
+        <v>14005108893</v>
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>سرمایه گذاری گروه صنعتی رازی</t>
+          <t>اختصاصی بازار گردان صبا نیک</t>
         </is>
       </c>
       <c r="D873" t="n">
@@ -14407,11 +14407,11 @@
         <v>872</v>
       </c>
       <c r="B874" t="n">
-        <v>14005108893</v>
+        <v>10000000036</v>
       </c>
       <c r="C874" t="inlineStr">
         <is>
-          <t>اختصاصی بازار گردان صبا نیک</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی توسعه فولاد مبارکه</t>
         </is>
       </c>
       <c r="D874" t="n">
@@ -14423,11 +14423,11 @@
         <v>873</v>
       </c>
       <c r="B875" t="n">
-        <v>10000000036</v>
+        <v>14000074621</v>
       </c>
       <c r="C875" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی توسعه فولاد مبارکه</t>
+          <t>شرکت پویا فراز کیش</t>
         </is>
       </c>
       <c r="D875" t="n">
@@ -14439,11 +14439,11 @@
         <v>874</v>
       </c>
       <c r="B876" t="n">
-        <v>14000074621</v>
+        <v>10102801942</v>
       </c>
       <c r="C876" t="inlineStr">
         <is>
-          <t>شرکت پویا فراز کیش</t>
+          <t>گروه مالی ملت</t>
         </is>
       </c>
       <c r="D876" t="n">
@@ -14455,11 +14455,11 @@
         <v>875</v>
       </c>
       <c r="B877" t="n">
-        <v>10102801942</v>
+        <v>10861530138</v>
       </c>
       <c r="C877" t="inlineStr">
         <is>
-          <t>گروه مالی ملت</t>
+          <t>سرمایه گذاری ای اف جی اج کیش</t>
         </is>
       </c>
       <c r="D877" t="n">
@@ -14471,11 +14471,11 @@
         <v>876</v>
       </c>
       <c r="B878" t="n">
-        <v>10861530138</v>
+        <v>10103037570</v>
       </c>
       <c r="C878" t="inlineStr">
         <is>
-          <t>سرمایه گذاری ای اف جی اج کیش</t>
+          <t>مؤسسه صندوق بازنشستگی وظیفه از کار افتادگی و پس انداز کارکنان بانکهای ملی و ادغام شده</t>
         </is>
       </c>
       <c r="D878" t="n">
@@ -14487,11 +14487,11 @@
         <v>877</v>
       </c>
       <c r="B879" t="n">
-        <v>10103037570</v>
+        <v>10101997560</v>
       </c>
       <c r="C879" t="inlineStr">
         <is>
-          <t>مؤسسه صندوق بازنشستگی وظیفه از کار افتادگی و پس انداز کارکنان بانکهای ملی و ادغام شده</t>
+          <t>صبا میهن</t>
         </is>
       </c>
       <c r="D879" t="n">
@@ -14503,11 +14503,11 @@
         <v>878</v>
       </c>
       <c r="B880" t="n">
-        <v>10101997560</v>
+        <v>14004107956</v>
       </c>
       <c r="C880" t="inlineStr">
         <is>
-          <t>صبا میهن</t>
+          <t>مشترک ارزش کاوان آینده</t>
         </is>
       </c>
       <c r="D880" t="n">
@@ -14519,11 +14519,11 @@
         <v>879</v>
       </c>
       <c r="B881" t="n">
-        <v>14004107956</v>
+        <v>10380520955</v>
       </c>
       <c r="C881" t="inlineStr">
         <is>
-          <t>مشترک ارزش کاوان آینده</t>
+          <t>توسعه توس بان امین</t>
         </is>
       </c>
       <c r="D881" t="n">
@@ -14535,11 +14535,11 @@
         <v>880</v>
       </c>
       <c r="B882" t="n">
-        <v>10380520955</v>
+        <v>14006243544</v>
       </c>
       <c r="C882" t="inlineStr">
         <is>
-          <t>توسعه توس بان امین</t>
+          <t>گسترش سرمایه هوشمند</t>
         </is>
       </c>
       <c r="D882" t="n">
@@ -14551,11 +14551,11 @@
         <v>881</v>
       </c>
       <c r="B883" t="n">
-        <v>14006243544</v>
+        <v>10103761233</v>
       </c>
       <c r="C883" t="inlineStr">
         <is>
-          <t>گسترش سرمایه هوشمند</t>
+          <t>گروه مالی ملل</t>
         </is>
       </c>
       <c r="D883" t="n">
@@ -14567,11 +14567,11 @@
         <v>882</v>
       </c>
       <c r="B884" t="n">
-        <v>10103761233</v>
+        <v>14004407347</v>
       </c>
       <c r="C884" t="inlineStr">
         <is>
-          <t>گروه مالی ملل</t>
+          <t>بازارگردانی نوین پیشرو</t>
         </is>
       </c>
       <c r="D884" t="n">
@@ -14583,11 +14583,11 @@
         <v>883</v>
       </c>
       <c r="B885" t="n">
-        <v>14004407347</v>
+        <v>10380647203</v>
       </c>
       <c r="C885" t="inlineStr">
         <is>
-          <t>بازارگردانی نوین پیشرو</t>
+          <t>افق رهباد خاوران توس</t>
         </is>
       </c>
       <c r="D885" t="n">
@@ -14599,11 +14599,11 @@
         <v>884</v>
       </c>
       <c r="B886" t="n">
-        <v>10380647203</v>
+        <v>14007411551</v>
       </c>
       <c r="C886" t="inlineStr">
         <is>
-          <t>افق رهباد خاوران توس</t>
+          <t>تامین انرژی سپنتا توس</t>
         </is>
       </c>
       <c r="D886" t="n">
@@ -14615,11 +14615,11 @@
         <v>885</v>
       </c>
       <c r="B887" t="n">
-        <v>14007411551</v>
+        <v>10320352137</v>
       </c>
       <c r="C887" t="inlineStr">
         <is>
-          <t>تامین انرژی سپنتا توس</t>
+          <t>گروه توسعه اقتصاد ملل</t>
         </is>
       </c>
       <c r="D887" t="n">
@@ -14631,11 +14631,11 @@
         <v>886</v>
       </c>
       <c r="B888" t="n">
-        <v>10320352137</v>
+        <v>10320774211</v>
       </c>
       <c r="C888" t="inlineStr">
         <is>
-          <t>گروه توسعه اقتصاد ملل</t>
+          <t>تجارت نصر البرز</t>
         </is>
       </c>
       <c r="D888" t="n">
@@ -14647,11 +14647,11 @@
         <v>887</v>
       </c>
       <c r="B889" t="n">
-        <v>10320774211</v>
+        <v>10380647222</v>
       </c>
       <c r="C889" t="inlineStr">
         <is>
-          <t>تجارت نصر البرز</t>
+          <t>خاوران جم گسترش تابران</t>
         </is>
       </c>
       <c r="D889" t="n">
@@ -14663,11 +14663,11 @@
         <v>888</v>
       </c>
       <c r="B890" t="n">
-        <v>10380647222</v>
+        <v>10862064732</v>
       </c>
       <c r="C890" t="inlineStr">
         <is>
-          <t>خاوران جم گسترش تابران</t>
+          <t>بانک سپه</t>
         </is>
       </c>
       <c r="D890" t="n">
@@ -14679,11 +14679,11 @@
         <v>889</v>
       </c>
       <c r="B891" t="n">
-        <v>10862064732</v>
+        <v>10101364297</v>
       </c>
       <c r="C891" t="inlineStr">
         <is>
-          <t>بانک سپه</t>
+          <t>صنعتی و بازرگانی غدیر</t>
         </is>
       </c>
       <c r="D891" t="n">
@@ -14695,11 +14695,11 @@
         <v>890</v>
       </c>
       <c r="B892" t="n">
-        <v>10101364297</v>
+        <v>10103837742</v>
       </c>
       <c r="C892" t="inlineStr">
         <is>
-          <t>صنعتی و بازرگانی غدیر</t>
+          <t>سرمایه گذاری آذر</t>
         </is>
       </c>
       <c r="D892" t="n">
@@ -14711,11 +14711,11 @@
         <v>891</v>
       </c>
       <c r="B893" t="n">
-        <v>10103837742</v>
+        <v>10000000043</v>
       </c>
       <c r="C893" t="inlineStr">
         <is>
-          <t>سرمایه گذاری آذر</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی لاجورد دماوند</t>
         </is>
       </c>
       <c r="D893" t="n">
@@ -14727,11 +14727,11 @@
         <v>892</v>
       </c>
       <c r="B894" t="n">
-        <v>10000000043</v>
+        <v>10102898876</v>
       </c>
       <c r="C894" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی لاجورد دماوند</t>
+          <t>سرمایه گذاری مهرگان سرمایه پارس</t>
         </is>
       </c>
       <c r="D894" t="n">
@@ -14743,11 +14743,11 @@
         <v>893</v>
       </c>
       <c r="B895" t="n">
-        <v>10102898876</v>
+        <v>10000000024</v>
       </c>
       <c r="C895" t="inlineStr">
         <is>
-          <t>سرمایه گذاری مهرگان سرمایه پارس</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی آتیه باران</t>
         </is>
       </c>
       <c r="D895" t="n">
@@ -14759,11 +14759,11 @@
         <v>894</v>
       </c>
       <c r="B896" t="n">
-        <v>10000000024</v>
+        <v>14008247684</v>
       </c>
       <c r="C896" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی آتیه باران</t>
+          <t>فناوری اطلاعات و ارتباطات راهبرد</t>
         </is>
       </c>
       <c r="D896" t="n">
@@ -14775,11 +14775,11 @@
         <v>895</v>
       </c>
       <c r="B897" t="n">
-        <v>14008247684</v>
+        <v>14007707492</v>
       </c>
       <c r="C897" t="inlineStr">
         <is>
-          <t>فناوری اطلاعات و ارتباطات راهبرد</t>
+          <t>رسا سازه پی کاوان مهام</t>
         </is>
       </c>
       <c r="D897" t="n">
@@ -14791,11 +14791,11 @@
         <v>896</v>
       </c>
       <c r="B898" t="n">
-        <v>14007707492</v>
+        <v>10320692265</v>
       </c>
       <c r="C898" t="inlineStr">
         <is>
-          <t>رسا سازه پی کاوان مهام</t>
+          <t>آرتا ایده نفیس</t>
         </is>
       </c>
       <c r="D898" t="n">
@@ -14807,11 +14807,11 @@
         <v>897</v>
       </c>
       <c r="B899" t="n">
-        <v>10320692265</v>
+        <v>10320673140</v>
       </c>
       <c r="C899" t="inlineStr">
         <is>
-          <t>آرتا ایده نفیس</t>
+          <t>سرمایه گذاری صنعتی معدنی آریا فاتح خاورمیانه</t>
         </is>
       </c>
       <c r="D899" t="n">
@@ -14823,11 +14823,11 @@
         <v>898</v>
       </c>
       <c r="B900" t="n">
-        <v>10320673140</v>
+        <v>10320692094</v>
       </c>
       <c r="C900" t="inlineStr">
         <is>
-          <t>سرمایه گذاری صنعتی معدنی آریا فاتح خاورمیانه</t>
+          <t>سرمایه گذاری آتیه مداران</t>
         </is>
       </c>
       <c r="D900" t="n">
@@ -14839,11 +14839,11 @@
         <v>899</v>
       </c>
       <c r="B901" t="n">
-        <v>10320692094</v>
+        <v>14004068870</v>
       </c>
       <c r="C901" t="inlineStr">
         <is>
-          <t>سرمایه گذاری آتیه مداران</t>
+          <t>خدمات مدیریت اندیشه آتیه مداران</t>
         </is>
       </c>
       <c r="D901" t="n">
@@ -14855,11 +14855,11 @@
         <v>900</v>
       </c>
       <c r="B902" t="n">
-        <v>14004068870</v>
+        <v>14008556974</v>
       </c>
       <c r="C902" t="inlineStr">
         <is>
-          <t>خدمات مدیریت اندیشه آتیه مداران</t>
+          <t>فناوری ارتباطات و اطلاعات ایده دیجیتال هوشمند</t>
         </is>
       </c>
       <c r="D902" t="n">
@@ -14871,11 +14871,11 @@
         <v>901</v>
       </c>
       <c r="B903" t="n">
-        <v>14008556974</v>
+        <v>10103460290</v>
       </c>
       <c r="C903" t="inlineStr">
         <is>
-          <t>فناوری ارتباطات و اطلاعات ایده دیجیتال هوشمند</t>
+          <t>سرمایه گذاری مهرگان تامین پارس</t>
         </is>
       </c>
       <c r="D903" t="n">
@@ -14887,11 +14887,11 @@
         <v>902</v>
       </c>
       <c r="B904" t="n">
-        <v>10103460290</v>
+        <v>10101442691</v>
       </c>
       <c r="C904" t="inlineStr">
         <is>
-          <t>سرمایه گذاری مهرگان تامین پارس</t>
+          <t>کارگزاری بانک صنعت ومعدن</t>
         </is>
       </c>
       <c r="D904" t="n">
@@ -14903,11 +14903,11 @@
         <v>903</v>
       </c>
       <c r="B905" t="n">
-        <v>10101442691</v>
+        <v>10320307426</v>
       </c>
       <c r="C905" t="inlineStr">
         <is>
-          <t>کارگزاری بانک صنعت ومعدن</t>
+          <t>سرمایه گذاری تامین آتیه مسکن</t>
         </is>
       </c>
       <c r="D905" t="n">
@@ -14919,11 +14919,11 @@
         <v>904</v>
       </c>
       <c r="B906" t="n">
-        <v>10320307426</v>
+        <v>14005253222</v>
       </c>
       <c r="C906" t="inlineStr">
         <is>
-          <t>سرمایه گذاری تامین آتیه مسکن</t>
+          <t>صنعتی ومعدنی ایران</t>
         </is>
       </c>
       <c r="D906" t="n">
@@ -14935,11 +14935,11 @@
         <v>905</v>
       </c>
       <c r="B907" t="n">
-        <v>14005253222</v>
+        <v>10200450670</v>
       </c>
       <c r="C907" t="inlineStr">
         <is>
-          <t>صنعتی ومعدنی ایران</t>
+          <t>گروه صنعتی اشتالز فولاد خاورمیانه</t>
         </is>
       </c>
       <c r="D907" t="n">
@@ -14951,11 +14951,11 @@
         <v>906</v>
       </c>
       <c r="B908" t="n">
-        <v>10200450670</v>
+        <v>14008076836</v>
       </c>
       <c r="C908" t="inlineStr">
         <is>
-          <t>گروه صنعتی اشتالز فولاد خاورمیانه</t>
+          <t>تدبیر فردای نیک</t>
         </is>
       </c>
       <c r="D908" t="n">
@@ -14967,11 +14967,11 @@
         <v>907</v>
       </c>
       <c r="B909" t="n">
-        <v>14008076836</v>
+        <v>10100937493</v>
       </c>
       <c r="C909" t="inlineStr">
         <is>
-          <t>تدبیر فردای نیک</t>
+          <t>مدیریت طرح و توسعه آینده پویا</t>
         </is>
       </c>
       <c r="D909" t="n">
@@ -14983,11 +14983,11 @@
         <v>908</v>
       </c>
       <c r="B910" t="n">
-        <v>10100937493</v>
+        <v>10100505148</v>
       </c>
       <c r="C910" t="inlineStr">
         <is>
-          <t>مدیریت طرح و توسعه آینده پویا</t>
+          <t>مؤسسه بهارستان آسایش</t>
         </is>
       </c>
       <c r="D910" t="n">
@@ -14999,11 +14999,11 @@
         <v>909</v>
       </c>
       <c r="B911" t="n">
-        <v>10100505148</v>
+        <v>10101814661</v>
       </c>
       <c r="C911" t="inlineStr">
         <is>
-          <t>مؤسسه بهارستان آسایش</t>
+          <t>آرتا مبین سحر</t>
         </is>
       </c>
       <c r="D911" t="n">
@@ -15015,11 +15015,11 @@
         <v>910</v>
       </c>
       <c r="B912" t="n">
-        <v>10101814661</v>
+        <v>10320884761</v>
       </c>
       <c r="C912" t="inlineStr">
         <is>
-          <t>آرتا مبین سحر</t>
+          <t>محب گردشگری سلامت ایرانیان</t>
         </is>
       </c>
       <c r="D912" t="n">
@@ -15031,11 +15031,11 @@
         <v>911</v>
       </c>
       <c r="B913" t="n">
-        <v>10320884761</v>
+        <v>10102173008</v>
       </c>
       <c r="C913" t="inlineStr">
         <is>
-          <t>محب گردشگری سلامت ایرانیان</t>
+          <t>گروه تولیدی رنان طب</t>
         </is>
       </c>
       <c r="D913" t="n">
@@ -15047,11 +15047,11 @@
         <v>912</v>
       </c>
       <c r="B914" t="n">
-        <v>10102173008</v>
+        <v>10102593722</v>
       </c>
       <c r="C914" t="inlineStr">
         <is>
-          <t>گروه تولیدی رنان طب</t>
+          <t>گسترش فناوری عمران زیست</t>
         </is>
       </c>
       <c r="D914" t="n">
@@ -15063,11 +15063,11 @@
         <v>913</v>
       </c>
       <c r="B915" t="n">
-        <v>10102593722</v>
+        <v>10104060856</v>
       </c>
       <c r="C915" t="inlineStr">
         <is>
-          <t>گسترش فناوری عمران زیست</t>
+          <t>محب مهر سلامت پارس</t>
         </is>
       </c>
       <c r="D915" t="n">
@@ -15079,11 +15079,11 @@
         <v>914</v>
       </c>
       <c r="B916" t="n">
-        <v>10104060856</v>
+        <v>10000000034</v>
       </c>
       <c r="C916" t="inlineStr">
         <is>
-          <t>محب مهر سلامت پارس</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی توسعه سهام نیکی</t>
         </is>
       </c>
       <c r="D916" t="n">
@@ -15095,11 +15095,11 @@
         <v>915</v>
       </c>
       <c r="B917" t="n">
-        <v>10000000034</v>
+        <v>10000000033</v>
       </c>
       <c r="C917" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی توسعه سهام نیکی</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی تصمیم ساز</t>
         </is>
       </c>
       <c r="D917" t="n">
@@ -15111,11 +15111,11 @@
         <v>916</v>
       </c>
       <c r="B918" t="n">
-        <v>10000000033</v>
+        <v>10320895923</v>
       </c>
       <c r="C918" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی تصمیم ساز</t>
+          <t>سرزمین پهناور مهر</t>
         </is>
       </c>
       <c r="D918" t="n">
@@ -15127,11 +15127,11 @@
         <v>917</v>
       </c>
       <c r="B919" t="n">
-        <v>10320895923</v>
+        <v>14005828941</v>
       </c>
       <c r="C919" t="inlineStr">
         <is>
-          <t>سرزمین پهناور مهر</t>
+          <t>مؤسسه دانش بنیان برکت</t>
         </is>
       </c>
       <c r="D919" t="n">
@@ -15143,11 +15143,11 @@
         <v>918</v>
       </c>
       <c r="B920" t="n">
-        <v>14005828941</v>
+        <v>14006793310</v>
       </c>
       <c r="C920" t="inlineStr">
         <is>
-          <t>مؤسسه دانش بنیان برکت</t>
+          <t>اختصاصی بازارگردانی تدبیرگران فردا</t>
         </is>
       </c>
       <c r="D920" t="n">
@@ -15159,11 +15159,11 @@
         <v>919</v>
       </c>
       <c r="B921" t="n">
-        <v>14006793310</v>
+        <v>14005786478</v>
       </c>
       <c r="C921" t="inlineStr">
         <is>
-          <t>اختصاصی بازارگردانی تدبیرگران فردا</t>
+          <t>مدیریت سرمایه ارزش آفرین دانا</t>
         </is>
       </c>
       <c r="D921" t="n">
@@ -15175,11 +15175,11 @@
         <v>920</v>
       </c>
       <c r="B922" t="n">
-        <v>14005786478</v>
+        <v>14005965618</v>
       </c>
       <c r="C922" t="inlineStr">
         <is>
-          <t>مدیریت سرمایه ارزش آفرین دانا</t>
+          <t>مدیریت سرمایه آسای دانا</t>
         </is>
       </c>
       <c r="D922" t="n">
@@ -15191,11 +15191,11 @@
         <v>921</v>
       </c>
       <c r="B923" t="n">
-        <v>14005965618</v>
+        <v>14005925472</v>
       </c>
       <c r="C923" t="inlineStr">
         <is>
-          <t>مدیریت سرمایه آسای دانا</t>
+          <t>توسعه سرمایه پارمیس</t>
         </is>
       </c>
       <c r="D923" t="n">
@@ -15207,11 +15207,11 @@
         <v>922</v>
       </c>
       <c r="B924" t="n">
-        <v>14005925472</v>
+        <v>14007027064</v>
       </c>
       <c r="C924" t="inlineStr">
         <is>
-          <t>توسعه سرمایه پارمیس</t>
+          <t>باز آفرین ابهر نیکو</t>
         </is>
       </c>
       <c r="D924" t="n">
@@ -15223,11 +15223,11 @@
         <v>923</v>
       </c>
       <c r="B925" t="n">
-        <v>14007027064</v>
+        <v>14007137903</v>
       </c>
       <c r="C925" t="inlineStr">
         <is>
-          <t>باز آفرین ابهر نیکو</t>
+          <t>توسعه کسب و کار باتیس</t>
         </is>
       </c>
       <c r="D925" t="n">
@@ -15239,11 +15239,11 @@
         <v>924</v>
       </c>
       <c r="B926" t="n">
-        <v>14007137903</v>
+        <v>14006082952</v>
       </c>
       <c r="C926" t="inlineStr">
         <is>
-          <t>توسعه کسب و کار باتیس</t>
+          <t>راه سازان تلاش معدن</t>
         </is>
       </c>
       <c r="D926" t="n">
@@ -15255,11 +15255,11 @@
         <v>925</v>
       </c>
       <c r="B927" t="n">
-        <v>14006082952</v>
+        <v>10320780362</v>
       </c>
       <c r="C927" t="inlineStr">
         <is>
-          <t>راه سازان تلاش معدن</t>
+          <t>بنیاد خیریه تات</t>
         </is>
       </c>
       <c r="D927" t="n">
@@ -15271,11 +15271,11 @@
         <v>926</v>
       </c>
       <c r="B928" t="n">
-        <v>10320780362</v>
+        <v>10320858723</v>
       </c>
       <c r="C928" t="inlineStr">
         <is>
-          <t>بنیاد خیریه تات</t>
+          <t>زینت تجارت آریا</t>
         </is>
       </c>
       <c r="D928" t="n">
@@ -15287,11 +15287,11 @@
         <v>927</v>
       </c>
       <c r="B929" t="n">
-        <v>10320858723</v>
+        <v>10320661767</v>
       </c>
       <c r="C929" t="inlineStr">
         <is>
-          <t>زینت تجارت آریا</t>
+          <t>پارس سرمایه تابا</t>
         </is>
       </c>
       <c r="D929" t="n">
@@ -15303,11 +15303,11 @@
         <v>928</v>
       </c>
       <c r="B930" t="n">
-        <v>10320661767</v>
+        <v>10320169213</v>
       </c>
       <c r="C930" t="inlineStr">
         <is>
-          <t>پارس سرمایه تابا</t>
+          <t>تولیدی و صنعتی مهرآوران آتیه البرز</t>
         </is>
       </c>
       <c r="D930" t="n">
@@ -15319,11 +15319,11 @@
         <v>929</v>
       </c>
       <c r="B931" t="n">
-        <v>10320169213</v>
+        <v>10000000055</v>
       </c>
       <c r="C931" t="inlineStr">
         <is>
-          <t>تولیدی و صنعتی مهرآوران آتیه البرز</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی امیدلوتوس پارسیان</t>
         </is>
       </c>
       <c r="D931" t="n">
@@ -15335,11 +15335,11 @@
         <v>930</v>
       </c>
       <c r="B932" t="n">
-        <v>10000000055</v>
+        <v>14005933591</v>
       </c>
       <c r="C932" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی امیدلوتوس پارسیان</t>
+          <t>گروه مالی و اقتصادی آینده</t>
         </is>
       </c>
       <c r="D932" t="n">
@@ -15351,11 +15351,11 @@
         <v>931</v>
       </c>
       <c r="B933" t="n">
-        <v>14005933591</v>
+        <v>10980226256</v>
       </c>
       <c r="C933" t="inlineStr">
         <is>
-          <t>گروه مالی و اقتصادی آینده</t>
+          <t>تجارت کالای دنا کیش</t>
         </is>
       </c>
       <c r="D933" t="n">
@@ -15367,11 +15367,11 @@
         <v>932</v>
       </c>
       <c r="B934" t="n">
-        <v>10980226256</v>
+        <v>10320503955</v>
       </c>
       <c r="C934" t="inlineStr">
         <is>
-          <t>تجارت کالای دنا کیش</t>
+          <t>صندوق سرمایه گذاری یکم کارگزاری بانک کشاورزی</t>
         </is>
       </c>
       <c r="D934" t="n">
@@ -15383,11 +15383,11 @@
         <v>933</v>
       </c>
       <c r="B935" t="n">
-        <v>10320503955</v>
+        <v>10000000026</v>
       </c>
       <c r="C935" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری یکم کارگزاری بانک کشاورزی</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی آرمان اندیش</t>
         </is>
       </c>
       <c r="D935" t="n">
@@ -15399,11 +15399,11 @@
         <v>934</v>
       </c>
       <c r="B936" t="n">
-        <v>10000000026</v>
+        <v>10420196707</v>
       </c>
       <c r="C936" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی آرمان اندیش</t>
+          <t>فنی و مهندسی جنوب تاسیسات</t>
         </is>
       </c>
       <c r="D936" t="n">
@@ -15415,11 +15415,11 @@
         <v>935</v>
       </c>
       <c r="B937" t="n">
-        <v>10420196707</v>
+        <v>10860411138</v>
       </c>
       <c r="C937" t="inlineStr">
         <is>
-          <t>فنی و مهندسی جنوب تاسیسات</t>
+          <t>مهندسی بازرگانی پیام قشم</t>
         </is>
       </c>
       <c r="D937" t="n">
@@ -15431,11 +15431,11 @@
         <v>936</v>
       </c>
       <c r="B938" t="n">
-        <v>10860411138</v>
+        <v>10101759580</v>
       </c>
       <c r="C938" t="inlineStr">
         <is>
-          <t>مهندسی بازرگانی پیام قشم</t>
+          <t>خدمات بازرگانی پیمان امیر</t>
         </is>
       </c>
       <c r="D938" t="n">
@@ -15447,11 +15447,11 @@
         <v>937</v>
       </c>
       <c r="B939" t="n">
-        <v>10101759580</v>
+        <v>10320832748</v>
       </c>
       <c r="C939" t="inlineStr">
         <is>
-          <t>خدمات بازرگانی پیمان امیر</t>
+          <t>گروه مالی شهر</t>
         </is>
       </c>
       <c r="D939" t="n">
@@ -15463,11 +15463,11 @@
         <v>938</v>
       </c>
       <c r="B940" t="n">
-        <v>10320832748</v>
+        <v>10760094603</v>
       </c>
       <c r="C940" t="inlineStr">
         <is>
-          <t>گروه مالی شهر</t>
+          <t>گسترش کشاورزی و دامپروری فردوس پارس</t>
         </is>
       </c>
       <c r="D940" t="n">
@@ -15479,11 +15479,11 @@
         <v>939</v>
       </c>
       <c r="B941" t="n">
-        <v>10760094603</v>
+        <v>10100171920</v>
       </c>
       <c r="C941" t="inlineStr">
         <is>
-          <t>گسترش کشاورزی و دامپروری فردوس پارس</t>
+          <t>بنیاد مستضعفان انقلاب اسلامی</t>
         </is>
       </c>
       <c r="D941" t="n">
@@ -15495,11 +15495,11 @@
         <v>940</v>
       </c>
       <c r="B942" t="n">
-        <v>10100171920</v>
+        <v>10000000040</v>
       </c>
       <c r="C942" t="inlineStr">
         <is>
-          <t>بنیاد مستضعفان انقلاب اسلامی</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی سینا بهگزین</t>
         </is>
       </c>
       <c r="D942" t="n">
@@ -15511,11 +15511,11 @@
         <v>941</v>
       </c>
       <c r="B943" t="n">
-        <v>10000000040</v>
+        <v>10100625070</v>
       </c>
       <c r="C943" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی سینا بهگزین</t>
+          <t>مؤسسه صندوق بیمه اجتماعی روستاییان و عشایر</t>
         </is>
       </c>
       <c r="D943" t="n">
@@ -15527,11 +15527,11 @@
         <v>942</v>
       </c>
       <c r="B944" t="n">
-        <v>10100625070</v>
+        <v>14003674869</v>
       </c>
       <c r="C944" t="inlineStr">
         <is>
-          <t>مؤسسه صندوق بیمه اجتماعی روستاییان و عشایر</t>
+          <t>خردمندان صابر عصر</t>
         </is>
       </c>
       <c r="D944" t="n">
@@ -15543,11 +15543,11 @@
         <v>943</v>
       </c>
       <c r="B945" t="n">
-        <v>14003674869</v>
+        <v>14009108895</v>
       </c>
       <c r="C945" t="inlineStr">
         <is>
-          <t>خردمندان صابر عصر</t>
+          <t>صندوق سرمايه گذاري واسطه گري مالي يكم</t>
         </is>
       </c>
       <c r="D945" t="n">
@@ -15559,11 +15559,11 @@
         <v>944</v>
       </c>
       <c r="B946" t="n">
-        <v>14009108895</v>
+        <v>10000000030</v>
       </c>
       <c r="C946" t="inlineStr">
         <is>
-          <t>صندوق سرمايه گذاري واسطه گري مالي يكم</t>
+          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی اکسیرسودا</t>
         </is>
       </c>
       <c r="D946" t="n">
@@ -15575,11 +15575,11 @@
         <v>945</v>
       </c>
       <c r="B947" t="n">
-        <v>10000000030</v>
+        <v>14008036097</v>
       </c>
       <c r="C947" t="inlineStr">
         <is>
-          <t>صندوق سرمایه گذاری اختصاصی بازارگردانی اکسیرسودا</t>
+          <t>سرمایه گذاری تجاری سامانه های رایانه ای هوپاد هونامیک</t>
         </is>
       </c>
       <c r="D947" t="n">
@@ -15591,11 +15591,11 @@
         <v>946</v>
       </c>
       <c r="B948" t="n">
-        <v>14008036097</v>
+        <v>10100053930</v>
       </c>
       <c r="C948" t="inlineStr">
         <is>
-          <t>سرمایه گذاری تجاری سامانه های رایانه ای هوپاد هونامیک</t>
+          <t>خدمات مدیریت صبا تامین</t>
         </is>
       </c>
       <c r="D948" t="n">
@@ -15607,11 +15607,11 @@
         <v>947</v>
       </c>
       <c r="B949" t="n">
-        <v>10100053930</v>
+        <v>14004684611</v>
       </c>
       <c r="C949" t="inlineStr">
         <is>
-          <t>خدمات مدیریت صبا تامین</t>
+          <t>با درآمد ثابت کاردان</t>
         </is>
       </c>
       <c r="D949" t="n">
@@ -15623,11 +15623,11 @@
         <v>948</v>
       </c>
       <c r="B950" t="n">
-        <v>14004684611</v>
+        <v>10100351811</v>
       </c>
       <c r="C950" t="inlineStr">
         <is>
-          <t>با درآمد ثابت کاردان</t>
+          <t>گروه مالی و اقتصادی دی</t>
         </is>
       </c>
       <c r="D950" t="n">
@@ -15639,11 +15639,11 @@
         <v>949</v>
       </c>
       <c r="B951" t="n">
-        <v>10100351811</v>
+        <v>10320539175</v>
       </c>
       <c r="C951" t="inlineStr">
         <is>
-          <t>گروه مالی و اقتصادی دی</t>
+          <t>خدمات مالی حسابداری دی ایرانیان</t>
         </is>
       </c>
       <c r="D951" t="n">
@@ -15655,11 +15655,11 @@
         <v>950</v>
       </c>
       <c r="B952" t="n">
-        <v>10320539175</v>
+        <v>10100567400</v>
       </c>
       <c r="C952" t="inlineStr">
         <is>
-          <t>خدمات مالی حسابداری دی ایرانیان</t>
+          <t>اندوخته شاهد</t>
         </is>
       </c>
       <c r="D952" t="n">
@@ -15671,11 +15671,11 @@
         <v>951</v>
       </c>
       <c r="B953" t="n">
-        <v>10100567400</v>
+        <v>14009263160</v>
       </c>
       <c r="C953" t="inlineStr">
         <is>
-          <t>اندوخته شاهد</t>
+          <t>سرمایه گذاری اقتصادی هامرز راتین</t>
         </is>
       </c>
       <c r="D953" t="n">
@@ -15687,11 +15687,11 @@
         <v>952</v>
       </c>
       <c r="B954" t="n">
-        <v>14009263160</v>
+        <v>10861677542</v>
       </c>
       <c r="C954" t="inlineStr">
         <is>
-          <t>سرمایه گذاری اقتصادی هامرز راتین</t>
+          <t>بانک ملی</t>
         </is>
       </c>
       <c r="D954" t="n">

</xml_diff>

<commit_message>
Seperating business group graph and adding Mellat banks
</commit_message>
<xml_diff>
--- a/f_Vector_for_family.xlsx
+++ b/f_Vector_for_family.xlsx
@@ -2044,9 +2044,6 @@
     <t>سيمان‌ تهران‌</t>
   </si>
   <si>
-    <t>سرمايه گذاري صبا تامين</t>
-  </si>
-  <si>
     <t>پتروشيمي گلستان</t>
   </si>
   <si>
@@ -3242,6 +3239,9 @@
   </si>
   <si>
     <t>ویرا سهند تبریز</t>
+  </si>
+  <si>
+    <t>دولت جمهوري اسلامي ايران</t>
   </si>
   <si>
     <t>اختصاصی بازارگردانی ملت</t>
@@ -7188,7 +7188,7 @@
         <v>54</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>0.0635</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -7272,7 +7272,7 @@
         <v>60</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>0.124</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -7650,7 +7650,7 @@
         <v>87</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>0.0992</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -7678,7 +7678,7 @@
         <v>89</v>
       </c>
       <c r="D88">
-        <v>0.1116</v>
+        <v>0.0334</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -7748,7 +7748,7 @@
         <v>94</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -7818,7 +7818,7 @@
         <v>99</v>
       </c>
       <c r="D98">
-        <v>0.5099</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -7874,7 +7874,7 @@
         <v>103</v>
       </c>
       <c r="D102">
-        <v>0.0871</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -7958,7 +7958,7 @@
         <v>109</v>
       </c>
       <c r="D108">
-        <v>0.1014</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -8014,7 +8014,7 @@
         <v>113</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -8756,7 +8756,7 @@
         <v>166</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>0.0673</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -8910,7 +8910,7 @@
         <v>177</v>
       </c>
       <c r="D176">
-        <v>0</v>
+        <v>0.0648</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -9260,7 +9260,7 @@
         <v>202</v>
       </c>
       <c r="D201">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -10016,7 +10016,7 @@
         <v>256</v>
       </c>
       <c r="D255">
-        <v>0</v>
+        <v>0.6596</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -10170,7 +10170,7 @@
         <v>267</v>
       </c>
       <c r="D266">
-        <v>0</v>
+        <v>0.0236</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -11346,7 +11346,7 @@
         <v>351</v>
       </c>
       <c r="D350">
-        <v>0</v>
+        <v>0.0751</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -12130,7 +12130,7 @@
         <v>407</v>
       </c>
       <c r="D406">
-        <v>0</v>
+        <v>0.0738</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -12200,7 +12200,7 @@
         <v>412</v>
       </c>
       <c r="D411">
-        <v>0.1976</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -12606,7 +12606,7 @@
         <v>441</v>
       </c>
       <c r="D440">
-        <v>0</v>
+        <v>0.0636</v>
       </c>
     </row>
     <row r="441" spans="1:4">
@@ -14006,7 +14006,7 @@
         <v>541</v>
       </c>
       <c r="D540">
-        <v>0</v>
+        <v>0.0891</v>
       </c>
     </row>
     <row r="541" spans="1:4">
@@ -14482,7 +14482,7 @@
         <v>575</v>
       </c>
       <c r="D574">
-        <v>0</v>
+        <v>0.2514</v>
       </c>
     </row>
     <row r="575" spans="1:4">
@@ -15890,7 +15890,7 @@
         <v>673</v>
       </c>
       <c r="B675">
-        <v>10101908370</v>
+        <v>10700144582</v>
       </c>
       <c r="C675" t="s">
         <v>676</v>
@@ -15904,7 +15904,7 @@
         <v>674</v>
       </c>
       <c r="B676">
-        <v>10700144582</v>
+        <v>10220016318</v>
       </c>
       <c r="C676" t="s">
         <v>677</v>
@@ -15918,7 +15918,7 @@
         <v>675</v>
       </c>
       <c r="B677">
-        <v>10220016318</v>
+        <v>10460051496</v>
       </c>
       <c r="C677" t="s">
         <v>678</v>
@@ -15932,7 +15932,7 @@
         <v>676</v>
       </c>
       <c r="B678">
-        <v>10460051496</v>
+        <v>10102239945</v>
       </c>
       <c r="C678" t="s">
         <v>679</v>
@@ -15946,7 +15946,7 @@
         <v>677</v>
       </c>
       <c r="B679">
-        <v>10102239945</v>
+        <v>10101212701</v>
       </c>
       <c r="C679" t="s">
         <v>680</v>
@@ -15960,7 +15960,7 @@
         <v>678</v>
       </c>
       <c r="B680">
-        <v>10101212701</v>
+        <v>10101754741</v>
       </c>
       <c r="C680" t="s">
         <v>681</v>
@@ -15974,7 +15974,7 @@
         <v>679</v>
       </c>
       <c r="B681">
-        <v>10101754741</v>
+        <v>10260328876</v>
       </c>
       <c r="C681" t="s">
         <v>682</v>
@@ -15988,7 +15988,7 @@
         <v>680</v>
       </c>
       <c r="B682">
-        <v>10260328876</v>
+        <v>10100387143</v>
       </c>
       <c r="C682" t="s">
         <v>683</v>
@@ -16002,7 +16002,7 @@
         <v>681</v>
       </c>
       <c r="B683">
-        <v>10100387143</v>
+        <v>10100580397</v>
       </c>
       <c r="C683" t="s">
         <v>684</v>
@@ -16016,7 +16016,7 @@
         <v>682</v>
       </c>
       <c r="B684">
-        <v>10100580397</v>
+        <v>10101044869</v>
       </c>
       <c r="C684" t="s">
         <v>685</v>
@@ -16030,7 +16030,7 @@
         <v>683</v>
       </c>
       <c r="B685">
-        <v>10101044869</v>
+        <v>14005751499</v>
       </c>
       <c r="C685" t="s">
         <v>686</v>
@@ -16044,7 +16044,7 @@
         <v>684</v>
       </c>
       <c r="B686">
-        <v>14005751499</v>
+        <v>10320839651</v>
       </c>
       <c r="C686" t="s">
         <v>687</v>
@@ -16058,7 +16058,7 @@
         <v>685</v>
       </c>
       <c r="B687">
-        <v>10320839651</v>
+        <v>10100478433</v>
       </c>
       <c r="C687" t="s">
         <v>688</v>
@@ -16072,7 +16072,7 @@
         <v>686</v>
       </c>
       <c r="B688">
-        <v>10100478433</v>
+        <v>10200142417</v>
       </c>
       <c r="C688" t="s">
         <v>689</v>
@@ -16086,7 +16086,7 @@
         <v>687</v>
       </c>
       <c r="B689">
-        <v>10200142417</v>
+        <v>10260357602</v>
       </c>
       <c r="C689" t="s">
         <v>690</v>
@@ -16100,7 +16100,7 @@
         <v>688</v>
       </c>
       <c r="B690">
-        <v>10260357602</v>
+        <v>10260377008</v>
       </c>
       <c r="C690" t="s">
         <v>691</v>
@@ -16114,7 +16114,7 @@
         <v>689</v>
       </c>
       <c r="B691">
-        <v>10260377008</v>
+        <v>10101907666</v>
       </c>
       <c r="C691" t="s">
         <v>692</v>
@@ -16128,7 +16128,7 @@
         <v>690</v>
       </c>
       <c r="B692">
-        <v>10101907666</v>
+        <v>10260439863</v>
       </c>
       <c r="C692" t="s">
         <v>693</v>
@@ -16142,7 +16142,7 @@
         <v>691</v>
       </c>
       <c r="B693">
-        <v>10260439863</v>
+        <v>10380266337</v>
       </c>
       <c r="C693" t="s">
         <v>694</v>
@@ -16156,7 +16156,7 @@
         <v>692</v>
       </c>
       <c r="B694">
-        <v>10380266337</v>
+        <v>10100254685</v>
       </c>
       <c r="C694" t="s">
         <v>695</v>
@@ -16170,7 +16170,7 @@
         <v>693</v>
       </c>
       <c r="B695">
-        <v>10100254685</v>
+        <v>10380466986</v>
       </c>
       <c r="C695" t="s">
         <v>696</v>
@@ -16184,7 +16184,7 @@
         <v>694</v>
       </c>
       <c r="B696">
-        <v>10380466986</v>
+        <v>10103251617</v>
       </c>
       <c r="C696" t="s">
         <v>697</v>
@@ -16198,7 +16198,7 @@
         <v>695</v>
       </c>
       <c r="B697">
-        <v>10103251617</v>
+        <v>10260289240</v>
       </c>
       <c r="C697" t="s">
         <v>698</v>
@@ -16212,7 +16212,7 @@
         <v>696</v>
       </c>
       <c r="B698">
-        <v>10260289240</v>
+        <v>10101477062</v>
       </c>
       <c r="C698" t="s">
         <v>699</v>
@@ -16226,7 +16226,7 @@
         <v>697</v>
       </c>
       <c r="B699">
-        <v>10101477062</v>
+        <v>10000000004</v>
       </c>
       <c r="C699" t="s">
         <v>700</v>
@@ -16240,7 +16240,7 @@
         <v>698</v>
       </c>
       <c r="B700">
-        <v>10000000004</v>
+        <v>10861658680</v>
       </c>
       <c r="C700" t="s">
         <v>701</v>
@@ -16254,7 +16254,7 @@
         <v>699</v>
       </c>
       <c r="B701">
-        <v>10861658680</v>
+        <v>10260294158</v>
       </c>
       <c r="C701" t="s">
         <v>702</v>
@@ -16268,7 +16268,7 @@
         <v>700</v>
       </c>
       <c r="B702">
-        <v>10260294158</v>
+        <v>10101021508</v>
       </c>
       <c r="C702" t="s">
         <v>703</v>
@@ -16282,7 +16282,7 @@
         <v>701</v>
       </c>
       <c r="B703">
-        <v>10101021508</v>
+        <v>10320741707</v>
       </c>
       <c r="C703" t="s">
         <v>704</v>
@@ -16296,7 +16296,7 @@
         <v>702</v>
       </c>
       <c r="B704">
-        <v>10320741707</v>
+        <v>10102501905</v>
       </c>
       <c r="C704" t="s">
         <v>705</v>
@@ -16310,7 +16310,7 @@
         <v>703</v>
       </c>
       <c r="B705">
-        <v>10102501905</v>
+        <v>10320585987</v>
       </c>
       <c r="C705" t="s">
         <v>706</v>
@@ -16324,7 +16324,7 @@
         <v>704</v>
       </c>
       <c r="B706">
-        <v>10320585987</v>
+        <v>10101136712</v>
       </c>
       <c r="C706" t="s">
         <v>707</v>
@@ -16338,7 +16338,7 @@
         <v>705</v>
       </c>
       <c r="B707">
-        <v>10101136712</v>
+        <v>10320453421</v>
       </c>
       <c r="C707" t="s">
         <v>708</v>
@@ -16352,7 +16352,7 @@
         <v>706</v>
       </c>
       <c r="B708">
-        <v>10320453421</v>
+        <v>10320826260</v>
       </c>
       <c r="C708" t="s">
         <v>709</v>
@@ -16366,7 +16366,7 @@
         <v>707</v>
       </c>
       <c r="B709">
-        <v>10320826260</v>
+        <v>10101725603</v>
       </c>
       <c r="C709" t="s">
         <v>710</v>
@@ -16380,7 +16380,7 @@
         <v>708</v>
       </c>
       <c r="B710">
-        <v>10101725603</v>
+        <v>14005725237</v>
       </c>
       <c r="C710" t="s">
         <v>711</v>
@@ -16394,7 +16394,7 @@
         <v>709</v>
       </c>
       <c r="B711">
-        <v>14005725237</v>
+        <v>10103584900</v>
       </c>
       <c r="C711" t="s">
         <v>712</v>
@@ -16408,7 +16408,7 @@
         <v>710</v>
       </c>
       <c r="B712">
-        <v>10103584900</v>
+        <v>14005652664</v>
       </c>
       <c r="C712" t="s">
         <v>713</v>
@@ -16422,7 +16422,7 @@
         <v>711</v>
       </c>
       <c r="B713">
-        <v>14005652664</v>
+        <v>10260272518</v>
       </c>
       <c r="C713" t="s">
         <v>714</v>
@@ -16436,7 +16436,7 @@
         <v>712</v>
       </c>
       <c r="B714">
-        <v>10260272518</v>
+        <v>10260041071</v>
       </c>
       <c r="C714" t="s">
         <v>715</v>
@@ -16450,7 +16450,7 @@
         <v>713</v>
       </c>
       <c r="B715">
-        <v>10260041071</v>
+        <v>10101912330</v>
       </c>
       <c r="C715" t="s">
         <v>716</v>
@@ -16464,7 +16464,7 @@
         <v>714</v>
       </c>
       <c r="B716">
-        <v>10101912330</v>
+        <v>10100595801</v>
       </c>
       <c r="C716" t="s">
         <v>717</v>
@@ -16478,7 +16478,7 @@
         <v>715</v>
       </c>
       <c r="B717">
-        <v>10100595801</v>
+        <v>10260450980</v>
       </c>
       <c r="C717" t="s">
         <v>718</v>
@@ -16492,7 +16492,7 @@
         <v>716</v>
       </c>
       <c r="B718">
-        <v>10260450980</v>
+        <v>10101702561</v>
       </c>
       <c r="C718" t="s">
         <v>719</v>
@@ -16506,7 +16506,7 @@
         <v>717</v>
       </c>
       <c r="B719">
-        <v>10101702561</v>
+        <v>10103637809</v>
       </c>
       <c r="C719" t="s">
         <v>720</v>
@@ -16520,7 +16520,7 @@
         <v>718</v>
       </c>
       <c r="B720">
-        <v>10103637809</v>
+        <v>10840053064</v>
       </c>
       <c r="C720" t="s">
         <v>721</v>
@@ -16534,7 +16534,7 @@
         <v>719</v>
       </c>
       <c r="B721">
-        <v>10840053064</v>
+        <v>10860726096</v>
       </c>
       <c r="C721" t="s">
         <v>722</v>
@@ -16548,7 +16548,7 @@
         <v>720</v>
       </c>
       <c r="B722">
-        <v>10860726096</v>
+        <v>10260322490</v>
       </c>
       <c r="C722" t="s">
         <v>723</v>
@@ -16562,7 +16562,7 @@
         <v>721</v>
       </c>
       <c r="B723">
-        <v>10260322490</v>
+        <v>10260492543</v>
       </c>
       <c r="C723" t="s">
         <v>724</v>
@@ -16576,7 +16576,7 @@
         <v>722</v>
       </c>
       <c r="B724">
-        <v>10260492543</v>
+        <v>10200044047</v>
       </c>
       <c r="C724" t="s">
         <v>725</v>
@@ -16590,7 +16590,7 @@
         <v>723</v>
       </c>
       <c r="B725">
-        <v>10200044047</v>
+        <v>10861521552</v>
       </c>
       <c r="C725" t="s">
         <v>726</v>
@@ -16604,7 +16604,7 @@
         <v>724</v>
       </c>
       <c r="B726">
-        <v>10861521552</v>
+        <v>10100433825</v>
       </c>
       <c r="C726" t="s">
         <v>727</v>
@@ -16618,13 +16618,13 @@
         <v>725</v>
       </c>
       <c r="B727">
-        <v>10100433825</v>
+        <v>10103525426</v>
       </c>
       <c r="C727" t="s">
         <v>728</v>
       </c>
       <c r="D727">
-        <v>0</v>
+        <v>0.2563</v>
       </c>
     </row>
     <row r="728" spans="1:4">
@@ -16632,7 +16632,7 @@
         <v>726</v>
       </c>
       <c r="B728">
-        <v>10103525426</v>
+        <v>10101117032</v>
       </c>
       <c r="C728" t="s">
         <v>729</v>
@@ -16646,7 +16646,7 @@
         <v>727</v>
       </c>
       <c r="B729">
-        <v>10101117032</v>
+        <v>10100539090</v>
       </c>
       <c r="C729" t="s">
         <v>730</v>
@@ -16660,7 +16660,7 @@
         <v>728</v>
       </c>
       <c r="B730">
-        <v>10100539090</v>
+        <v>10101767219</v>
       </c>
       <c r="C730" t="s">
         <v>731</v>
@@ -16674,7 +16674,7 @@
         <v>729</v>
       </c>
       <c r="B731">
-        <v>10101767219</v>
+        <v>10100782085</v>
       </c>
       <c r="C731" t="s">
         <v>732</v>
@@ -16688,7 +16688,7 @@
         <v>730</v>
       </c>
       <c r="B732">
-        <v>10100782085</v>
+        <v>10100993098</v>
       </c>
       <c r="C732" t="s">
         <v>733</v>
@@ -16702,7 +16702,7 @@
         <v>731</v>
       </c>
       <c r="B733">
-        <v>10100993098</v>
+        <v>10380019602</v>
       </c>
       <c r="C733" t="s">
         <v>734</v>
@@ -16716,7 +16716,7 @@
         <v>732</v>
       </c>
       <c r="B734">
-        <v>10380019602</v>
+        <v>10460096368</v>
       </c>
       <c r="C734" t="s">
         <v>735</v>
@@ -16730,7 +16730,7 @@
         <v>733</v>
       </c>
       <c r="B735">
-        <v>10460096368</v>
+        <v>10260057369</v>
       </c>
       <c r="C735" t="s">
         <v>736</v>
@@ -16744,7 +16744,7 @@
         <v>734</v>
       </c>
       <c r="B736">
-        <v>10260057369</v>
+        <v>10220079472</v>
       </c>
       <c r="C736" t="s">
         <v>737</v>
@@ -16758,7 +16758,7 @@
         <v>735</v>
       </c>
       <c r="B737">
-        <v>10220079472</v>
+        <v>10220022017</v>
       </c>
       <c r="C737" t="s">
         <v>738</v>
@@ -16772,7 +16772,7 @@
         <v>736</v>
       </c>
       <c r="B738">
-        <v>10220022017</v>
+        <v>10103024860</v>
       </c>
       <c r="C738" t="s">
         <v>739</v>
@@ -16786,7 +16786,7 @@
         <v>737</v>
       </c>
       <c r="B739">
-        <v>10103024860</v>
+        <v>10380270277</v>
       </c>
       <c r="C739" t="s">
         <v>740</v>
@@ -16800,7 +16800,7 @@
         <v>738</v>
       </c>
       <c r="B740">
-        <v>10380270277</v>
+        <v>10260326724</v>
       </c>
       <c r="C740" t="s">
         <v>741</v>
@@ -16814,7 +16814,7 @@
         <v>739</v>
       </c>
       <c r="B741">
-        <v>10260326724</v>
+        <v>10101324421</v>
       </c>
       <c r="C741" t="s">
         <v>742</v>
@@ -16828,7 +16828,7 @@
         <v>740</v>
       </c>
       <c r="B742">
-        <v>10101324421</v>
+        <v>10100304130</v>
       </c>
       <c r="C742" t="s">
         <v>743</v>
@@ -16842,7 +16842,7 @@
         <v>741</v>
       </c>
       <c r="B743">
-        <v>10100304130</v>
+        <v>10103972003</v>
       </c>
       <c r="C743" t="s">
         <v>744</v>
@@ -16856,7 +16856,7 @@
         <v>742</v>
       </c>
       <c r="B744">
-        <v>10103972003</v>
+        <v>10102617399</v>
       </c>
       <c r="C744" t="s">
         <v>745</v>
@@ -16870,7 +16870,7 @@
         <v>743</v>
       </c>
       <c r="B745">
-        <v>10102617399</v>
+        <v>14004810068</v>
       </c>
       <c r="C745" t="s">
         <v>746</v>
@@ -16884,7 +16884,7 @@
         <v>744</v>
       </c>
       <c r="B746">
-        <v>14004810068</v>
+        <v>10320821816</v>
       </c>
       <c r="C746" t="s">
         <v>747</v>
@@ -16898,7 +16898,7 @@
         <v>745</v>
       </c>
       <c r="B747">
-        <v>10320821816</v>
+        <v>10102681950</v>
       </c>
       <c r="C747" t="s">
         <v>748</v>
@@ -16912,7 +16912,7 @@
         <v>746</v>
       </c>
       <c r="B748">
-        <v>10102681950</v>
+        <v>10860246171</v>
       </c>
       <c r="C748" t="s">
         <v>749</v>
@@ -16926,7 +16926,7 @@
         <v>747</v>
       </c>
       <c r="B749">
-        <v>10860246171</v>
+        <v>10102529006</v>
       </c>
       <c r="C749" t="s">
         <v>750</v>
@@ -16940,7 +16940,7 @@
         <v>748</v>
       </c>
       <c r="B750">
-        <v>10102529006</v>
+        <v>10861638925</v>
       </c>
       <c r="C750" t="s">
         <v>751</v>
@@ -16954,7 +16954,7 @@
         <v>749</v>
       </c>
       <c r="B751">
-        <v>10861638925</v>
+        <v>10100440525</v>
       </c>
       <c r="C751" t="s">
         <v>752</v>
@@ -16968,7 +16968,7 @@
         <v>750</v>
       </c>
       <c r="B752">
-        <v>10100440525</v>
+        <v>10101016508</v>
       </c>
       <c r="C752" t="s">
         <v>753</v>
@@ -16982,7 +16982,7 @@
         <v>751</v>
       </c>
       <c r="B753">
-        <v>10101016508</v>
+        <v>10102967236</v>
       </c>
       <c r="C753" t="s">
         <v>754</v>
@@ -16996,7 +16996,7 @@
         <v>752</v>
       </c>
       <c r="B754">
-        <v>10102967236</v>
+        <v>10000000005</v>
       </c>
       <c r="C754" t="s">
         <v>755</v>
@@ -17010,7 +17010,7 @@
         <v>753</v>
       </c>
       <c r="B755">
-        <v>10000000005</v>
+        <v>10000000006</v>
       </c>
       <c r="C755" t="s">
         <v>756</v>
@@ -17024,7 +17024,7 @@
         <v>754</v>
       </c>
       <c r="B756">
-        <v>10000000006</v>
+        <v>10102801066</v>
       </c>
       <c r="C756" t="s">
         <v>757</v>
@@ -17038,7 +17038,7 @@
         <v>755</v>
       </c>
       <c r="B757">
-        <v>10102801066</v>
+        <v>10000000007</v>
       </c>
       <c r="C757" t="s">
         <v>758</v>
@@ -17052,7 +17052,7 @@
         <v>756</v>
       </c>
       <c r="B758">
-        <v>10000000007</v>
+        <v>10102801961</v>
       </c>
       <c r="C758" t="s">
         <v>759</v>
@@ -17066,7 +17066,7 @@
         <v>757</v>
       </c>
       <c r="B759">
-        <v>10102801961</v>
+        <v>10102773137</v>
       </c>
       <c r="C759" t="s">
         <v>760</v>
@@ -17080,7 +17080,7 @@
         <v>758</v>
       </c>
       <c r="B760">
-        <v>10102773137</v>
+        <v>10000000008</v>
       </c>
       <c r="C760" t="s">
         <v>761</v>
@@ -17094,7 +17094,7 @@
         <v>759</v>
       </c>
       <c r="B761">
-        <v>10000000008</v>
+        <v>10000000009</v>
       </c>
       <c r="C761" t="s">
         <v>762</v>
@@ -17108,7 +17108,7 @@
         <v>760</v>
       </c>
       <c r="B762">
-        <v>10000000009</v>
+        <v>10320856814</v>
       </c>
       <c r="C762" t="s">
         <v>763</v>
@@ -17122,7 +17122,7 @@
         <v>761</v>
       </c>
       <c r="B763">
-        <v>10320856814</v>
+        <v>10102399345</v>
       </c>
       <c r="C763" t="s">
         <v>764</v>
@@ -17136,7 +17136,7 @@
         <v>762</v>
       </c>
       <c r="B764">
-        <v>10102399345</v>
+        <v>10320814852</v>
       </c>
       <c r="C764" t="s">
         <v>765</v>
@@ -17150,7 +17150,7 @@
         <v>763</v>
       </c>
       <c r="B765">
-        <v>10320814852</v>
+        <v>10102169938</v>
       </c>
       <c r="C765" t="s">
         <v>766</v>
@@ -17164,7 +17164,7 @@
         <v>764</v>
       </c>
       <c r="B766">
-        <v>10102169938</v>
+        <v>10000000010</v>
       </c>
       <c r="C766" t="s">
         <v>767</v>
@@ -17178,7 +17178,7 @@
         <v>765</v>
       </c>
       <c r="B767">
-        <v>10000000010</v>
+        <v>10000000011</v>
       </c>
       <c r="C767" t="s">
         <v>768</v>
@@ -17192,7 +17192,7 @@
         <v>766</v>
       </c>
       <c r="B768">
-        <v>10000000011</v>
+        <v>10102855345</v>
       </c>
       <c r="C768" t="s">
         <v>769</v>
@@ -17206,7 +17206,7 @@
         <v>767</v>
       </c>
       <c r="B769">
-        <v>10102855345</v>
+        <v>10103754436</v>
       </c>
       <c r="C769" t="s">
         <v>770</v>
@@ -17220,7 +17220,7 @@
         <v>768</v>
       </c>
       <c r="B770">
-        <v>10103754436</v>
+        <v>10104088225</v>
       </c>
       <c r="C770" t="s">
         <v>771</v>
@@ -17234,7 +17234,7 @@
         <v>769</v>
       </c>
       <c r="B771">
-        <v>10104088225</v>
+        <v>10000000012</v>
       </c>
       <c r="C771" t="s">
         <v>772</v>
@@ -17248,7 +17248,7 @@
         <v>770</v>
       </c>
       <c r="B772">
-        <v>10000000012</v>
+        <v>10460086306</v>
       </c>
       <c r="C772" t="s">
         <v>773</v>
@@ -17262,7 +17262,7 @@
         <v>771</v>
       </c>
       <c r="B773">
-        <v>10460086306</v>
+        <v>10100047773</v>
       </c>
       <c r="C773" t="s">
         <v>774</v>
@@ -17276,7 +17276,7 @@
         <v>772</v>
       </c>
       <c r="B774">
-        <v>10100047773</v>
+        <v>10101335387</v>
       </c>
       <c r="C774" t="s">
         <v>775</v>
@@ -17290,7 +17290,7 @@
         <v>773</v>
       </c>
       <c r="B775">
-        <v>10101335387</v>
+        <v>10000000014</v>
       </c>
       <c r="C775" t="s">
         <v>776</v>
@@ -17304,7 +17304,7 @@
         <v>774</v>
       </c>
       <c r="B776">
-        <v>10000000014</v>
+        <v>10000000013</v>
       </c>
       <c r="C776" t="s">
         <v>777</v>
@@ -17318,7 +17318,7 @@
         <v>775</v>
       </c>
       <c r="B777">
-        <v>10000000013</v>
+        <v>10000000015</v>
       </c>
       <c r="C777" t="s">
         <v>778</v>
@@ -17332,7 +17332,7 @@
         <v>776</v>
       </c>
       <c r="B778">
-        <v>10000000015</v>
+        <v>10000000016</v>
       </c>
       <c r="C778" t="s">
         <v>779</v>
@@ -17346,7 +17346,7 @@
         <v>777</v>
       </c>
       <c r="B779">
-        <v>10000000016</v>
+        <v>10000000017</v>
       </c>
       <c r="C779" t="s">
         <v>780</v>
@@ -17360,7 +17360,7 @@
         <v>778</v>
       </c>
       <c r="B780">
-        <v>10000000017</v>
+        <v>10000000018</v>
       </c>
       <c r="C780" t="s">
         <v>781</v>
@@ -17374,7 +17374,7 @@
         <v>779</v>
       </c>
       <c r="B781">
-        <v>10000000018</v>
+        <v>10861351572</v>
       </c>
       <c r="C781" t="s">
         <v>782</v>
@@ -17388,7 +17388,7 @@
         <v>780</v>
       </c>
       <c r="B782">
-        <v>10861351572</v>
+        <v>10101336772</v>
       </c>
       <c r="C782" t="s">
         <v>783</v>
@@ -17402,7 +17402,7 @@
         <v>781</v>
       </c>
       <c r="B783">
-        <v>10101336772</v>
+        <v>14008126329</v>
       </c>
       <c r="C783" t="s">
         <v>784</v>
@@ -17416,7 +17416,7 @@
         <v>782</v>
       </c>
       <c r="B784">
-        <v>14008126329</v>
+        <v>10103978066</v>
       </c>
       <c r="C784" t="s">
         <v>785</v>
@@ -17430,7 +17430,7 @@
         <v>783</v>
       </c>
       <c r="B785">
-        <v>10103978066</v>
+        <v>10100627111</v>
       </c>
       <c r="C785" t="s">
         <v>786</v>
@@ -17444,7 +17444,7 @@
         <v>784</v>
       </c>
       <c r="B786">
-        <v>10100627111</v>
+        <v>10100655069</v>
       </c>
       <c r="C786" t="s">
         <v>787</v>
@@ -17458,7 +17458,7 @@
         <v>785</v>
       </c>
       <c r="B787">
-        <v>10100655069</v>
+        <v>10480037917</v>
       </c>
       <c r="C787" t="s">
         <v>788</v>
@@ -17472,7 +17472,7 @@
         <v>786</v>
       </c>
       <c r="B788">
-        <v>10480037917</v>
+        <v>10840007960</v>
       </c>
       <c r="C788" t="s">
         <v>789</v>
@@ -17486,7 +17486,7 @@
         <v>787</v>
       </c>
       <c r="B789">
-        <v>10840007960</v>
+        <v>14005155456</v>
       </c>
       <c r="C789" t="s">
         <v>790</v>
@@ -17500,7 +17500,7 @@
         <v>788</v>
       </c>
       <c r="B790">
-        <v>14005155456</v>
+        <v>10680047080</v>
       </c>
       <c r="C790" t="s">
         <v>791</v>
@@ -17514,7 +17514,7 @@
         <v>789</v>
       </c>
       <c r="B791">
-        <v>10680047080</v>
+        <v>10320503079</v>
       </c>
       <c r="C791" t="s">
         <v>792</v>
@@ -17528,7 +17528,7 @@
         <v>790</v>
       </c>
       <c r="B792">
-        <v>10320503079</v>
+        <v>10100370594</v>
       </c>
       <c r="C792" t="s">
         <v>793</v>
@@ -17542,7 +17542,7 @@
         <v>791</v>
       </c>
       <c r="B793">
-        <v>10100370594</v>
+        <v>10260482101</v>
       </c>
       <c r="C793" t="s">
         <v>794</v>
@@ -17556,7 +17556,7 @@
         <v>792</v>
       </c>
       <c r="B794">
-        <v>10260482101</v>
+        <v>10460101525</v>
       </c>
       <c r="C794" t="s">
         <v>795</v>
@@ -17570,7 +17570,7 @@
         <v>793</v>
       </c>
       <c r="B795">
-        <v>10460101525</v>
+        <v>10260085303</v>
       </c>
       <c r="C795" t="s">
         <v>796</v>
@@ -17584,7 +17584,7 @@
         <v>794</v>
       </c>
       <c r="B796">
-        <v>10260085303</v>
+        <v>10240011565</v>
       </c>
       <c r="C796" t="s">
         <v>797</v>
@@ -17598,7 +17598,7 @@
         <v>795</v>
       </c>
       <c r="B797">
-        <v>10240011565</v>
+        <v>10184001687</v>
       </c>
       <c r="C797" t="s">
         <v>798</v>
@@ -17612,7 +17612,7 @@
         <v>796</v>
       </c>
       <c r="B798">
-        <v>10184001687</v>
+        <v>10320311482</v>
       </c>
       <c r="C798" t="s">
         <v>799</v>
@@ -17626,7 +17626,7 @@
         <v>797</v>
       </c>
       <c r="B799">
-        <v>10320311482</v>
+        <v>10320718470</v>
       </c>
       <c r="C799" t="s">
         <v>800</v>
@@ -17640,7 +17640,7 @@
         <v>798</v>
       </c>
       <c r="B800">
-        <v>10320718470</v>
+        <v>10103714248</v>
       </c>
       <c r="C800" t="s">
         <v>801</v>
@@ -17654,7 +17654,7 @@
         <v>799</v>
       </c>
       <c r="B801">
-        <v>10103714248</v>
+        <v>14008341286</v>
       </c>
       <c r="C801" t="s">
         <v>802</v>
@@ -17668,7 +17668,7 @@
         <v>800</v>
       </c>
       <c r="B802">
-        <v>14008341286</v>
+        <v>14005790156</v>
       </c>
       <c r="C802" t="s">
         <v>803</v>
@@ -17682,7 +17682,7 @@
         <v>801</v>
       </c>
       <c r="B803">
-        <v>14005790156</v>
+        <v>10102801942</v>
       </c>
       <c r="C803" t="s">
         <v>804</v>
@@ -17696,7 +17696,7 @@
         <v>802</v>
       </c>
       <c r="B804">
-        <v>10102801942</v>
+        <v>10101165910</v>
       </c>
       <c r="C804" t="s">
         <v>805</v>
@@ -17710,7 +17710,7 @@
         <v>803</v>
       </c>
       <c r="B805">
-        <v>10101165910</v>
+        <v>14004003162</v>
       </c>
       <c r="C805" t="s">
         <v>806</v>
@@ -17724,7 +17724,7 @@
         <v>804</v>
       </c>
       <c r="B806">
-        <v>14004003162</v>
+        <v>10861406488</v>
       </c>
       <c r="C806" t="s">
         <v>807</v>
@@ -17738,7 +17738,7 @@
         <v>805</v>
       </c>
       <c r="B807">
-        <v>10861406488</v>
+        <v>10102363667</v>
       </c>
       <c r="C807" t="s">
         <v>808</v>
@@ -17752,7 +17752,7 @@
         <v>806</v>
       </c>
       <c r="B808">
-        <v>10102363667</v>
+        <v>14006408218</v>
       </c>
       <c r="C808" t="s">
         <v>809</v>
@@ -17766,7 +17766,7 @@
         <v>807</v>
       </c>
       <c r="B809">
-        <v>14006408218</v>
+        <v>14007070869</v>
       </c>
       <c r="C809" t="s">
         <v>810</v>
@@ -17780,7 +17780,7 @@
         <v>808</v>
       </c>
       <c r="B810">
-        <v>14007070869</v>
+        <v>10000000054</v>
       </c>
       <c r="C810" t="s">
         <v>811</v>
@@ -17794,7 +17794,7 @@
         <v>809</v>
       </c>
       <c r="B811">
-        <v>10000000054</v>
+        <v>10260181270</v>
       </c>
       <c r="C811" t="s">
         <v>812</v>
@@ -17808,7 +17808,7 @@
         <v>810</v>
       </c>
       <c r="B812">
-        <v>10260181270</v>
+        <v>10000000019</v>
       </c>
       <c r="C812" t="s">
         <v>813</v>
@@ -17822,7 +17822,7 @@
         <v>811</v>
       </c>
       <c r="B813">
-        <v>10000000019</v>
+        <v>10102773194</v>
       </c>
       <c r="C813" t="s">
         <v>814</v>
@@ -17836,7 +17836,7 @@
         <v>812</v>
       </c>
       <c r="B814">
-        <v>10102773194</v>
+        <v>10103492170</v>
       </c>
       <c r="C814" t="s">
         <v>815</v>
@@ -17850,7 +17850,7 @@
         <v>813</v>
       </c>
       <c r="B815">
-        <v>10103492170</v>
+        <v>10000000063</v>
       </c>
       <c r="C815" t="s">
         <v>816</v>
@@ -17864,7 +17864,7 @@
         <v>814</v>
       </c>
       <c r="B816">
-        <v>10000000063</v>
+        <v>10103891706</v>
       </c>
       <c r="C816" t="s">
         <v>817</v>
@@ -17878,7 +17878,7 @@
         <v>815</v>
       </c>
       <c r="B817">
-        <v>10103891706</v>
+        <v>10102987556</v>
       </c>
       <c r="C817" t="s">
         <v>818</v>
@@ -17892,7 +17892,7 @@
         <v>816</v>
       </c>
       <c r="B818">
-        <v>10102987556</v>
+        <v>10103891690</v>
       </c>
       <c r="C818" t="s">
         <v>819</v>
@@ -17906,7 +17906,7 @@
         <v>817</v>
       </c>
       <c r="B819">
-        <v>10103891690</v>
+        <v>10102911447</v>
       </c>
       <c r="C819" t="s">
         <v>820</v>
@@ -17920,7 +17920,7 @@
         <v>818</v>
       </c>
       <c r="B820">
-        <v>10102911447</v>
+        <v>14008302538</v>
       </c>
       <c r="C820" t="s">
         <v>821</v>
@@ -17934,7 +17934,7 @@
         <v>819</v>
       </c>
       <c r="B821">
-        <v>14008302538</v>
+        <v>10103137408</v>
       </c>
       <c r="C821" t="s">
         <v>822</v>
@@ -17948,7 +17948,7 @@
         <v>820</v>
       </c>
       <c r="B822">
-        <v>10103137408</v>
+        <v>14010024250</v>
       </c>
       <c r="C822" t="s">
         <v>823</v>
@@ -17962,7 +17962,7 @@
         <v>821</v>
       </c>
       <c r="B823">
-        <v>14010024250</v>
+        <v>14006953961</v>
       </c>
       <c r="C823" t="s">
         <v>824</v>
@@ -17976,7 +17976,7 @@
         <v>822</v>
       </c>
       <c r="B824">
-        <v>14006953961</v>
+        <v>14009224728</v>
       </c>
       <c r="C824" t="s">
         <v>825</v>
@@ -17990,7 +17990,7 @@
         <v>823</v>
       </c>
       <c r="B825">
-        <v>14009224728</v>
+        <v>10101885990</v>
       </c>
       <c r="C825" t="s">
         <v>826</v>
@@ -18004,7 +18004,7 @@
         <v>824</v>
       </c>
       <c r="B826">
-        <v>10101885990</v>
+        <v>10861503629</v>
       </c>
       <c r="C826" t="s">
         <v>827</v>
@@ -18018,7 +18018,7 @@
         <v>825</v>
       </c>
       <c r="B827">
-        <v>10861503629</v>
+        <v>10861394039</v>
       </c>
       <c r="C827" t="s">
         <v>828</v>
@@ -18032,7 +18032,7 @@
         <v>826</v>
       </c>
       <c r="B828">
-        <v>10861394039</v>
+        <v>14001907528</v>
       </c>
       <c r="C828" t="s">
         <v>829</v>
@@ -18046,7 +18046,7 @@
         <v>827</v>
       </c>
       <c r="B829">
-        <v>14001907528</v>
+        <v>14004046372</v>
       </c>
       <c r="C829" t="s">
         <v>830</v>
@@ -18060,7 +18060,7 @@
         <v>828</v>
       </c>
       <c r="B830">
-        <v>14004046372</v>
+        <v>10103652364</v>
       </c>
       <c r="C830" t="s">
         <v>831</v>
@@ -18074,7 +18074,7 @@
         <v>829</v>
       </c>
       <c r="B831">
-        <v>10103652364</v>
+        <v>10780110885</v>
       </c>
       <c r="C831" t="s">
         <v>832</v>
@@ -18088,7 +18088,7 @@
         <v>830</v>
       </c>
       <c r="B832">
-        <v>10780110885</v>
+        <v>10103529793</v>
       </c>
       <c r="C832" t="s">
         <v>833</v>
@@ -18102,7 +18102,7 @@
         <v>831</v>
       </c>
       <c r="B833">
-        <v>10103529793</v>
+        <v>10103529800</v>
       </c>
       <c r="C833" t="s">
         <v>834</v>
@@ -18116,7 +18116,7 @@
         <v>832</v>
       </c>
       <c r="B834">
-        <v>10103529800</v>
+        <v>10101195187</v>
       </c>
       <c r="C834" t="s">
         <v>835</v>
@@ -18130,7 +18130,7 @@
         <v>833</v>
       </c>
       <c r="B835">
-        <v>10101195187</v>
+        <v>10380430077</v>
       </c>
       <c r="C835" t="s">
         <v>836</v>
@@ -18144,7 +18144,7 @@
         <v>834</v>
       </c>
       <c r="B836">
-        <v>10380430077</v>
+        <v>10530320996</v>
       </c>
       <c r="C836" t="s">
         <v>837</v>
@@ -18158,7 +18158,7 @@
         <v>835</v>
       </c>
       <c r="B837">
-        <v>10530320996</v>
+        <v>10860903365</v>
       </c>
       <c r="C837" t="s">
         <v>838</v>
@@ -18172,7 +18172,7 @@
         <v>836</v>
       </c>
       <c r="B838">
-        <v>10860903365</v>
+        <v>10260490269</v>
       </c>
       <c r="C838" t="s">
         <v>839</v>
@@ -18186,7 +18186,7 @@
         <v>837</v>
       </c>
       <c r="B839">
-        <v>10260490269</v>
+        <v>10102158022</v>
       </c>
       <c r="C839" t="s">
         <v>840</v>
@@ -18200,7 +18200,7 @@
         <v>838</v>
       </c>
       <c r="B840">
-        <v>10102158022</v>
+        <v>14008307703</v>
       </c>
       <c r="C840" t="s">
         <v>841</v>
@@ -18214,7 +18214,7 @@
         <v>839</v>
       </c>
       <c r="B841">
-        <v>14008307703</v>
+        <v>14006249920</v>
       </c>
       <c r="C841" t="s">
         <v>842</v>
@@ -18228,7 +18228,7 @@
         <v>840</v>
       </c>
       <c r="B842">
-        <v>14006249920</v>
+        <v>14011339503</v>
       </c>
       <c r="C842" t="s">
         <v>843</v>
@@ -18242,7 +18242,7 @@
         <v>841</v>
       </c>
       <c r="B843">
-        <v>14011339503</v>
+        <v>10320866327</v>
       </c>
       <c r="C843" t="s">
         <v>844</v>
@@ -18256,7 +18256,7 @@
         <v>842</v>
       </c>
       <c r="B844">
-        <v>10320866327</v>
+        <v>14006852814</v>
       </c>
       <c r="C844" t="s">
         <v>845</v>
@@ -18270,7 +18270,7 @@
         <v>843</v>
       </c>
       <c r="B845">
-        <v>14006852814</v>
+        <v>14006012357</v>
       </c>
       <c r="C845" t="s">
         <v>846</v>
@@ -18284,7 +18284,7 @@
         <v>844</v>
       </c>
       <c r="B846">
-        <v>14006012357</v>
+        <v>14008473366</v>
       </c>
       <c r="C846" t="s">
         <v>847</v>
@@ -18298,7 +18298,7 @@
         <v>845</v>
       </c>
       <c r="B847">
-        <v>14008473366</v>
+        <v>10000000059</v>
       </c>
       <c r="C847" t="s">
         <v>848</v>
@@ -18312,7 +18312,7 @@
         <v>846</v>
       </c>
       <c r="B848">
-        <v>10000000059</v>
+        <v>14003959426</v>
       </c>
       <c r="C848" t="s">
         <v>849</v>
@@ -18326,7 +18326,7 @@
         <v>847</v>
       </c>
       <c r="B849">
-        <v>14003959426</v>
+        <v>10320600788</v>
       </c>
       <c r="C849" t="s">
         <v>850</v>
@@ -18340,7 +18340,7 @@
         <v>848</v>
       </c>
       <c r="B850">
-        <v>10320600788</v>
+        <v>14005496342</v>
       </c>
       <c r="C850" t="s">
         <v>851</v>
@@ -18354,7 +18354,7 @@
         <v>849</v>
       </c>
       <c r="B851">
-        <v>14005496342</v>
+        <v>10000000099</v>
       </c>
       <c r="C851" t="s">
         <v>852</v>
@@ -18368,7 +18368,7 @@
         <v>850</v>
       </c>
       <c r="B852">
-        <v>10000000099</v>
+        <v>14004128084</v>
       </c>
       <c r="C852" t="s">
         <v>853</v>
@@ -18382,7 +18382,7 @@
         <v>851</v>
       </c>
       <c r="B853">
-        <v>14004128084</v>
+        <v>10103679112</v>
       </c>
       <c r="C853" t="s">
         <v>854</v>
@@ -18396,7 +18396,7 @@
         <v>852</v>
       </c>
       <c r="B854">
-        <v>10103679112</v>
+        <v>10100589211</v>
       </c>
       <c r="C854" t="s">
         <v>855</v>
@@ -18410,7 +18410,7 @@
         <v>853</v>
       </c>
       <c r="B855">
-        <v>10100589211</v>
+        <v>10320752394</v>
       </c>
       <c r="C855" t="s">
         <v>856</v>
@@ -18424,7 +18424,7 @@
         <v>854</v>
       </c>
       <c r="B856">
-        <v>10320752394</v>
+        <v>14004183170</v>
       </c>
       <c r="C856" t="s">
         <v>857</v>
@@ -18438,7 +18438,7 @@
         <v>855</v>
       </c>
       <c r="B857">
-        <v>14004183170</v>
+        <v>10100258391</v>
       </c>
       <c r="C857" t="s">
         <v>858</v>
@@ -18452,7 +18452,7 @@
         <v>856</v>
       </c>
       <c r="B858">
-        <v>10100258391</v>
+        <v>10100906047</v>
       </c>
       <c r="C858" t="s">
         <v>859</v>
@@ -18466,7 +18466,7 @@
         <v>857</v>
       </c>
       <c r="B859">
-        <v>10100906047</v>
+        <v>10100976112</v>
       </c>
       <c r="C859" t="s">
         <v>860</v>
@@ -18480,7 +18480,7 @@
         <v>858</v>
       </c>
       <c r="B860">
-        <v>10100976112</v>
+        <v>10103372005</v>
       </c>
       <c r="C860" t="s">
         <v>861</v>
@@ -18494,7 +18494,7 @@
         <v>859</v>
       </c>
       <c r="B861">
-        <v>10103372005</v>
+        <v>14007120347</v>
       </c>
       <c r="C861" t="s">
         <v>862</v>
@@ -18508,7 +18508,7 @@
         <v>860</v>
       </c>
       <c r="B862">
-        <v>14007120347</v>
+        <v>14009518268</v>
       </c>
       <c r="C862" t="s">
         <v>863</v>
@@ -18522,7 +18522,7 @@
         <v>861</v>
       </c>
       <c r="B863">
-        <v>14009518268</v>
+        <v>10630025764</v>
       </c>
       <c r="C863" t="s">
         <v>864</v>
@@ -18536,7 +18536,7 @@
         <v>862</v>
       </c>
       <c r="B864">
-        <v>10630025764</v>
+        <v>10101915348</v>
       </c>
       <c r="C864" t="s">
         <v>865</v>
@@ -18550,7 +18550,7 @@
         <v>863</v>
       </c>
       <c r="B865">
-        <v>10101915348</v>
+        <v>10320469990</v>
       </c>
       <c r="C865" t="s">
         <v>866</v>
@@ -18564,7 +18564,7 @@
         <v>864</v>
       </c>
       <c r="B866">
-        <v>10320469990</v>
+        <v>14007123145</v>
       </c>
       <c r="C866" t="s">
         <v>867</v>
@@ -18578,7 +18578,7 @@
         <v>865</v>
       </c>
       <c r="B867">
-        <v>14007123145</v>
+        <v>10103258569</v>
       </c>
       <c r="C867" t="s">
         <v>868</v>
@@ -18592,7 +18592,7 @@
         <v>866</v>
       </c>
       <c r="B868">
-        <v>10103258569</v>
+        <v>10380450359</v>
       </c>
       <c r="C868" t="s">
         <v>869</v>
@@ -18606,7 +18606,7 @@
         <v>867</v>
       </c>
       <c r="B869">
-        <v>10380450359</v>
+        <v>14006336023</v>
       </c>
       <c r="C869" t="s">
         <v>870</v>
@@ -18620,7 +18620,7 @@
         <v>868</v>
       </c>
       <c r="B870">
-        <v>14006336023</v>
+        <v>10320400445</v>
       </c>
       <c r="C870" t="s">
         <v>871</v>
@@ -18634,7 +18634,7 @@
         <v>869</v>
       </c>
       <c r="B871">
-        <v>10320400445</v>
+        <v>14008157950</v>
       </c>
       <c r="C871" t="s">
         <v>872</v>
@@ -18648,7 +18648,7 @@
         <v>870</v>
       </c>
       <c r="B872">
-        <v>14008157950</v>
+        <v>10861529184</v>
       </c>
       <c r="C872" t="s">
         <v>873</v>
@@ -18662,7 +18662,7 @@
         <v>871</v>
       </c>
       <c r="B873">
-        <v>10861529184</v>
+        <v>10000000029</v>
       </c>
       <c r="C873" t="s">
         <v>874</v>
@@ -18676,7 +18676,7 @@
         <v>872</v>
       </c>
       <c r="B874">
-        <v>10000000029</v>
+        <v>10102803281</v>
       </c>
       <c r="C874" t="s">
         <v>875</v>
@@ -18690,7 +18690,7 @@
         <v>873</v>
       </c>
       <c r="B875">
-        <v>10102803281</v>
+        <v>10320650723</v>
       </c>
       <c r="C875" t="s">
         <v>876</v>
@@ -18704,7 +18704,7 @@
         <v>874</v>
       </c>
       <c r="B876">
-        <v>10320650723</v>
+        <v>10380305808</v>
       </c>
       <c r="C876" t="s">
         <v>877</v>
@@ -18718,7 +18718,7 @@
         <v>875</v>
       </c>
       <c r="B877">
-        <v>10380305808</v>
+        <v>14009263200</v>
       </c>
       <c r="C877" t="s">
         <v>878</v>
@@ -18732,7 +18732,7 @@
         <v>876</v>
       </c>
       <c r="B878">
-        <v>14009263200</v>
+        <v>10000000060</v>
       </c>
       <c r="C878" t="s">
         <v>879</v>
@@ -18746,7 +18746,7 @@
         <v>877</v>
       </c>
       <c r="B879">
-        <v>10000000060</v>
+        <v>10320813657</v>
       </c>
       <c r="C879" t="s">
         <v>880</v>
@@ -18760,7 +18760,7 @@
         <v>878</v>
       </c>
       <c r="B880">
-        <v>10320813657</v>
+        <v>10102694700</v>
       </c>
       <c r="C880" t="s">
         <v>881</v>
@@ -18774,7 +18774,7 @@
         <v>879</v>
       </c>
       <c r="B881">
-        <v>10102694700</v>
+        <v>14005108893</v>
       </c>
       <c r="C881" t="s">
         <v>882</v>
@@ -18788,7 +18788,7 @@
         <v>880</v>
       </c>
       <c r="B882">
-        <v>14005108893</v>
+        <v>10000000036</v>
       </c>
       <c r="C882" t="s">
         <v>883</v>
@@ -18802,7 +18802,7 @@
         <v>881</v>
       </c>
       <c r="B883">
-        <v>10000000036</v>
+        <v>14000074621</v>
       </c>
       <c r="C883" t="s">
         <v>884</v>
@@ -18816,7 +18816,7 @@
         <v>882</v>
       </c>
       <c r="B884">
-        <v>14000074621</v>
+        <v>10861530138</v>
       </c>
       <c r="C884" t="s">
         <v>885</v>
@@ -18830,7 +18830,7 @@
         <v>883</v>
       </c>
       <c r="B885">
-        <v>10861530138</v>
+        <v>10103037570</v>
       </c>
       <c r="C885" t="s">
         <v>886</v>
@@ -18844,7 +18844,7 @@
         <v>884</v>
       </c>
       <c r="B886">
-        <v>10103037570</v>
+        <v>10101997560</v>
       </c>
       <c r="C886" t="s">
         <v>887</v>
@@ -18858,7 +18858,7 @@
         <v>885</v>
       </c>
       <c r="B887">
-        <v>10101997560</v>
+        <v>14004107956</v>
       </c>
       <c r="C887" t="s">
         <v>888</v>
@@ -18872,7 +18872,7 @@
         <v>886</v>
       </c>
       <c r="B888">
-        <v>14004107956</v>
+        <v>10380520955</v>
       </c>
       <c r="C888" t="s">
         <v>889</v>
@@ -18886,7 +18886,7 @@
         <v>887</v>
       </c>
       <c r="B889">
-        <v>10380520955</v>
+        <v>14006243544</v>
       </c>
       <c r="C889" t="s">
         <v>890</v>
@@ -18900,7 +18900,7 @@
         <v>888</v>
       </c>
       <c r="B890">
-        <v>14006243544</v>
+        <v>10103761233</v>
       </c>
       <c r="C890" t="s">
         <v>891</v>
@@ -18914,7 +18914,7 @@
         <v>889</v>
       </c>
       <c r="B891">
-        <v>10103761233</v>
+        <v>14004407347</v>
       </c>
       <c r="C891" t="s">
         <v>892</v>
@@ -18928,7 +18928,7 @@
         <v>890</v>
       </c>
       <c r="B892">
-        <v>14004407347</v>
+        <v>10380647203</v>
       </c>
       <c r="C892" t="s">
         <v>893</v>
@@ -18942,7 +18942,7 @@
         <v>891</v>
       </c>
       <c r="B893">
-        <v>10380647203</v>
+        <v>14007411551</v>
       </c>
       <c r="C893" t="s">
         <v>894</v>
@@ -18956,7 +18956,7 @@
         <v>892</v>
       </c>
       <c r="B894">
-        <v>14007411551</v>
+        <v>10320352137</v>
       </c>
       <c r="C894" t="s">
         <v>895</v>
@@ -18970,7 +18970,7 @@
         <v>893</v>
       </c>
       <c r="B895">
-        <v>10320352137</v>
+        <v>10320774211</v>
       </c>
       <c r="C895" t="s">
         <v>896</v>
@@ -18984,7 +18984,7 @@
         <v>894</v>
       </c>
       <c r="B896">
-        <v>10320774211</v>
+        <v>10380647222</v>
       </c>
       <c r="C896" t="s">
         <v>897</v>
@@ -18998,7 +18998,7 @@
         <v>895</v>
       </c>
       <c r="B897">
-        <v>10380647222</v>
+        <v>10862064732</v>
       </c>
       <c r="C897" t="s">
         <v>898</v>
@@ -19012,7 +19012,7 @@
         <v>896</v>
       </c>
       <c r="B898">
-        <v>10862064732</v>
+        <v>10101364297</v>
       </c>
       <c r="C898" t="s">
         <v>899</v>
@@ -19026,7 +19026,7 @@
         <v>897</v>
       </c>
       <c r="B899">
-        <v>10101364297</v>
+        <v>10103837742</v>
       </c>
       <c r="C899" t="s">
         <v>900</v>
@@ -19040,7 +19040,7 @@
         <v>898</v>
       </c>
       <c r="B900">
-        <v>10103837742</v>
+        <v>10000000043</v>
       </c>
       <c r="C900" t="s">
         <v>901</v>
@@ -19054,7 +19054,7 @@
         <v>899</v>
       </c>
       <c r="B901">
-        <v>10000000043</v>
+        <v>10102898876</v>
       </c>
       <c r="C901" t="s">
         <v>902</v>
@@ -19068,7 +19068,7 @@
         <v>900</v>
       </c>
       <c r="B902">
-        <v>10102898876</v>
+        <v>10000000024</v>
       </c>
       <c r="C902" t="s">
         <v>903</v>
@@ -19082,7 +19082,7 @@
         <v>901</v>
       </c>
       <c r="B903">
-        <v>10000000024</v>
+        <v>14008247684</v>
       </c>
       <c r="C903" t="s">
         <v>904</v>
@@ -19096,7 +19096,7 @@
         <v>902</v>
       </c>
       <c r="B904">
-        <v>14008247684</v>
+        <v>14007707492</v>
       </c>
       <c r="C904" t="s">
         <v>905</v>
@@ -19110,7 +19110,7 @@
         <v>903</v>
       </c>
       <c r="B905">
-        <v>14007707492</v>
+        <v>10320692265</v>
       </c>
       <c r="C905" t="s">
         <v>906</v>
@@ -19124,7 +19124,7 @@
         <v>904</v>
       </c>
       <c r="B906">
-        <v>10320692265</v>
+        <v>10320673140</v>
       </c>
       <c r="C906" t="s">
         <v>907</v>
@@ -19138,7 +19138,7 @@
         <v>905</v>
       </c>
       <c r="B907">
-        <v>10320673140</v>
+        <v>10320692094</v>
       </c>
       <c r="C907" t="s">
         <v>908</v>
@@ -19152,7 +19152,7 @@
         <v>906</v>
       </c>
       <c r="B908">
-        <v>10320692094</v>
+        <v>14004068870</v>
       </c>
       <c r="C908" t="s">
         <v>909</v>
@@ -19166,7 +19166,7 @@
         <v>907</v>
       </c>
       <c r="B909">
-        <v>14004068870</v>
+        <v>14008556974</v>
       </c>
       <c r="C909" t="s">
         <v>910</v>
@@ -19180,7 +19180,7 @@
         <v>908</v>
       </c>
       <c r="B910">
-        <v>14008556974</v>
+        <v>10103460290</v>
       </c>
       <c r="C910" t="s">
         <v>911</v>
@@ -19194,7 +19194,7 @@
         <v>909</v>
       </c>
       <c r="B911">
-        <v>10103460290</v>
+        <v>10101442691</v>
       </c>
       <c r="C911" t="s">
         <v>912</v>
@@ -19208,7 +19208,7 @@
         <v>910</v>
       </c>
       <c r="B912">
-        <v>10101442691</v>
+        <v>10320307426</v>
       </c>
       <c r="C912" t="s">
         <v>913</v>
@@ -19222,7 +19222,7 @@
         <v>911</v>
       </c>
       <c r="B913">
-        <v>10320307426</v>
+        <v>14005253222</v>
       </c>
       <c r="C913" t="s">
         <v>914</v>
@@ -19236,7 +19236,7 @@
         <v>912</v>
       </c>
       <c r="B914">
-        <v>14005253222</v>
+        <v>10200450670</v>
       </c>
       <c r="C914" t="s">
         <v>915</v>
@@ -19250,7 +19250,7 @@
         <v>913</v>
       </c>
       <c r="B915">
-        <v>10200450670</v>
+        <v>14008076836</v>
       </c>
       <c r="C915" t="s">
         <v>916</v>
@@ -19264,7 +19264,7 @@
         <v>914</v>
       </c>
       <c r="B916">
-        <v>14008076836</v>
+        <v>10100937493</v>
       </c>
       <c r="C916" t="s">
         <v>917</v>
@@ -19278,7 +19278,7 @@
         <v>915</v>
       </c>
       <c r="B917">
-        <v>10100937493</v>
+        <v>10100505148</v>
       </c>
       <c r="C917" t="s">
         <v>918</v>
@@ -19292,7 +19292,7 @@
         <v>916</v>
       </c>
       <c r="B918">
-        <v>10100505148</v>
+        <v>10101814661</v>
       </c>
       <c r="C918" t="s">
         <v>919</v>
@@ -19306,7 +19306,7 @@
         <v>917</v>
       </c>
       <c r="B919">
-        <v>10101814661</v>
+        <v>10320884761</v>
       </c>
       <c r="C919" t="s">
         <v>920</v>
@@ -19320,7 +19320,7 @@
         <v>918</v>
       </c>
       <c r="B920">
-        <v>10320884761</v>
+        <v>10102173008</v>
       </c>
       <c r="C920" t="s">
         <v>921</v>
@@ -19334,7 +19334,7 @@
         <v>919</v>
       </c>
       <c r="B921">
-        <v>10102173008</v>
+        <v>10102593722</v>
       </c>
       <c r="C921" t="s">
         <v>922</v>
@@ -19348,7 +19348,7 @@
         <v>920</v>
       </c>
       <c r="B922">
-        <v>10102593722</v>
+        <v>10104060856</v>
       </c>
       <c r="C922" t="s">
         <v>923</v>
@@ -19362,7 +19362,7 @@
         <v>921</v>
       </c>
       <c r="B923">
-        <v>10104060856</v>
+        <v>10000000034</v>
       </c>
       <c r="C923" t="s">
         <v>924</v>
@@ -19376,7 +19376,7 @@
         <v>922</v>
       </c>
       <c r="B924">
-        <v>10000000034</v>
+        <v>10000000033</v>
       </c>
       <c r="C924" t="s">
         <v>925</v>
@@ -19390,7 +19390,7 @@
         <v>923</v>
       </c>
       <c r="B925">
-        <v>10000000033</v>
+        <v>10320895923</v>
       </c>
       <c r="C925" t="s">
         <v>926</v>
@@ -19404,7 +19404,7 @@
         <v>924</v>
       </c>
       <c r="B926">
-        <v>10320895923</v>
+        <v>14005828941</v>
       </c>
       <c r="C926" t="s">
         <v>927</v>
@@ -19418,7 +19418,7 @@
         <v>925</v>
       </c>
       <c r="B927">
-        <v>14005828941</v>
+        <v>14006793310</v>
       </c>
       <c r="C927" t="s">
         <v>928</v>
@@ -19432,7 +19432,7 @@
         <v>926</v>
       </c>
       <c r="B928">
-        <v>14006793310</v>
+        <v>14005786478</v>
       </c>
       <c r="C928" t="s">
         <v>929</v>
@@ -19446,7 +19446,7 @@
         <v>927</v>
       </c>
       <c r="B929">
-        <v>14005786478</v>
+        <v>14005965618</v>
       </c>
       <c r="C929" t="s">
         <v>930</v>
@@ -19460,7 +19460,7 @@
         <v>928</v>
       </c>
       <c r="B930">
-        <v>14005965618</v>
+        <v>14005925472</v>
       </c>
       <c r="C930" t="s">
         <v>931</v>
@@ -19474,7 +19474,7 @@
         <v>929</v>
       </c>
       <c r="B931">
-        <v>14005925472</v>
+        <v>14007027064</v>
       </c>
       <c r="C931" t="s">
         <v>932</v>
@@ -19488,7 +19488,7 @@
         <v>930</v>
       </c>
       <c r="B932">
-        <v>14007027064</v>
+        <v>14007137903</v>
       </c>
       <c r="C932" t="s">
         <v>933</v>
@@ -19502,7 +19502,7 @@
         <v>931</v>
       </c>
       <c r="B933">
-        <v>14007137903</v>
+        <v>14006082952</v>
       </c>
       <c r="C933" t="s">
         <v>934</v>
@@ -19516,7 +19516,7 @@
         <v>932</v>
       </c>
       <c r="B934">
-        <v>14006082952</v>
+        <v>10320780362</v>
       </c>
       <c r="C934" t="s">
         <v>935</v>
@@ -19530,7 +19530,7 @@
         <v>933</v>
       </c>
       <c r="B935">
-        <v>10320780362</v>
+        <v>10320858723</v>
       </c>
       <c r="C935" t="s">
         <v>936</v>
@@ -19544,7 +19544,7 @@
         <v>934</v>
       </c>
       <c r="B936">
-        <v>10320858723</v>
+        <v>10320661767</v>
       </c>
       <c r="C936" t="s">
         <v>937</v>
@@ -19558,7 +19558,7 @@
         <v>935</v>
       </c>
       <c r="B937">
-        <v>10320661767</v>
+        <v>10320169213</v>
       </c>
       <c r="C937" t="s">
         <v>938</v>
@@ -19572,7 +19572,7 @@
         <v>936</v>
       </c>
       <c r="B938">
-        <v>10320169213</v>
+        <v>10000000055</v>
       </c>
       <c r="C938" t="s">
         <v>939</v>
@@ -19586,7 +19586,7 @@
         <v>937</v>
       </c>
       <c r="B939">
-        <v>10000000055</v>
+        <v>14005933591</v>
       </c>
       <c r="C939" t="s">
         <v>940</v>
@@ -19600,7 +19600,7 @@
         <v>938</v>
       </c>
       <c r="B940">
-        <v>14005933591</v>
+        <v>10980226256</v>
       </c>
       <c r="C940" t="s">
         <v>941</v>
@@ -19614,7 +19614,7 @@
         <v>939</v>
       </c>
       <c r="B941">
-        <v>10980226256</v>
+        <v>10320503955</v>
       </c>
       <c r="C941" t="s">
         <v>942</v>
@@ -19628,7 +19628,7 @@
         <v>940</v>
       </c>
       <c r="B942">
-        <v>10320503955</v>
+        <v>10000000026</v>
       </c>
       <c r="C942" t="s">
         <v>943</v>
@@ -19642,7 +19642,7 @@
         <v>941</v>
       </c>
       <c r="B943">
-        <v>10000000026</v>
+        <v>10420196707</v>
       </c>
       <c r="C943" t="s">
         <v>944</v>
@@ -19656,7 +19656,7 @@
         <v>942</v>
       </c>
       <c r="B944">
-        <v>10420196707</v>
+        <v>10860411138</v>
       </c>
       <c r="C944" t="s">
         <v>945</v>
@@ -19670,7 +19670,7 @@
         <v>943</v>
       </c>
       <c r="B945">
-        <v>10860411138</v>
+        <v>10101759580</v>
       </c>
       <c r="C945" t="s">
         <v>946</v>
@@ -19684,7 +19684,7 @@
         <v>944</v>
       </c>
       <c r="B946">
-        <v>10101759580</v>
+        <v>10320832748</v>
       </c>
       <c r="C946" t="s">
         <v>947</v>
@@ -19698,7 +19698,7 @@
         <v>945</v>
       </c>
       <c r="B947">
-        <v>10320832748</v>
+        <v>10760094603</v>
       </c>
       <c r="C947" t="s">
         <v>948</v>
@@ -19712,7 +19712,7 @@
         <v>946</v>
       </c>
       <c r="B948">
-        <v>10760094603</v>
+        <v>10100171920</v>
       </c>
       <c r="C948" t="s">
         <v>949</v>
@@ -19726,7 +19726,7 @@
         <v>947</v>
       </c>
       <c r="B949">
-        <v>10100171920</v>
+        <v>10000000040</v>
       </c>
       <c r="C949" t="s">
         <v>950</v>
@@ -19740,7 +19740,7 @@
         <v>948</v>
       </c>
       <c r="B950">
-        <v>10000000040</v>
+        <v>10100625070</v>
       </c>
       <c r="C950" t="s">
         <v>951</v>
@@ -19754,7 +19754,7 @@
         <v>949</v>
       </c>
       <c r="B951">
-        <v>10100625070</v>
+        <v>14003674869</v>
       </c>
       <c r="C951" t="s">
         <v>952</v>
@@ -19768,7 +19768,7 @@
         <v>950</v>
       </c>
       <c r="B952">
-        <v>14003674869</v>
+        <v>14009108895</v>
       </c>
       <c r="C952" t="s">
         <v>953</v>
@@ -19782,7 +19782,7 @@
         <v>951</v>
       </c>
       <c r="B953">
-        <v>14009108895</v>
+        <v>10000000030</v>
       </c>
       <c r="C953" t="s">
         <v>954</v>
@@ -19796,7 +19796,7 @@
         <v>952</v>
       </c>
       <c r="B954">
-        <v>10000000030</v>
+        <v>14008036097</v>
       </c>
       <c r="C954" t="s">
         <v>955</v>
@@ -19810,7 +19810,7 @@
         <v>953</v>
       </c>
       <c r="B955">
-        <v>14008036097</v>
+        <v>10100053930</v>
       </c>
       <c r="C955" t="s">
         <v>956</v>
@@ -19824,7 +19824,7 @@
         <v>954</v>
       </c>
       <c r="B956">
-        <v>10100053930</v>
+        <v>14004684611</v>
       </c>
       <c r="C956" t="s">
         <v>957</v>
@@ -19838,7 +19838,7 @@
         <v>955</v>
       </c>
       <c r="B957">
-        <v>14004684611</v>
+        <v>10100351811</v>
       </c>
       <c r="C957" t="s">
         <v>958</v>
@@ -19852,7 +19852,7 @@
         <v>956</v>
       </c>
       <c r="B958">
-        <v>10100351811</v>
+        <v>10320539175</v>
       </c>
       <c r="C958" t="s">
         <v>959</v>
@@ -19866,7 +19866,7 @@
         <v>957</v>
       </c>
       <c r="B959">
-        <v>10320539175</v>
+        <v>10100567400</v>
       </c>
       <c r="C959" t="s">
         <v>960</v>
@@ -19880,7 +19880,7 @@
         <v>958</v>
       </c>
       <c r="B960">
-        <v>10100567400</v>
+        <v>14009263160</v>
       </c>
       <c r="C960" t="s">
         <v>961</v>
@@ -19894,7 +19894,7 @@
         <v>959</v>
       </c>
       <c r="B961">
-        <v>14009263160</v>
+        <v>10861677542</v>
       </c>
       <c r="C961" t="s">
         <v>962</v>
@@ -19908,7 +19908,7 @@
         <v>960</v>
       </c>
       <c r="B962">
-        <v>10861677542</v>
+        <v>10000000073</v>
       </c>
       <c r="C962" t="s">
         <v>963</v>
@@ -19922,7 +19922,7 @@
         <v>961</v>
       </c>
       <c r="B963">
-        <v>10000000073</v>
+        <v>10103858742</v>
       </c>
       <c r="C963" t="s">
         <v>964</v>
@@ -19936,7 +19936,7 @@
         <v>962</v>
       </c>
       <c r="B964">
-        <v>10103858742</v>
+        <v>10102279261</v>
       </c>
       <c r="C964" t="s">
         <v>965</v>
@@ -19950,7 +19950,7 @@
         <v>963</v>
       </c>
       <c r="B965">
-        <v>10102279261</v>
+        <v>10102803034</v>
       </c>
       <c r="C965" t="s">
         <v>966</v>
@@ -19964,7 +19964,7 @@
         <v>964</v>
       </c>
       <c r="B966">
-        <v>10102803034</v>
+        <v>14003699653</v>
       </c>
       <c r="C966" t="s">
         <v>967</v>
@@ -19978,7 +19978,7 @@
         <v>965</v>
       </c>
       <c r="B967">
-        <v>14003699653</v>
+        <v>14004081532</v>
       </c>
       <c r="C967" t="s">
         <v>968</v>
@@ -19992,7 +19992,7 @@
         <v>966</v>
       </c>
       <c r="B968">
-        <v>14004081532</v>
+        <v>10103297319</v>
       </c>
       <c r="C968" t="s">
         <v>969</v>
@@ -20006,7 +20006,7 @@
         <v>967</v>
       </c>
       <c r="B969">
-        <v>10103297319</v>
+        <v>10380179815</v>
       </c>
       <c r="C969" t="s">
         <v>970</v>
@@ -20020,7 +20020,7 @@
         <v>968</v>
       </c>
       <c r="B970">
-        <v>10380179815</v>
+        <v>14003902009</v>
       </c>
       <c r="C970" t="s">
         <v>971</v>
@@ -20034,7 +20034,7 @@
         <v>969</v>
       </c>
       <c r="B971">
-        <v>14003902009</v>
+        <v>10200258715</v>
       </c>
       <c r="C971" t="s">
         <v>972</v>
@@ -20048,7 +20048,7 @@
         <v>970</v>
       </c>
       <c r="B972">
-        <v>10200258715</v>
+        <v>10760345687</v>
       </c>
       <c r="C972" t="s">
         <v>973</v>
@@ -20062,7 +20062,7 @@
         <v>971</v>
       </c>
       <c r="B973">
-        <v>10760345687</v>
+        <v>10630135824</v>
       </c>
       <c r="C973" t="s">
         <v>974</v>
@@ -20076,7 +20076,7 @@
         <v>972</v>
       </c>
       <c r="B974">
-        <v>10630135824</v>
+        <v>10220124165</v>
       </c>
       <c r="C974" t="s">
         <v>975</v>
@@ -20090,7 +20090,7 @@
         <v>973</v>
       </c>
       <c r="B975">
-        <v>10220124165</v>
+        <v>10860405350</v>
       </c>
       <c r="C975" t="s">
         <v>976</v>
@@ -20104,7 +20104,7 @@
         <v>974</v>
       </c>
       <c r="B976">
-        <v>10860405350</v>
+        <v>10720243977</v>
       </c>
       <c r="C976" t="s">
         <v>977</v>
@@ -20118,7 +20118,7 @@
         <v>975</v>
       </c>
       <c r="B977">
-        <v>10720243977</v>
+        <v>10700141201</v>
       </c>
       <c r="C977" t="s">
         <v>978</v>
@@ -20132,7 +20132,7 @@
         <v>976</v>
       </c>
       <c r="B978">
-        <v>10700141201</v>
+        <v>10320528091</v>
       </c>
       <c r="C978" t="s">
         <v>979</v>
@@ -20146,7 +20146,7 @@
         <v>977</v>
       </c>
       <c r="B979">
-        <v>10320528091</v>
+        <v>10320354635</v>
       </c>
       <c r="C979" t="s">
         <v>980</v>
@@ -20160,7 +20160,7 @@
         <v>978</v>
       </c>
       <c r="B980">
-        <v>10320354635</v>
+        <v>10101380313</v>
       </c>
       <c r="C980" t="s">
         <v>981</v>
@@ -20174,7 +20174,7 @@
         <v>979</v>
       </c>
       <c r="B981">
-        <v>10101380313</v>
+        <v>10103349751</v>
       </c>
       <c r="C981" t="s">
         <v>982</v>
@@ -20188,7 +20188,7 @@
         <v>980</v>
       </c>
       <c r="B982">
-        <v>10103349751</v>
+        <v>10104052682</v>
       </c>
       <c r="C982" t="s">
         <v>983</v>
@@ -20202,7 +20202,7 @@
         <v>981</v>
       </c>
       <c r="B983">
-        <v>10104052682</v>
+        <v>14004356528</v>
       </c>
       <c r="C983" t="s">
         <v>984</v>
@@ -20216,7 +20216,7 @@
         <v>982</v>
       </c>
       <c r="B984">
-        <v>14004356528</v>
+        <v>10260434191</v>
       </c>
       <c r="C984" t="s">
         <v>985</v>
@@ -20230,7 +20230,7 @@
         <v>983</v>
       </c>
       <c r="B985">
-        <v>10260434191</v>
+        <v>10260334425</v>
       </c>
       <c r="C985" t="s">
         <v>986</v>
@@ -20244,7 +20244,7 @@
         <v>984</v>
       </c>
       <c r="B986">
-        <v>10260334425</v>
+        <v>10102399005</v>
       </c>
       <c r="C986" t="s">
         <v>987</v>
@@ -20258,7 +20258,7 @@
         <v>985</v>
       </c>
       <c r="B987">
-        <v>10102399005</v>
+        <v>10103663870</v>
       </c>
       <c r="C987" t="s">
         <v>988</v>
@@ -20272,7 +20272,7 @@
         <v>986</v>
       </c>
       <c r="B988">
-        <v>10103663870</v>
+        <v>10103871690</v>
       </c>
       <c r="C988" t="s">
         <v>989</v>
@@ -20286,7 +20286,7 @@
         <v>987</v>
       </c>
       <c r="B989">
-        <v>10103871690</v>
+        <v>10320823442</v>
       </c>
       <c r="C989" t="s">
         <v>990</v>
@@ -20300,7 +20300,7 @@
         <v>988</v>
       </c>
       <c r="B990">
-        <v>10320823442</v>
+        <v>14006847020</v>
       </c>
       <c r="C990" t="s">
         <v>991</v>
@@ -20314,7 +20314,7 @@
         <v>989</v>
       </c>
       <c r="B991">
-        <v>14006847020</v>
+        <v>14003772673</v>
       </c>
       <c r="C991" t="s">
         <v>992</v>
@@ -20328,7 +20328,7 @@
         <v>990</v>
       </c>
       <c r="B992">
-        <v>14003772673</v>
+        <v>10104055685</v>
       </c>
       <c r="C992" t="s">
         <v>993</v>
@@ -20342,7 +20342,7 @@
         <v>991</v>
       </c>
       <c r="B993">
-        <v>10104055685</v>
+        <v>14006123572</v>
       </c>
       <c r="C993" t="s">
         <v>994</v>
@@ -20356,7 +20356,7 @@
         <v>992</v>
       </c>
       <c r="B994">
-        <v>14006123572</v>
+        <v>10000000038</v>
       </c>
       <c r="C994" t="s">
         <v>995</v>
@@ -20370,7 +20370,7 @@
         <v>993</v>
       </c>
       <c r="B995">
-        <v>10000000038</v>
+        <v>10102986880</v>
       </c>
       <c r="C995" t="s">
         <v>996</v>
@@ -20384,7 +20384,7 @@
         <v>994</v>
       </c>
       <c r="B996">
-        <v>10102986880</v>
+        <v>10000000028</v>
       </c>
       <c r="C996" t="s">
         <v>997</v>
@@ -20398,7 +20398,7 @@
         <v>995</v>
       </c>
       <c r="B997">
-        <v>10000000028</v>
+        <v>10000000050</v>
       </c>
       <c r="C997" t="s">
         <v>998</v>
@@ -20412,7 +20412,7 @@
         <v>996</v>
       </c>
       <c r="B998">
-        <v>10000000050</v>
+        <v>10100845276</v>
       </c>
       <c r="C998" t="s">
         <v>999</v>
@@ -20426,7 +20426,7 @@
         <v>997</v>
       </c>
       <c r="B999">
-        <v>10100845276</v>
+        <v>10101727833</v>
       </c>
       <c r="C999" t="s">
         <v>1000</v>
@@ -20440,7 +20440,7 @@
         <v>998</v>
       </c>
       <c r="B1000">
-        <v>10101727833</v>
+        <v>10840070153</v>
       </c>
       <c r="C1000" t="s">
         <v>1001</v>
@@ -20454,7 +20454,7 @@
         <v>999</v>
       </c>
       <c r="B1001">
-        <v>10840070153</v>
+        <v>10840086913</v>
       </c>
       <c r="C1001" t="s">
         <v>1002</v>
@@ -20468,7 +20468,7 @@
         <v>1000</v>
       </c>
       <c r="B1002">
-        <v>10840086913</v>
+        <v>10000000046</v>
       </c>
       <c r="C1002" t="s">
         <v>1003</v>
@@ -20482,7 +20482,7 @@
         <v>1001</v>
       </c>
       <c r="B1003">
-        <v>10000000046</v>
+        <v>10102685249</v>
       </c>
       <c r="C1003" t="s">
         <v>1004</v>
@@ -20496,7 +20496,7 @@
         <v>1002</v>
       </c>
       <c r="B1004">
-        <v>10102685249</v>
+        <v>14003725635</v>
       </c>
       <c r="C1004" t="s">
         <v>1005</v>
@@ -20510,7 +20510,7 @@
         <v>1003</v>
       </c>
       <c r="B1005">
-        <v>14003725635</v>
+        <v>14003767221</v>
       </c>
       <c r="C1005" t="s">
         <v>1006</v>
@@ -20524,7 +20524,7 @@
         <v>1004</v>
       </c>
       <c r="B1006">
-        <v>14003767221</v>
+        <v>10102727560</v>
       </c>
       <c r="C1006" t="s">
         <v>1007</v>
@@ -20538,7 +20538,7 @@
         <v>1005</v>
       </c>
       <c r="B1007">
-        <v>10102727560</v>
+        <v>10102803015</v>
       </c>
       <c r="C1007" t="s">
         <v>1008</v>
@@ -20552,7 +20552,7 @@
         <v>1006</v>
       </c>
       <c r="B1008">
-        <v>10102803015</v>
+        <v>10102802996</v>
       </c>
       <c r="C1008" t="s">
         <v>1009</v>
@@ -20566,7 +20566,7 @@
         <v>1007</v>
       </c>
       <c r="B1009">
-        <v>10102802996</v>
+        <v>10102803205</v>
       </c>
       <c r="C1009" t="s">
         <v>1010</v>
@@ -20580,7 +20580,7 @@
         <v>1008</v>
       </c>
       <c r="B1010">
-        <v>10102803205</v>
+        <v>10101997272</v>
       </c>
       <c r="C1010" t="s">
         <v>1011</v>
@@ -20594,7 +20594,7 @@
         <v>1009</v>
       </c>
       <c r="B1011">
-        <v>10101997272</v>
+        <v>10000000041</v>
       </c>
       <c r="C1011" t="s">
         <v>1012</v>
@@ -20608,7 +20608,7 @@
         <v>1010</v>
       </c>
       <c r="B1012">
-        <v>10000000041</v>
+        <v>10000000075</v>
       </c>
       <c r="C1012" t="s">
         <v>1013</v>
@@ -20622,7 +20622,7 @@
         <v>1011</v>
       </c>
       <c r="B1013">
-        <v>10000000075</v>
+        <v>10000000092</v>
       </c>
       <c r="C1013" t="s">
         <v>1014</v>
@@ -20636,7 +20636,7 @@
         <v>1012</v>
       </c>
       <c r="B1014">
-        <v>10000000092</v>
+        <v>10102960400</v>
       </c>
       <c r="C1014" t="s">
         <v>1015</v>
@@ -20650,7 +20650,7 @@
         <v>1013</v>
       </c>
       <c r="B1015">
-        <v>10102960400</v>
+        <v>10103705170</v>
       </c>
       <c r="C1015" t="s">
         <v>1016</v>
@@ -20664,7 +20664,7 @@
         <v>1014</v>
       </c>
       <c r="B1016">
-        <v>10103705170</v>
+        <v>10320839039</v>
       </c>
       <c r="C1016" t="s">
         <v>1017</v>
@@ -20678,7 +20678,7 @@
         <v>1015</v>
       </c>
       <c r="B1017">
-        <v>10320839039</v>
+        <v>10320836357</v>
       </c>
       <c r="C1017" t="s">
         <v>1018</v>
@@ -20692,7 +20692,7 @@
         <v>1016</v>
       </c>
       <c r="B1018">
-        <v>10320836357</v>
+        <v>10320876676</v>
       </c>
       <c r="C1018" t="s">
         <v>1019</v>
@@ -20706,7 +20706,7 @@
         <v>1017</v>
       </c>
       <c r="B1019">
-        <v>10320876676</v>
+        <v>10320635617</v>
       </c>
       <c r="C1019" t="s">
         <v>1020</v>
@@ -20720,7 +20720,7 @@
         <v>1018</v>
       </c>
       <c r="B1020">
-        <v>10320635617</v>
+        <v>10320635904</v>
       </c>
       <c r="C1020" t="s">
         <v>1021</v>
@@ -20734,7 +20734,7 @@
         <v>1019</v>
       </c>
       <c r="B1021">
-        <v>10320635904</v>
+        <v>14004210872</v>
       </c>
       <c r="C1021" t="s">
         <v>1022</v>
@@ -20748,7 +20748,7 @@
         <v>1020</v>
       </c>
       <c r="B1022">
-        <v>14004210872</v>
+        <v>14004156637</v>
       </c>
       <c r="C1022" t="s">
         <v>1023</v>
@@ -20762,7 +20762,7 @@
         <v>1021</v>
       </c>
       <c r="B1023">
-        <v>14004156637</v>
+        <v>14008079936</v>
       </c>
       <c r="C1023" t="s">
         <v>1024</v>
@@ -20776,7 +20776,7 @@
         <v>1022</v>
       </c>
       <c r="B1024">
-        <v>14008079936</v>
+        <v>10320634937</v>
       </c>
       <c r="C1024" t="s">
         <v>1025</v>
@@ -20790,7 +20790,7 @@
         <v>1023</v>
       </c>
       <c r="B1025">
-        <v>10320634937</v>
+        <v>10100385648</v>
       </c>
       <c r="C1025" t="s">
         <v>1026</v>
@@ -20804,7 +20804,7 @@
         <v>1024</v>
       </c>
       <c r="B1026">
-        <v>10100385648</v>
+        <v>10320635047</v>
       </c>
       <c r="C1026" t="s">
         <v>1027</v>
@@ -20818,7 +20818,7 @@
         <v>1025</v>
       </c>
       <c r="B1027">
-        <v>10320635047</v>
+        <v>10630107136</v>
       </c>
       <c r="C1027" t="s">
         <v>1028</v>
@@ -20832,7 +20832,7 @@
         <v>1026</v>
       </c>
       <c r="B1028">
-        <v>10630107136</v>
+        <v>10380474989</v>
       </c>
       <c r="C1028" t="s">
         <v>1029</v>
@@ -20846,7 +20846,7 @@
         <v>1027</v>
       </c>
       <c r="B1029">
-        <v>10380474989</v>
+        <v>14004975980</v>
       </c>
       <c r="C1029" t="s">
         <v>1030</v>
@@ -20860,7 +20860,7 @@
         <v>1028</v>
       </c>
       <c r="B1030">
-        <v>14004975980</v>
+        <v>10102417191</v>
       </c>
       <c r="C1030" t="s">
         <v>1031</v>
@@ -20874,7 +20874,7 @@
         <v>1029</v>
       </c>
       <c r="B1031">
-        <v>10102417191</v>
+        <v>14009224859</v>
       </c>
       <c r="C1031" t="s">
         <v>1032</v>
@@ -20888,7 +20888,7 @@
         <v>1030</v>
       </c>
       <c r="B1032">
-        <v>14009224859</v>
+        <v>10101730772</v>
       </c>
       <c r="C1032" t="s">
         <v>1033</v>
@@ -20902,7 +20902,7 @@
         <v>1031</v>
       </c>
       <c r="B1033">
-        <v>10101730772</v>
+        <v>10102558446</v>
       </c>
       <c r="C1033" t="s">
         <v>1034</v>
@@ -20916,7 +20916,7 @@
         <v>1032</v>
       </c>
       <c r="B1034">
-        <v>10102558446</v>
+        <v>10101476080</v>
       </c>
       <c r="C1034" t="s">
         <v>1035</v>
@@ -20930,7 +20930,7 @@
         <v>1033</v>
       </c>
       <c r="B1035">
-        <v>10101476080</v>
+        <v>10760335630</v>
       </c>
       <c r="C1035" t="s">
         <v>1036</v>
@@ -20944,7 +20944,7 @@
         <v>1034</v>
       </c>
       <c r="B1036">
-        <v>10760335630</v>
+        <v>10102702966</v>
       </c>
       <c r="C1036" t="s">
         <v>1037</v>
@@ -20958,7 +20958,7 @@
         <v>1035</v>
       </c>
       <c r="B1037">
-        <v>10102702966</v>
+        <v>10102634872</v>
       </c>
       <c r="C1037" t="s">
         <v>1038</v>
@@ -20972,7 +20972,7 @@
         <v>1036</v>
       </c>
       <c r="B1038">
-        <v>10102634872</v>
+        <v>10102002047</v>
       </c>
       <c r="C1038" t="s">
         <v>1039</v>
@@ -20986,7 +20986,7 @@
         <v>1037</v>
       </c>
       <c r="B1039">
-        <v>10102002047</v>
+        <v>10860222183</v>
       </c>
       <c r="C1039" t="s">
         <v>1040</v>
@@ -21000,7 +21000,7 @@
         <v>1038</v>
       </c>
       <c r="B1040">
-        <v>10860222183</v>
+        <v>10102775538</v>
       </c>
       <c r="C1040" t="s">
         <v>1041</v>
@@ -21014,7 +21014,7 @@
         <v>1039</v>
       </c>
       <c r="B1041">
-        <v>10102775538</v>
+        <v>14007297814</v>
       </c>
       <c r="C1041" t="s">
         <v>1042</v>
@@ -21028,7 +21028,7 @@
         <v>1040</v>
       </c>
       <c r="B1042">
-        <v>14007297814</v>
+        <v>10101559627</v>
       </c>
       <c r="C1042" t="s">
         <v>1043</v>
@@ -21042,7 +21042,7 @@
         <v>1041</v>
       </c>
       <c r="B1043">
-        <v>10101559627</v>
+        <v>10102040894</v>
       </c>
       <c r="C1043" t="s">
         <v>1044</v>
@@ -21056,7 +21056,7 @@
         <v>1042</v>
       </c>
       <c r="B1044">
-        <v>10102040894</v>
+        <v>10102676190</v>
       </c>
       <c r="C1044" t="s">
         <v>1045</v>
@@ -21070,7 +21070,7 @@
         <v>1043</v>
       </c>
       <c r="B1045">
-        <v>10102676190</v>
+        <v>10102631183</v>
       </c>
       <c r="C1045" t="s">
         <v>1046</v>
@@ -21084,7 +21084,7 @@
         <v>1044</v>
       </c>
       <c r="B1046">
-        <v>10102631183</v>
+        <v>10101553125</v>
       </c>
       <c r="C1046" t="s">
         <v>1047</v>
@@ -21098,7 +21098,7 @@
         <v>1045</v>
       </c>
       <c r="B1047">
-        <v>10101553125</v>
+        <v>10104011299</v>
       </c>
       <c r="C1047" t="s">
         <v>1048</v>
@@ -21112,7 +21112,7 @@
         <v>1046</v>
       </c>
       <c r="B1048">
-        <v>10104011299</v>
+        <v>10103653560</v>
       </c>
       <c r="C1048" t="s">
         <v>1049</v>
@@ -21126,7 +21126,7 @@
         <v>1047</v>
       </c>
       <c r="B1049">
-        <v>10103653560</v>
+        <v>10000000093</v>
       </c>
       <c r="C1049" t="s">
         <v>1050</v>
@@ -21140,7 +21140,7 @@
         <v>1048</v>
       </c>
       <c r="B1050">
-        <v>10000000093</v>
+        <v>10000000094</v>
       </c>
       <c r="C1050" t="s">
         <v>1051</v>
@@ -21154,7 +21154,7 @@
         <v>1049</v>
       </c>
       <c r="B1051">
-        <v>10000000094</v>
+        <v>10000000095</v>
       </c>
       <c r="C1051" t="s">
         <v>1052</v>
@@ -21168,7 +21168,7 @@
         <v>1050</v>
       </c>
       <c r="B1052">
-        <v>10000000095</v>
+        <v>10101954690</v>
       </c>
       <c r="C1052" t="s">
         <v>1053</v>
@@ -21182,7 +21182,7 @@
         <v>1051</v>
       </c>
       <c r="B1053">
-        <v>10101954690</v>
+        <v>10320330972</v>
       </c>
       <c r="C1053" t="s">
         <v>1054</v>
@@ -21196,7 +21196,7 @@
         <v>1052</v>
       </c>
       <c r="B1054">
-        <v>10320330972</v>
+        <v>10320683865</v>
       </c>
       <c r="C1054" t="s">
         <v>1055</v>
@@ -21210,7 +21210,7 @@
         <v>1053</v>
       </c>
       <c r="B1055">
-        <v>10320683865</v>
+        <v>10320145605</v>
       </c>
       <c r="C1055" t="s">
         <v>1056</v>
@@ -21224,7 +21224,7 @@
         <v>1054</v>
       </c>
       <c r="B1056">
-        <v>10320145605</v>
+        <v>10260135725</v>
       </c>
       <c r="C1056" t="s">
         <v>1057</v>
@@ -21238,7 +21238,7 @@
         <v>1055</v>
       </c>
       <c r="B1057">
-        <v>10260135725</v>
+        <v>10104000426</v>
       </c>
       <c r="C1057" t="s">
         <v>1058</v>
@@ -21252,7 +21252,7 @@
         <v>1056</v>
       </c>
       <c r="B1058">
-        <v>10104000426</v>
+        <v>10380667692</v>
       </c>
       <c r="C1058" t="s">
         <v>1059</v>
@@ -21266,7 +21266,7 @@
         <v>1057</v>
       </c>
       <c r="B1059">
-        <v>10380667692</v>
+        <v>10102927198</v>
       </c>
       <c r="C1059" t="s">
         <v>1060</v>
@@ -21280,7 +21280,7 @@
         <v>1058</v>
       </c>
       <c r="B1060">
-        <v>10102927198</v>
+        <v>10860712482</v>
       </c>
       <c r="C1060" t="s">
         <v>1061</v>
@@ -21294,7 +21294,7 @@
         <v>1059</v>
       </c>
       <c r="B1061">
-        <v>10860712482</v>
+        <v>14004460426</v>
       </c>
       <c r="C1061" t="s">
         <v>1062</v>
@@ -21308,7 +21308,7 @@
         <v>1060</v>
       </c>
       <c r="B1062">
-        <v>14004460426</v>
+        <v>10000000051</v>
       </c>
       <c r="C1062" t="s">
         <v>1063</v>
@@ -21322,7 +21322,7 @@
         <v>1061</v>
       </c>
       <c r="B1063">
-        <v>10000000051</v>
+        <v>10101128860</v>
       </c>
       <c r="C1063" t="s">
         <v>1064</v>
@@ -21336,7 +21336,7 @@
         <v>1062</v>
       </c>
       <c r="B1064">
-        <v>10101128860</v>
+        <v>10320824078</v>
       </c>
       <c r="C1064" t="s">
         <v>1065</v>
@@ -21350,7 +21350,7 @@
         <v>1063</v>
       </c>
       <c r="B1065">
-        <v>10320824078</v>
+        <v>10100687843</v>
       </c>
       <c r="C1065" t="s">
         <v>1066</v>
@@ -21364,7 +21364,7 @@
         <v>1064</v>
       </c>
       <c r="B1066">
-        <v>10100687843</v>
+        <v>10320782725</v>
       </c>
       <c r="C1066" t="s">
         <v>1067</v>
@@ -21378,7 +21378,7 @@
         <v>1065</v>
       </c>
       <c r="B1067">
-        <v>10320782725</v>
+        <v>10320658317</v>
       </c>
       <c r="C1067" t="s">
         <v>1068</v>
@@ -21392,7 +21392,7 @@
         <v>1066</v>
       </c>
       <c r="B1068">
-        <v>10320658317</v>
+        <v>14007562887</v>
       </c>
       <c r="C1068" t="s">
         <v>1069</v>
@@ -21406,7 +21406,7 @@
         <v>1067</v>
       </c>
       <c r="B1069">
-        <v>14007562887</v>
+        <v>14007982406</v>
       </c>
       <c r="C1069" t="s">
         <v>1070</v>
@@ -21420,7 +21420,7 @@
         <v>1068</v>
       </c>
       <c r="B1070">
-        <v>14007982406</v>
+        <v>14008783355</v>
       </c>
       <c r="C1070" t="s">
         <v>1071</v>
@@ -21434,7 +21434,7 @@
         <v>1069</v>
       </c>
       <c r="B1071">
-        <v>14008783355</v>
+        <v>10320637769</v>
       </c>
       <c r="C1071" t="s">
         <v>1072</v>
@@ -21448,7 +21448,7 @@
         <v>1070</v>
       </c>
       <c r="B1072">
-        <v>10320637769</v>
+        <v>10103679146</v>
       </c>
       <c r="C1072" t="s">
         <v>1073</v>
@@ -21462,7 +21462,7 @@
         <v>1071</v>
       </c>
       <c r="B1073">
-        <v>10103679146</v>
+        <v>10200255770</v>
       </c>
       <c r="C1073" t="s">
         <v>1074</v>
@@ -21476,7 +21476,7 @@
         <v>1072</v>
       </c>
       <c r="B1074">
-        <v>10200255770</v>
+        <v>14000187509</v>
       </c>
       <c r="C1074" t="s">
         <v>1075</v>

</xml_diff>